<commit_message>
finish the formulas for metrics of sample_medium/running some different simulations
</commit_message>
<xml_diff>
--- a/simulation_check.xlsx
+++ b/simulation_check.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\C-Final-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5A4305-D8D6-484B-ADF6-D4BD7F5BBC59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2B2023-0FB3-4D00-B318-6ED407597B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{603FAE4F-A0F0-414C-B275-6F2A5451B931}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="4" r:id="rId1"/>
     <sheet name="simulations_small" sheetId="1" r:id="rId2"/>
-    <sheet name="output_small_th" sheetId="3" r:id="rId3"/>
+    <sheet name="output_small_th" sheetId="3" state="hidden" r:id="rId3"/>
     <sheet name="simulations_medium" sheetId="7" r:id="rId4"/>
-    <sheet name="output_medium_th" sheetId="8" r:id="rId5"/>
+    <sheet name="output_medium_th" sheetId="8" state="hidden" r:id="rId5"/>
     <sheet name="simulations_large" sheetId="5" r:id="rId6"/>
-    <sheet name="output_large_th" sheetId="6" r:id="rId7"/>
+    <sheet name="output_large_th" sheetId="6" state="hidden" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -452,7 +452,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -559,6 +559,10 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -571,14 +575,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1032,27 +1035,27 @@
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B9" s="27">
         <f>MIN(simulations_medium!$J$3:$J$15)</f>
-        <v>3200.3169472499999</v>
+        <v>3.3914888888889942</v>
       </c>
       <c r="C9" s="27">
         <f>MIN(simulations_medium!$K$3:$K$15)</f>
-        <v>10419347.336163143</v>
+        <v>20.723022475219242</v>
       </c>
       <c r="D9" s="27">
         <f>MIN(simulations_medium!$L$3:$L$15)</f>
-        <v>3227.9013826576461</v>
+        <v>4.5522546584323731</v>
       </c>
       <c r="E9" s="27">
         <f>MIN(simulations_medium!$M$3:$M$15)</f>
-        <v>4833457.222222222</v>
+        <v>8437.0454593332634</v>
       </c>
       <c r="F9" s="27">
         <f>MIN(simulations_medium!$N$3:$N$15)</f>
-        <v>31488038583147.668</v>
+        <v>133442937.64094336</v>
       </c>
       <c r="G9" s="27">
         <f>MIN(simulations_medium!$O$3:$O$15)</f>
-        <v>5611420.3712738957</v>
+        <v>11551.750414588403</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -1061,27 +1064,27 @@
       </c>
       <c r="B10" s="25">
         <f>VLOOKUP(B9,simulations_medium!$J$3:$P$18,7,FALSE)</f>
-        <v>30000</v>
+        <v>25000</v>
       </c>
       <c r="C10" s="25">
         <f>VLOOKUP(C9,simulations_medium!$K$3:$P$18,6,FALSE)</f>
-        <v>30000</v>
+        <v>25000</v>
       </c>
       <c r="D10" s="25">
         <f>VLOOKUP(D9,simulations_medium!$L$3:$P$18,5,FALSE)</f>
-        <v>30000</v>
+        <v>25000</v>
       </c>
       <c r="E10" s="25">
         <f>VLOOKUP(E9,simulations_medium!$M$3:$P$18,4,FALSE)</f>
-        <v>10000</v>
+        <v>25000</v>
       </c>
       <c r="F10" s="25">
         <f>VLOOKUP(F9,simulations_medium!$N$3:$P$18,3,FALSE)</f>
-        <v>10000</v>
+        <v>25000</v>
       </c>
       <c r="G10" s="25">
         <f>VLOOKUP(G9,simulations_medium!$O$3:$P$18,2,FALSE)</f>
-        <v>10000</v>
+        <v>25000</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -1116,27 +1119,27 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B15" s="48">
+      <c r="B15" s="44">
         <f>MIN(simulations_large!$J$3:$J$15)</f>
         <v>30.783059199999915</v>
       </c>
-      <c r="C15" s="48">
+      <c r="C15" s="44">
         <f>MIN(simulations_large!$K$3:$K$15)</f>
         <v>20030.831877420351</v>
       </c>
-      <c r="D15" s="48">
+      <c r="D15" s="44">
         <f>MIN(simulations_large!$L$3:$L$15)</f>
         <v>141.53032140647582</v>
       </c>
-      <c r="E15" s="48">
+      <c r="E15" s="44">
         <f>MIN(simulations_large!$M$3:$M$15)</f>
         <v>12465.253210959938</v>
       </c>
-      <c r="F15" s="48">
+      <c r="F15" s="44">
         <f>MIN(simulations_large!$N$3:$N$15)</f>
         <v>331300469.0961979</v>
       </c>
-      <c r="G15" s="48">
+      <c r="G15" s="44">
         <f>MIN(simulations_large!$O$3:$O$15)</f>
         <v>18201.661163097117</v>
       </c>
@@ -1180,7 +1183,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{544FD0B2-A7ED-4478-8092-5F67F619DD9A}">
   <dimension ref="A1:P64"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="90" workbookViewId="0">
+    <sheetView topLeftCell="B45" zoomScale="90" workbookViewId="0">
       <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
@@ -1205,13 +1208,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
@@ -1588,14 +1591,14 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="47"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="49"/>
       <c r="I11" s="6">
         <v>50000</v>
       </c>
@@ -3136,8 +3139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32199EA4-1B1E-4F05-B93A-A4002D945EFC}">
   <dimension ref="A1:P132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="90" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43:E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3161,13 +3164,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
@@ -3211,41 +3214,41 @@
       <c r="B3">
         <v>0</v>
       </c>
-      <c r="C3" s="50">
+      <c r="C3" s="45">
         <v>0</v>
       </c>
-      <c r="D3" s="50">
+      <c r="D3" s="45">
         <v>0</v>
       </c>
-      <c r="E3" s="50">
+      <c r="E3" s="45">
         <v>0</v>
       </c>
-      <c r="I3" s="51">
+      <c r="I3" s="8">
         <v>10000</v>
       </c>
       <c r="J3" s="7">
         <f>AVERAGE(ABS($C$4-C16),ABS($C$5-C17),ABS($C$6-C18),ABS($C$7-C19),ABS($C$8-C20),ABS($C$9-C21), ABS($C$10-C22),ABS($C$11-C23),ABS($C$12-C24))</f>
-        <v>3827.263946</v>
+        <v>28.37109688888884</v>
       </c>
       <c r="K3" s="7">
         <f>AVERAGE(($C$4-C16)^2, ($C$5-C17)^2, ($C$6-C18)^2, ($C$7-C19)^2,($C$8-C20)^2,($C$9-C21)^2,($C$10-C22)^2,($C$11-C23)^2,($C$12-C24)^2)</f>
-        <v>15281291.864947332</v>
+        <v>884.51450456255623</v>
       </c>
       <c r="L3" s="7">
-        <f t="shared" ref="L3:L18" si="0">SQRT(K3)</f>
-        <v>3909.1292975478991</v>
+        <f t="shared" ref="L3:L7" si="0">SQRT(K3)</f>
+        <v>29.740788566589089</v>
       </c>
       <c r="M3" s="7">
         <f>AVERAGE(ABS($D$4-D16),ABS($D$5-D17),ABS($D$6-D18),ABS($D$7-D19),ABS($D$8-D20),ABS($D$9-D21), ABS($D$10-D22),ABS($D$11-D23),ABS($D$12-D24))</f>
-        <v>4833457.222222222</v>
+        <v>58809.317237777839</v>
       </c>
       <c r="N3" s="7">
         <f>AVERAGE(($D$4-D16)^2, ($D$5-D17)^2, ($D$6-D18)^2, ($D$7-D19)^2,($D$8-D20)^2,($D$9-D21)^2,($D$10-D22)^2,($D$11-D23)^2,($D$12-D24)^2)</f>
-        <v>31488038583147.668</v>
+        <v>8376344286.7277184</v>
       </c>
       <c r="O3" s="7">
-        <f t="shared" ref="O3:O18" si="1">SQRT(N3)</f>
-        <v>5611420.3712738957</v>
+        <f t="shared" ref="O3:O6" si="1">SQRT(N3)</f>
+        <v>91522.370416897087</v>
       </c>
       <c r="P3" s="6">
         <f>I3</f>
@@ -3259,41 +3262,41 @@
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" s="50">
+      <c r="C4" s="45">
         <v>3079.9488820000001</v>
       </c>
-      <c r="D4" s="50">
+      <c r="D4" s="45">
         <v>10578820</v>
       </c>
-      <c r="E4" s="50">
+      <c r="E4" s="45">
         <v>3252.509963</v>
       </c>
-      <c r="I4" s="51">
+      <c r="I4" s="8">
         <v>15000</v>
       </c>
       <c r="J4" s="7">
         <f>AVERAGE(ABS($C$4-C25),ABS($C$5-C26),ABS($C$6-C27),ABS($C$7-C28),ABS($C$8-C29),ABS($C$9-C30), ABS($C$10-C31),ABS($C$11-C32),ABS($C$12-C33))</f>
-        <v>3827.263946</v>
+        <v>21.371001222222226</v>
       </c>
       <c r="K4" s="7">
         <f>AVERAGE(($C$4-C25)^2, ($C$5-C26)^2, ($C$6-C27)^2, ($C$7-C28)^2,($C$8-C29)^2,($C$9-C30)^2,($C$10-C31)^2,($C$11-C32)^2,($C$12-C33)^2)</f>
-        <v>15281291.864947332</v>
+        <v>502.64469865889777</v>
       </c>
       <c r="L4" s="7">
         <f t="shared" si="0"/>
-        <v>3909.1292975478991</v>
+        <v>22.419739040829572</v>
       </c>
       <c r="M4" s="7">
         <f>AVERAGE(ABS($D$4-D25),ABS($D$5-D26),ABS($D$6-D27),ABS($D$7-D28),ABS($D$8-D29),ABS($D$9-D30), ABS($D$10-D31),ABS($D$11-D32),ABS($D$12-D33))</f>
-        <v>4833457.222222222</v>
+        <v>37486.552089555553</v>
       </c>
       <c r="N4" s="7">
         <f>AVERAGE(($D$4-D25)^2, ($D$5-D26)^2, ($D$6-D27)^2, ($D$7-D28)^2,($D$8-D29)^2,($D$9-D30)^2,($D$10-D31)^2,($D$11-D32)^2,($D$12-D33)^2)</f>
-        <v>31488038583147.668</v>
+        <v>2441128788.2266197</v>
       </c>
       <c r="O4" s="7">
         <f t="shared" si="1"/>
-        <v>5611420.3712738957</v>
+        <v>49407.780644617298</v>
       </c>
       <c r="P4" s="6">
         <f t="shared" ref="P4:P33" si="2">I4</f>
@@ -3307,41 +3310,41 @@
       <c r="B5">
         <v>2</v>
       </c>
-      <c r="C5" s="50">
+      <c r="C5" s="45">
         <v>2589.0103300000001</v>
       </c>
-      <c r="D5" s="50">
+      <c r="D5" s="45">
         <v>5804110</v>
       </c>
-      <c r="E5" s="50">
+      <c r="E5" s="45">
         <v>2409.1720749999999</v>
       </c>
-      <c r="I5" s="51">
+      <c r="I5" s="8">
         <v>20000</v>
       </c>
       <c r="J5" s="7">
         <f>AVERAGE(ABS($C$4-C34),ABS($C$5-C35),ABS($C$6-C36),ABS($C$7-C37),ABS($C$8-C38),ABS($C$9-C39),ABS($C$10-C40),ABS($C$11-C41),ABS($C$12-C42))</f>
-        <v>3827.263946</v>
+        <v>11.173401222222159</v>
       </c>
       <c r="K5" s="7">
         <f>AVERAGE(($C$4-C34)^2, ($C$5-C35)^2, ($C$6-C36)^2, ($C$7-C37)^2,($C$8-C38)^2,($C$9-C39)^2,($C$10-C40)^2,($C$11-C41)^2,($C$12-C42)^2)</f>
-        <v>15281291.864947332</v>
+        <v>172.42077382658005</v>
       </c>
       <c r="L5" s="7">
         <f t="shared" si="0"/>
-        <v>3909.1292975478991</v>
+        <v>13.130909101299119</v>
       </c>
       <c r="M5" s="7">
         <f>AVERAGE(ABS($D$4-D34),ABS($D$5-D35),ABS($D$6-D36),ABS($D$7-D37),ABS($D$8-D38),ABS($D$9-D39),ABS($D$10-D40),ABS($D$11-D41),ABS($D$12-D42))</f>
-        <v>4833457.222222222</v>
+        <v>20206.164804888864</v>
       </c>
       <c r="N5" s="7">
         <f>AVERAGE(($D$4-D34)^2, ($D$5-D35)^2, ($D$6-D36)^2, ($D$7-D37)^2,($D$8-D38)^2,($D$9-D39)^2,($D$10-D40)^2,($D$11-D41)^2,($D$12-D42)^2)</f>
-        <v>31488038583147.668</v>
+        <v>1127450728.4498024</v>
       </c>
       <c r="O5" s="7">
         <f t="shared" si="1"/>
-        <v>5611420.3712738957</v>
+        <v>33577.533090592027</v>
       </c>
       <c r="P5" s="6">
         <f t="shared" si="2"/>
@@ -3355,41 +3358,41 @@
       <c r="B6">
         <v>3</v>
       </c>
-      <c r="C6" s="50">
+      <c r="C6" s="45">
         <v>3729.5815219999999</v>
       </c>
-      <c r="D6" s="50">
+      <c r="D6" s="45">
         <v>3012089</v>
       </c>
-      <c r="E6" s="50">
+      <c r="E6" s="45">
         <v>1735.5371970000001</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="8">
         <v>25000</v>
       </c>
       <c r="J6" s="7">
         <f>AVERAGE(ABS($C$4-C43),ABS($C$5-C44),ABS($C$6-C45),ABS($C$7-C46),ABS($C$8-C47),ABS($C$9-C48),ABS($C$10-C49),ABS($C$11-C50),ABS($C$12-C51))</f>
-        <v>3827.263946</v>
+        <v>3.3914888888889942</v>
       </c>
       <c r="K6" s="7">
         <f>AVERAGE(($C$4-C43)^2, ($C$5-C44)^2, ($C$6-C45)^2, ($C$7-C46)^2,($C$8-C47)^2,($C$9-C48)^2,($C$10-C49)^2,($C$11-C50)^2,($C$12-C51)^2)</f>
-        <v>15281291.864947332</v>
+        <v>20.723022475219242</v>
       </c>
       <c r="L6" s="7">
         <f t="shared" si="0"/>
-        <v>3909.1292975478991</v>
+        <v>4.5522546584323731</v>
       </c>
       <c r="M6" s="7">
         <f>AVERAGE(ABS($D$4-D43),ABS($D$5-D44),ABS($D$6-D45),ABS($D$7-D46),ABS($D$8-D47),ABS($D$9-D48),ABS($D$10-D49),ABS($D$11-D50),ABS($D$12-D51))</f>
-        <v>4833457.222222222</v>
+        <v>8437.0454593332634</v>
       </c>
       <c r="N6" s="7">
         <f>AVERAGE(($D$4-D43)^2, ($D$5-D44)^2, ($D$6-D45)^2, ($D$7-D46)^2,($D$8-D47)^2,($D$9-D48)^2,($D$10-D49)^2,($D$11-D50)^2,($D$12-D51)^2)</f>
-        <v>31488038583147.668</v>
+        <v>133442937.64094336</v>
       </c>
       <c r="O6" s="7">
         <f t="shared" si="1"/>
-        <v>5611420.3712738957</v>
+        <v>11551.750414588403</v>
       </c>
       <c r="P6" s="6">
         <f t="shared" si="2"/>
@@ -3403,41 +3406,41 @@
       <c r="B7">
         <v>4</v>
       </c>
-      <c r="C7" s="50">
+      <c r="C7" s="45">
         <v>3402.7270549999998</v>
       </c>
-      <c r="D7" s="50">
+      <c r="D7" s="45">
         <v>1645894</v>
       </c>
-      <c r="E7" s="50">
+      <c r="E7" s="45">
         <v>1282.924162</v>
       </c>
       <c r="I7" s="9">
         <v>30000</v>
       </c>
       <c r="J7" s="7">
-        <f>AVERAGE(ABS($C$4-C52),ABS($C$5-C58),ABS($C$6-C59),ABS($C$7-C60))</f>
-        <v>3200.3169472499999</v>
+        <f>AVERAGE(ABS($C$4-C52),ABS($C$5-C53),ABS($C$6-C54),ABS($C$7-C55),ABS($C$8-C56),ABS($C$9-C57),ABS($C$10-C58),ABS($C$11-C59),ABS($C$12-C60))</f>
+        <v>3827.263946</v>
       </c>
       <c r="K7" s="7">
-        <f>AVERAGE(($C$4-C52)^2, ($C$5-C58)^2, ($C$6-C59)^2, ($C$7-C60)^2)</f>
-        <v>10419347.336163143</v>
+        <f>AVERAGE(($C$4-C52)^2, ($C$5-C53)^2, ($C$6-C54)^2, ($C$7-C55)^2,($C$8-C56)^2,($C$9-C57)^2,($C$10-C58)^2,($C$11-C59)^2,($C$12-C60)^2)</f>
+        <v>15281291.864947332</v>
       </c>
       <c r="L7" s="7">
         <f t="shared" si="0"/>
-        <v>3227.9013826576461</v>
+        <v>3909.1292975478991</v>
       </c>
       <c r="M7" s="7">
-        <f>AVERAGE(ABS($D$4-D52),ABS($D$5-D58),ABS($D$6-D59),ABS($D$7-D60))</f>
-        <v>5260228.25</v>
+        <f>AVERAGE(ABS($D$4-D52),ABS($D$5-D53),ABS($D$6-D54),ABS($D$7-D55),ABS($D$8-D56),ABS($D$9-D57),ABS($D$10-D58),ABS($D$11-D59),ABS($D$12-D60))</f>
+        <v>4833457.222222222</v>
       </c>
       <c r="N7" s="7">
-        <f>AVERAGE(($D$4-D52)^2, ($D$5-D58)^2, ($D$6-D59)^2, ($D$7-D60)^2)</f>
-        <v>39345193171914.25</v>
+        <f>AVERAGE(($D$4-D52)^2, ($D$5-D53)^2, ($D$6-D54)^2, ($D$7-D55)^2,($D$8-D56)^2,($D$9-D57)^2,($D$10-D58)^2,($D$11-D59)^2,($D$12-D60)^2)</f>
+        <v>31488038583147.668</v>
       </c>
       <c r="O7" s="7">
-        <f>SQRT(N7)</f>
-        <v>6272574.6844429243</v>
+        <f t="shared" ref="O7:O15" si="3">SQRT(N7)</f>
+        <v>5611420.3712738957</v>
       </c>
       <c r="P7" s="6">
         <f t="shared" si="2"/>
@@ -3451,41 +3454,41 @@
       <c r="B8">
         <v>5</v>
       </c>
-      <c r="C8" s="50">
+      <c r="C8" s="45">
         <v>3251.2381350000001</v>
       </c>
-      <c r="D8" s="50">
+      <c r="D8" s="45">
         <v>1215558</v>
       </c>
-      <c r="E8" s="50">
+      <c r="E8" s="45">
         <v>1102.5234109999999</v>
       </c>
       <c r="I8" s="6">
         <v>35000</v>
       </c>
       <c r="J8" s="7">
-        <f>AVERAGE(ABS($C$4-C61),ABS($C$5-C67),ABS($C$6-C68),ABS($C$7-C69))</f>
-        <v>3200.3169472499999</v>
+        <f>AVERAGE(ABS($C$4-C61),ABS($C$5-C62),ABS($C$6-C63),ABS($C$7-C64),ABS($C$8-C65),ABS($C$9-C66),ABS($C$10-C67),ABS($C$11-C68),ABS($C$12-C69))</f>
+        <v>3827.263946</v>
       </c>
       <c r="K8" s="7">
-        <f>AVERAGE(($C$4-C61)^2, ($C$5-C67)^2, ($C$6-C68)^2, ($C$7-C69)^2)</f>
-        <v>10419347.336163143</v>
+        <f>AVERAGE(($C$4-C61)^2, ($C$5-C62)^2, ($C$6-C63)^2, ($C$7-C64)^2,($C$8-C65)^2,($C$9-C66)^2,($C$10-C67)^2,($C$11-C68)^2,($C$12-C69)^2)</f>
+        <v>15281291.864947332</v>
       </c>
       <c r="L8" s="7">
-        <f>SQRT(K8)</f>
-        <v>3227.9013826576461</v>
+        <f t="shared" ref="L8:L15" si="4">SQRT(K8)</f>
+        <v>3909.1292975478991</v>
       </c>
       <c r="M8" s="7">
-        <f>AVERAGE(ABS($D$4-D61),ABS($D$5-D67),ABS($D$6-D68),ABS($D$7-D69))</f>
-        <v>5260228.25</v>
+        <f>AVERAGE(ABS($D$4-D61),ABS($D$5-D62),ABS($D$6-D63),ABS($D$7-D64),ABS($D$8-D65),ABS($D$9-D66),ABS($D$10-D67),ABS($D$11-D68),ABS($D$12-D69))</f>
+        <v>4833457.222222222</v>
       </c>
       <c r="N8" s="7">
-        <f>AVERAGE(($D$4-D61)^2, ($D$5-D67)^2, ($D$6-D68)^2, ($D$7-D69)^2)</f>
-        <v>39345193171914.25</v>
+        <f>AVERAGE(($D$4-D61)^2, ($D$5-D62)^2, ($D$6-D63)^2, ($D$7-D64)^2,($D$8-D65)^2,($D$9-D66)^2,($D$10-D67)^2,($D$11-D68)^2,($D$12-D69)^2)</f>
+        <v>31488038583147.668</v>
       </c>
       <c r="O8" s="7">
-        <f>SQRT(N8)</f>
-        <v>6272574.6844429243</v>
+        <f t="shared" si="3"/>
+        <v>5611420.3712738957</v>
       </c>
       <c r="P8" s="6"/>
     </row>
@@ -3496,41 +3499,41 @@
       <c r="B9">
         <v>6</v>
       </c>
-      <c r="C9" s="50">
+      <c r="C9" s="45">
         <v>4477.8493330000001</v>
       </c>
-      <c r="D9" s="50">
+      <c r="D9" s="45">
         <v>8230023</v>
       </c>
-      <c r="E9" s="50">
+      <c r="E9" s="45">
         <v>2868.8015869999999</v>
       </c>
       <c r="I9" s="6">
         <v>40000</v>
       </c>
       <c r="J9" s="7">
-        <f>AVERAGE(ABS($C$4-C70),ABS($C$5-C76),ABS($C$6-C77),ABS($C$7-C78))</f>
-        <v>3200.3169472499999</v>
+        <f>AVERAGE(ABS($C$4-C70),ABS($C$5-C71),ABS($C$6-C72),ABS($C$7-C73),ABS($C$8-C74),ABS($C$9-C75),ABS($C$10-C76),ABS($C$11-C77),ABS($C$12-C78))</f>
+        <v>3827.263946</v>
       </c>
       <c r="K9" s="7">
-        <f>AVERAGE(($C$4-C70)^2, ($C$5-C76)^2, ($C$6-C77)^2, ($C$7-C78)^2)</f>
-        <v>10419347.336163143</v>
+        <f>AVERAGE(($C$4-C70)^2, ($C$5-C71)^2, ($C$6-C72)^2, ($C$7-C73)^2,($C$8-C74)^2,($C$9-C75)^2,($C$10-C76)^2,($C$11-C77)^2,($C$12-C78)^2)</f>
+        <v>15281291.864947332</v>
       </c>
       <c r="L9" s="7">
-        <f>SQRT(K9)</f>
-        <v>3227.9013826576461</v>
+        <f t="shared" si="4"/>
+        <v>3909.1292975478991</v>
       </c>
       <c r="M9" s="7">
-        <f>AVERAGE(ABS($D$4-D70),ABS($D$5-D76),ABS($D$6-D77),ABS($D$7-D78))</f>
-        <v>5260228.25</v>
+        <f>AVERAGE(ABS($D$4-D70),ABS($D$5-D71),ABS($D$6-D72),ABS($D$7-D73),ABS($D$8-D74),ABS($D$9-D75),ABS($D$10-D76),ABS($D$11-D77),ABS($D$12-D78))</f>
+        <v>4833457.222222222</v>
       </c>
       <c r="N9" s="7">
-        <f>AVERAGE(($D$4-D70)^2, ($D$5-D76)^2, ($D$6-D77)^2, ($D$7-D78)^2)</f>
-        <v>39345193171914.25</v>
+        <f>AVERAGE(($D$4-D70)^2, ($D$5-D71)^2, ($D$6-D72)^2, ($D$7-D73)^2,($D$8-D74)^2,($D$9-D75)^2,($D$10-D76)^2,($D$11-D77)^2,($D$12-D78)^2)</f>
+        <v>31488038583147.668</v>
       </c>
       <c r="O9" s="7">
-        <f>SQRT(N9)</f>
-        <v>6272574.6844429243</v>
+        <f t="shared" si="3"/>
+        <v>5611420.3712738957</v>
       </c>
       <c r="P9" s="6"/>
     </row>
@@ -3541,41 +3544,41 @@
       <c r="B10">
         <v>7</v>
       </c>
-      <c r="C10" s="50">
+      <c r="C10" s="45">
         <v>3986.910781</v>
       </c>
-      <c r="D10" s="50">
+      <c r="D10" s="45">
         <v>4091321</v>
       </c>
-      <c r="E10" s="50">
+      <c r="E10" s="45">
         <v>2022.701468</v>
       </c>
       <c r="I10" s="6">
         <v>45000</v>
       </c>
       <c r="J10" s="7">
-        <f>AVERAGE(ABS($C$4-C79),ABS($C$5-C85),ABS($C$6-C86),ABS($C$7-C87))</f>
-        <v>3200.3169472499999</v>
+        <f>AVERAGE(ABS($C$4-C79),ABS($C$5-C80),ABS($C$6-C81),ABS($C$7-C82),ABS($C$8-C83),ABS($C$9-C84),ABS($C$10-C85),ABS($C$11-C86),ABS($C$12-C87))</f>
+        <v>3827.263946</v>
       </c>
       <c r="K10" s="7">
-        <f>AVERAGE(($C$4-C79)^2, ($C$5-C85)^2, ($C$6-C86)^2, ($C$7-C87)^2)</f>
-        <v>10419347.336163143</v>
+        <f>AVERAGE(($C$4-C79)^2, ($C$5-C80)^2, ($C$6-C81)^2, ($C$7-C82)^2,($C$8-C83)^2,($C$9-C84)^2,($C$10-C85)^2,($C$11-C86)^2,($C$12-C87)^2)</f>
+        <v>15281291.864947332</v>
       </c>
       <c r="L10" s="7">
-        <f>SQRT(K10)</f>
-        <v>3227.9013826576461</v>
+        <f t="shared" si="4"/>
+        <v>3909.1292975478991</v>
       </c>
       <c r="M10" s="7">
-        <f>AVERAGE(ABS($D$4-D79),ABS($D$5-D85),ABS($D$6-D86),ABS($D$7-D87))</f>
-        <v>5260228.25</v>
+        <f>AVERAGE(ABS($D$4-D79),ABS($D$5-D80),ABS($D$6-D81),ABS($D$7-D82),ABS($D$8-D83),ABS($D$9-D84),ABS($D$10-D85),ABS($D$11-D86),ABS($D$12-D87))</f>
+        <v>4833457.222222222</v>
       </c>
       <c r="N10" s="7">
-        <f>AVERAGE(($D$4-D79)^2, ($D$5-D85)^2, ($D$6-D86)^2, ($D$7-D87)^2)</f>
-        <v>39345193171914.25</v>
+        <f>AVERAGE(($D$4-D79)^2, ($D$5-D80)^2, ($D$6-D81)^2, ($D$7-D82)^2,($D$8-D83)^2,($D$9-D84)^2,($D$10-D85)^2,($D$11-D86)^2,($D$12-D87)^2)</f>
+        <v>31488038583147.668</v>
       </c>
       <c r="O10" s="7">
-        <f>SQRT(N10)</f>
-        <v>6272574.6844429243</v>
+        <f t="shared" si="3"/>
+        <v>5611420.3712738957</v>
       </c>
       <c r="P10" s="6"/>
     </row>
@@ -3586,44 +3589,44 @@
       <c r="B11">
         <v>8</v>
       </c>
-      <c r="C11" s="50">
+      <c r="C11" s="45">
         <v>5127.4819710000002</v>
       </c>
-      <c r="D11" s="50">
+      <c r="D11" s="45">
         <v>4814613</v>
       </c>
-      <c r="E11" s="50">
+      <c r="E11" s="45">
         <v>2194.222569</v>
       </c>
       <c r="I11" s="6">
         <v>50000</v>
       </c>
       <c r="J11" s="7">
-        <f>AVERAGE(ABS($C$4-C88),ABS($C$5-C94),ABS($C$6-C95),ABS($C$7-C96))</f>
-        <v>3200.3169472499999</v>
+        <f>AVERAGE(ABS($C$4-C88),ABS($C$5-C89),ABS($C$6-C90),ABS($C$7-C91),ABS($C$8-C92),ABS($C$9-C93),ABS($C$10-C94),ABS($C$11-C95),ABS($C$12-C96))</f>
+        <v>3827.263946</v>
       </c>
       <c r="K11" s="7">
-        <f>AVERAGE(($C$4-C88)^2, ($C$5-C94)^2, ($C$6-C95)^2, ($C$7-C96)^2)</f>
-        <v>10419347.336163143</v>
+        <f>AVERAGE(($C$4-C88)^2, ($C$5-C89)^2, ($C$6-C90)^2, ($C$7-C91)^2,($C$8-C92)^2,($C$9-C93)^2,($C$10-C94)^2,($C$11-C95)^2,($C$12-C96)^2)</f>
+        <v>15281291.864947332</v>
       </c>
       <c r="L11" s="7">
-        <f>SQRT(K11)</f>
-        <v>3227.9013826576461</v>
+        <f t="shared" si="4"/>
+        <v>3909.1292975478991</v>
       </c>
       <c r="M11" s="7">
-        <f>AVERAGE(ABS($D$4-D88),ABS($D$5-D94),ABS($D$6-D95),ABS($D$7-D96))</f>
-        <v>5260228.25</v>
+        <f>AVERAGE(ABS($D$4-D88),ABS($D$5-D89),ABS($D$6-D90),ABS($D$7-D91),ABS($D$8-D92),ABS($D$9-D93),ABS($D$10-D94),ABS($D$11-D95),ABS($D$12-D96))</f>
+        <v>4833457.222222222</v>
       </c>
       <c r="N11" s="7">
-        <f>AVERAGE(($D$4-D88)^2, ($D$5-D94)^2, ($D$6-D95)^2, ($D$7-D96)^2)</f>
-        <v>39345193171914.25</v>
+        <f>AVERAGE(($D$4-D88)^2, ($D$5-D89)^2, ($D$6-D90)^2, ($D$7-D91)^2,($D$8-D92)^2,($D$9-D93)^2,($D$10-D94)^2,($D$11-D95)^2,($D$12-D96)^2)</f>
+        <v>31488038583147.668</v>
       </c>
       <c r="O11" s="7">
-        <f>SQRT(N11)</f>
-        <v>6272574.6844429243</v>
+        <f t="shared" si="3"/>
+        <v>5611420.3712738957</v>
       </c>
       <c r="P11" s="6">
-        <f>I8</f>
+        <f t="shared" ref="P11:P18" si="5">I8</f>
         <v>35000</v>
       </c>
     </row>
@@ -3634,44 +3637,44 @@
       <c r="B12">
         <v>9</v>
       </c>
-      <c r="C12" s="50">
+      <c r="C12" s="45">
         <v>4800.6275050000004</v>
       </c>
-      <c r="D12" s="50">
+      <c r="D12" s="45">
         <v>4108687</v>
       </c>
-      <c r="E12" s="50">
+      <c r="E12" s="45">
         <v>2026.989632</v>
       </c>
       <c r="I12" s="9">
         <v>55000</v>
       </c>
       <c r="J12" s="7">
-        <f>AVERAGE(ABS($C$4-C97),ABS($C$5-C98),ABS($C$6-C99),ABS($C$7-C105))</f>
-        <v>3200.3169472499999</v>
+        <f>AVERAGE(ABS($C$4-C97),ABS($C$5-C98),ABS($C$6-C99),ABS($C$7-C100),ABS($C$8-C101),ABS($C$9-C102),ABS($C$10-C103),ABS($C$11-C104),ABS($C$12-C105))</f>
+        <v>3827.263946</v>
       </c>
       <c r="K12" s="7">
-        <f>AVERAGE(($C$4-C97)^2, ($C$5-C98)^2, ($C$6-C99)^2, ($C$7-C105)^2)</f>
-        <v>10419347.336163143</v>
+        <f>AVERAGE(($C$4-C97)^2, ($C$5-C98)^2, ($C$6-C99)^2, ($C$7-C100)^2,($C$8-C101)^2,($C$9-C102)^2,($C$10-C103)^2,($C$11-C104)^2,($C$12-C105)^2)</f>
+        <v>15281291.864947332</v>
       </c>
       <c r="L12" s="7">
-        <f>SQRT(K12)</f>
-        <v>3227.9013826576461</v>
+        <f t="shared" si="4"/>
+        <v>3909.1292975478991</v>
       </c>
       <c r="M12" s="7">
-        <f>AVERAGE(ABS($D$4-D97),ABS($D$5-D98),ABS($D$6-D99),ABS($D$7-D105))</f>
-        <v>5260228.25</v>
+        <f>AVERAGE(ABS($D$4-D97),ABS($D$5-D98),ABS($D$6-D99),ABS($D$7-D100),ABS($D$8-D101),ABS($D$9-D102),ABS($D$10-D103),ABS($D$11-D104),ABS($D$12-D105))</f>
+        <v>4833457.222222222</v>
       </c>
       <c r="N12" s="7">
-        <f>AVERAGE(($D$4-D97)^2, ($D$5-D98)^2, ($D$6-D99)^2, ($D$7-D105)^2)</f>
-        <v>39345193171914.25</v>
+        <f>AVERAGE(($D$4-D97)^2, ($D$5-D98)^2, ($D$6-D99)^2, ($D$7-D100)^2,($D$8-D101)^2,($D$9-D102)^2,($D$10-D103)^2,($D$11-D104)^2,($D$12-D105)^2)</f>
+        <v>31488038583147.668</v>
       </c>
       <c r="O12" s="7">
-        <f>SQRT(N12)</f>
-        <v>6272574.6844429243</v>
+        <f t="shared" si="3"/>
+        <v>5611420.3712738957</v>
       </c>
       <c r="P12" s="6">
-        <f>I9</f>
+        <f t="shared" si="5"/>
         <v>40000</v>
       </c>
     </row>
@@ -3680,72 +3683,72 @@
         <v>60000</v>
       </c>
       <c r="J13" s="7">
-        <f>AVERAGE(ABS($C$4-C106),ABS($C$5-C107),ABS($C$6-C113),ABS($C$7-C114))</f>
-        <v>3200.3169472499999</v>
+        <f>AVERAGE(ABS($C$4-C106),ABS($C$5-C107),ABS($C$6-C108),ABS($C$7-C109),ABS($C$8-C110),ABS($C$9-C111),ABS($C$10-C112),ABS($C$11-C113),ABS($C$12-C114))</f>
+        <v>3827.263946</v>
       </c>
       <c r="K13" s="7">
-        <f>AVERAGE(($C$4-C106)^2, ($C$5-C107)^2, ($C$6-C113)^2, ($C$7-C114)^2)</f>
-        <v>10419347.336163143</v>
+        <f>AVERAGE(($C$4-C106)^2, ($C$5-C107)^2, ($C$6-C108)^2, ($C$7-C109)^2,($C$8-C110)^2,($C$9-C111)^2,($C$10-C112)^2,($C$11-C113)^2,($C$12-C114)^2)</f>
+        <v>15281291.864947332</v>
       </c>
       <c r="L13" s="7">
-        <f>SQRT(K13)</f>
-        <v>3227.9013826576461</v>
+        <f t="shared" si="4"/>
+        <v>3909.1292975478991</v>
       </c>
       <c r="M13" s="7">
-        <f>AVERAGE(ABS($D$4-D106),ABS($D$5-D107),ABS($D$6-D113),ABS($D$7-D114))</f>
-        <v>5260228.25</v>
+        <f>AVERAGE(ABS($D$4-D106),ABS($D$5-D107),ABS($D$6-D108),ABS($D$7-D109),ABS($D$8-D110),ABS($D$9-D111),ABS($D$10-D112),ABS($D$11-D113),ABS($D$12-D114))</f>
+        <v>4833457.222222222</v>
       </c>
       <c r="N13" s="7">
-        <f>AVERAGE(($D$4-D106)^2, ($D$5-D107)^2, ($D$6-D113)^2, ($D$7-D114)^2)</f>
-        <v>39345193171914.25</v>
+        <f>AVERAGE(($D$4-D106)^2, ($D$5-D107)^2, ($D$6-D108)^2, ($D$7-D109)^2,($D$8-D110)^2,($D$9-D111)^2,($D$10-D112)^2,($D$11-D113)^2,($D$12-D114)^2)</f>
+        <v>31488038583147.668</v>
       </c>
       <c r="O13" s="7">
-        <f>SQRT(N13)</f>
-        <v>6272574.6844429243</v>
+        <f t="shared" si="3"/>
+        <v>5611420.3712738957</v>
       </c>
       <c r="P13" s="6">
-        <f>I10</f>
+        <f t="shared" si="5"/>
         <v>45000</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="46"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="47"/>
+      <c r="B14" s="48"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="49"/>
       <c r="I14" s="6">
         <v>65000</v>
       </c>
       <c r="J14" s="7">
-        <f>AVERAGE(ABS($C$4-C115),ABS($C$5-C121),ABS($C$6-C122),ABS($C$7-C123))</f>
-        <v>3200.3169472499999</v>
+        <f>AVERAGE(ABS($C$4-C115),ABS($C$5-C116),ABS($C$6-C117),ABS($C$7-C118),ABS($C$8-C119),ABS($C$9-C120),ABS($C$10-C121),ABS($C$11-C122),ABS($C$12-C123))</f>
+        <v>3827.263946</v>
       </c>
       <c r="K14" s="7">
-        <f>AVERAGE(($C$4-C115)^2, ($C$5-C121)^2, ($C$6-C122)^2, ($C$7-C123)^2)</f>
-        <v>10419347.336163143</v>
+        <f>AVERAGE(($C$4-C115)^2, ($C$5-C116)^2, ($C$6-C117)^2, ($C$7-C118)^2,($C$8-C119)^2,($C$9-C120)^2,($C$10-C121)^2,($C$11-C122)^2,($C$12-C123)^2)</f>
+        <v>15281291.864947332</v>
       </c>
       <c r="L14" s="7">
-        <f>SQRT(K14)</f>
-        <v>3227.9013826576461</v>
+        <f t="shared" si="4"/>
+        <v>3909.1292975478991</v>
       </c>
       <c r="M14" s="7">
-        <f>AVERAGE(ABS($D$4-D115),ABS($D$5-D121),ABS($D$6-D122),ABS($D$7-D123))</f>
-        <v>5260228.25</v>
+        <f>AVERAGE(ABS($D$4-D115),ABS($D$5-D116),ABS($D$6-D117),ABS($D$7-D118),ABS($D$8-D119),ABS($D$9-D120),ABS($D$10-D121),ABS($D$11-D122),ABS($D$12-D123))</f>
+        <v>4833457.222222222</v>
       </c>
       <c r="N14" s="7">
-        <f>AVERAGE(($D$4-D115)^2, ($D$5-D121)^2, ($D$6-D122)^2, ($D$7-D123)^2)</f>
-        <v>39345193171914.25</v>
+        <f>AVERAGE(($D$4-D115)^2, ($D$5-D116)^2, ($D$6-D117)^2, ($D$7-D118)^2,($D$8-D119)^2,($D$9-D120)^2,($D$10-D121)^2,($D$11-D122)^2,($D$12-D123)^2)</f>
+        <v>31488038583147.668</v>
       </c>
       <c r="O14" s="7">
-        <f>SQRT(N14)</f>
-        <v>6272574.6844429243</v>
+        <f t="shared" si="3"/>
+        <v>5611420.3712738957</v>
       </c>
       <c r="P14" s="6">
-        <f>I11</f>
+        <f t="shared" si="5"/>
         <v>50000</v>
       </c>
     </row>
@@ -3772,31 +3775,31 @@
         <v>70000</v>
       </c>
       <c r="J15" s="7">
-        <f>AVERAGE(ABS($C$4-C124),ABS($C$5-C130),ABS($C$6-C131),ABS($C$7-C132))</f>
-        <v>3200.3169472499999</v>
+        <f>AVERAGE(ABS($C$4-C124),ABS($C$5-C125),ABS($C$6-C126),ABS($C$7-C127),ABS($C$8-C128),ABS($C$9-C129),ABS($C$10-C130),ABS($C$11-C131),ABS($C$12-C132))</f>
+        <v>3827.263946</v>
       </c>
       <c r="K15" s="7">
-        <f>AVERAGE(($C$4-C124)^2, ($C$5-C130)^2, ($C$6-C131)^2, ($C$7-C132)^2)</f>
-        <v>10419347.336163143</v>
+        <f>AVERAGE(($C$4-C124)^2, ($C$5-C125)^2, ($C$6-C126)^2, ($C$7-C127)^2,($C$8-C128)^2,($C$9-C129)^2,($C$10-C130)^2,($C$11-C131)^2,($C$12-C132)^2)</f>
+        <v>15281291.864947332</v>
       </c>
       <c r="L15" s="7">
-        <f>SQRT(K15)</f>
-        <v>3227.9013826576461</v>
+        <f t="shared" si="4"/>
+        <v>3909.1292975478991</v>
       </c>
       <c r="M15" s="7">
-        <f>AVERAGE(ABS($D$4-D124),ABS($D$5-D130),ABS($D$6-D131),ABS($D$7-D132))</f>
-        <v>5260228.25</v>
+        <f>AVERAGE(ABS($D$4-D124),ABS($D$5-D125),ABS($D$6-D126),ABS($D$7-D127),ABS($D$8-D128),ABS($D$9-D129),ABS($D$10-D130),ABS($D$11-D131),ABS($D$12-D132))</f>
+        <v>4833457.222222222</v>
       </c>
       <c r="N15" s="7">
-        <f>AVERAGE(($D$4-D124)^2, ($D$5-D130)^2, ($D$6-D131)^2, ($D$7-D132)^2)</f>
-        <v>39345193171914.25</v>
+        <f>AVERAGE(($D$4-D124)^2, ($D$5-D125)^2, ($D$6-D126)^2, ($D$7-D127)^2,($D$8-D128)^2,($D$9-D129)^2,($D$10-D130)^2,($D$11-D131)^2,($D$12-D132)^2)</f>
+        <v>31488038583147.668</v>
       </c>
       <c r="O15" s="7">
-        <f>SQRT(N15)</f>
-        <v>6272574.6844429243</v>
+        <f t="shared" si="3"/>
+        <v>5611420.3712738957</v>
       </c>
       <c r="P15" s="6">
-        <f>I12</f>
+        <f t="shared" si="5"/>
         <v>55000</v>
       </c>
     </row>
@@ -3807,12 +3810,20 @@
       <c r="B16" s="11">
         <v>1</v>
       </c>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="13"/>
+      <c r="C16" s="12">
+        <v>3049.0503269999999</v>
+      </c>
+      <c r="D16" s="12">
+        <v>10356653.577031</v>
+      </c>
+      <c r="E16" s="12">
+        <v>3218.1755039999998</v>
+      </c>
+      <c r="F16" s="13">
+        <v>5706</v>
+      </c>
       <c r="P16" s="6">
-        <f>I13</f>
+        <f t="shared" si="5"/>
         <v>60000</v>
       </c>
     </row>
@@ -3820,15 +3831,21 @@
       <c r="A17" s="14">
         <v>10000</v>
       </c>
-      <c r="B17" s="49">
+      <c r="B17" s="2">
         <v>2</v>
       </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
+      <c r="C17" s="15">
+        <v>2570.2896620000001</v>
+      </c>
+      <c r="D17" s="15">
+        <v>5708028.8933659997</v>
+      </c>
+      <c r="E17" s="15">
+        <v>2389.1481520000002</v>
+      </c>
       <c r="F17" s="16"/>
       <c r="P17" s="6">
-        <f>I14</f>
+        <f t="shared" si="5"/>
         <v>65000</v>
       </c>
     </row>
@@ -3836,15 +3853,21 @@
       <c r="A18" s="14">
         <v>10000</v>
       </c>
-      <c r="B18" s="49">
+      <c r="B18" s="2">
         <v>3</v>
       </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
+      <c r="C18" s="15">
+        <v>3701.639048</v>
+      </c>
+      <c r="D18" s="15">
+        <v>2974224.9815380001</v>
+      </c>
+      <c r="E18" s="15">
+        <v>1724.5941499999999</v>
+      </c>
       <c r="F18" s="16"/>
       <c r="P18" s="6">
-        <f>I15</f>
+        <f t="shared" si="5"/>
         <v>70000</v>
       </c>
     </row>
@@ -3852,12 +3875,18 @@
       <c r="A19" s="14">
         <v>10000</v>
       </c>
-      <c r="B19" s="49">
+      <c r="B19" s="2">
         <v>4</v>
       </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
+      <c r="C19" s="15">
+        <v>3384.5157680000002</v>
+      </c>
+      <c r="D19" s="15">
+        <v>1639397.0015120001</v>
+      </c>
+      <c r="E19" s="15">
+        <v>1280.389394</v>
+      </c>
       <c r="F19" s="16"/>
       <c r="I19" s="6"/>
       <c r="P19" s="6">
@@ -3869,12 +3898,18 @@
       <c r="A20" s="14">
         <v>10000</v>
       </c>
-      <c r="B20" s="49">
+      <c r="B20" s="2">
         <v>5</v>
       </c>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
+      <c r="C20" s="15">
+        <v>3235.4788760000001</v>
+      </c>
+      <c r="D20" s="15">
+        <v>1215301.838708</v>
+      </c>
+      <c r="E20" s="15">
+        <v>1102.407293</v>
+      </c>
       <c r="F20" s="16"/>
       <c r="I20" s="6"/>
       <c r="P20" s="6"/>
@@ -3883,12 +3918,18 @@
       <c r="A21" s="14">
         <v>10000</v>
       </c>
-      <c r="B21" s="49">
+      <c r="B21" s="2">
         <v>6</v>
       </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
+      <c r="C21" s="15">
+        <v>4434.9421160000002</v>
+      </c>
+      <c r="D21" s="15">
+        <v>8110956.9532749997</v>
+      </c>
+      <c r="E21" s="15">
+        <v>2847.9741840000002</v>
+      </c>
       <c r="F21" s="16"/>
       <c r="I21" s="6"/>
       <c r="P21" s="6"/>
@@ -3897,12 +3938,18 @@
       <c r="A22" s="14">
         <v>10000</v>
       </c>
-      <c r="B22" s="49">
+      <c r="B22" s="2">
         <v>7</v>
       </c>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
+      <c r="C22" s="15">
+        <v>3956.1814509999999</v>
+      </c>
+      <c r="D22" s="15">
+        <v>4059705.6096029999</v>
+      </c>
+      <c r="E22" s="15">
+        <v>2014.8711149999999</v>
+      </c>
       <c r="F22" s="16"/>
       <c r="I22" s="6"/>
       <c r="P22" s="6"/>
@@ -3911,12 +3958,18 @@
       <c r="A23" s="14">
         <v>10000</v>
       </c>
-      <c r="B23" s="49">
+      <c r="B23" s="2">
         <v>8</v>
       </c>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
+      <c r="C23" s="15">
+        <v>5087.5308370000002</v>
+      </c>
+      <c r="D23" s="15">
+        <v>4810026.3224090002</v>
+      </c>
+      <c r="E23" s="15">
+        <v>2193.1772209999999</v>
+      </c>
       <c r="F23" s="16"/>
       <c r="I23" s="6"/>
       <c r="P23" s="6"/>
@@ -3928,9 +3981,15 @@
       <c r="B24" s="18">
         <v>9</v>
       </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
+      <c r="C24" s="19">
+        <v>4770.4075570000005</v>
+      </c>
+      <c r="D24" s="19">
+        <v>4097535.9674180001</v>
+      </c>
+      <c r="E24" s="19">
+        <v>2024.237132</v>
+      </c>
       <c r="F24" s="20"/>
       <c r="I24" s="6"/>
       <c r="P24" s="6"/>
@@ -3942,9 +4001,18 @@
       <c r="B25" s="2">
         <v>1</v>
       </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
+      <c r="C25" s="7">
+        <v>3049.1101739999999</v>
+      </c>
+      <c r="D25" s="7">
+        <v>10472240.012588</v>
+      </c>
+      <c r="E25" s="7">
+        <v>3236.0840549999998</v>
+      </c>
+      <c r="F25" s="2">
+        <v>8582</v>
+      </c>
       <c r="I25" s="6"/>
       <c r="P25" s="6">
         <f t="shared" si="2"/>
@@ -3958,9 +4026,15 @@
       <c r="B26" s="2">
         <v>2</v>
       </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
+      <c r="C26" s="7">
+        <v>2567.1164480000002</v>
+      </c>
+      <c r="D26" s="7">
+        <v>5759736.1639900003</v>
+      </c>
+      <c r="E26" s="7">
+        <v>2399.9450339999999</v>
+      </c>
       <c r="I26" s="6"/>
       <c r="P26" s="6">
         <f t="shared" si="2"/>
@@ -3974,9 +4048,15 @@
       <c r="B27" s="2">
         <v>3</v>
       </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
+      <c r="C27" s="7">
+        <v>3710.2449280000001</v>
+      </c>
+      <c r="D27" s="7">
+        <v>2985074.8147470001</v>
+      </c>
+      <c r="E27" s="7">
+        <v>1727.7369060000001</v>
+      </c>
       <c r="I27" s="6"/>
       <c r="P27" s="6">
         <f t="shared" si="2"/>
@@ -3990,9 +4070,15 @@
       <c r="B28" s="2">
         <v>4</v>
       </c>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
+      <c r="C28" s="7">
+        <v>3389.0880080000002</v>
+      </c>
+      <c r="D28" s="7">
+        <v>1632999.419431</v>
+      </c>
+      <c r="E28" s="7">
+        <v>1277.888657</v>
+      </c>
       <c r="I28" s="6"/>
       <c r="P28" s="6"/>
     </row>
@@ -4003,9 +4089,15 @@
       <c r="B29" s="2">
         <v>5</v>
       </c>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
+      <c r="C29" s="7">
+        <v>3239.1059740000001</v>
+      </c>
+      <c r="D29" s="7">
+        <v>1208470.435972</v>
+      </c>
+      <c r="E29" s="7">
+        <v>1099.3045239999999</v>
+      </c>
       <c r="I29" s="6"/>
       <c r="P29" s="6"/>
     </row>
@@ -4016,9 +4108,15 @@
       <c r="B30" s="2">
         <v>6</v>
       </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
+      <c r="C30" s="7">
+        <v>4444.8130270000001</v>
+      </c>
+      <c r="D30" s="7">
+        <v>8150757.8341779998</v>
+      </c>
+      <c r="E30" s="7">
+        <v>2854.953211</v>
+      </c>
       <c r="I30" s="6"/>
       <c r="P30" s="6"/>
     </row>
@@ -4029,9 +4127,15 @@
       <c r="B31" s="2">
         <v>7</v>
       </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
+      <c r="C31" s="7">
+        <v>3962.8193019999999</v>
+      </c>
+      <c r="D31" s="7">
+        <v>4059551.4531720001</v>
+      </c>
+      <c r="E31" s="7">
+        <v>2014.83286</v>
+      </c>
       <c r="I31" s="6"/>
       <c r="P31" s="6"/>
     </row>
@@ -4042,9 +4146,15 @@
       <c r="B32" s="2">
         <v>8</v>
       </c>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
+      <c r="C32" s="7">
+        <v>5105.9477809999998</v>
+      </c>
+      <c r="D32" s="7">
+        <v>4800711.6853759997</v>
+      </c>
+      <c r="E32" s="7">
+        <v>2191.052643</v>
+      </c>
       <c r="I32" s="6"/>
       <c r="P32" s="6"/>
     </row>
@@ -4055,9 +4165,15 @@
       <c r="B33" s="2">
         <v>9</v>
       </c>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
+      <c r="C33" s="7">
+        <v>4784.7908610000004</v>
+      </c>
+      <c r="D33" s="7">
+        <v>4094194.2117400002</v>
+      </c>
+      <c r="E33" s="7">
+        <v>2023.4115280000001</v>
+      </c>
       <c r="I33" s="6"/>
       <c r="P33" s="6">
         <f t="shared" si="2"/>
@@ -4071,81 +4187,125 @@
       <c r="B34" s="11">
         <v>1</v>
       </c>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="13"/>
+      <c r="C34" s="50">
+        <v>3076.2222879999999</v>
+      </c>
+      <c r="D34" s="50">
+        <v>10667607.274947001</v>
+      </c>
+      <c r="E34" s="50">
+        <v>3266.1303210000001</v>
+      </c>
+      <c r="F34" s="13">
+        <v>20300</v>
+      </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A35" s="14">
         <v>20000</v>
       </c>
-      <c r="B35" s="49">
+      <c r="B35" s="2">
         <v>2</v>
       </c>
-      <c r="C35" s="22"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="22"/>
+      <c r="C35" s="51">
+        <v>2583.7063280000002</v>
+      </c>
+      <c r="D35" s="51">
+        <v>5847004.8829929996</v>
+      </c>
+      <c r="E35" s="51">
+        <v>2418.0580810000001</v>
+      </c>
       <c r="F35" s="16"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A36" s="14">
         <v>20000</v>
       </c>
-      <c r="B36" s="49">
+      <c r="B36" s="2">
         <v>3</v>
       </c>
-      <c r="C36" s="22"/>
-      <c r="D36" s="22"/>
-      <c r="E36" s="22"/>
+      <c r="C36" s="51">
+        <v>3739.6070580000001</v>
+      </c>
+      <c r="D36" s="51">
+        <v>3015152.2028939999</v>
+      </c>
+      <c r="E36" s="51">
+        <v>1736.419363</v>
+      </c>
       <c r="F36" s="16"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A37" s="14">
         <v>20000</v>
       </c>
-      <c r="B37" s="49">
+      <c r="B37" s="2">
         <v>4</v>
       </c>
-      <c r="C37" s="22"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
+      <c r="C37" s="51">
+        <v>3411.4610699999998</v>
+      </c>
+      <c r="D37" s="51">
+        <v>1642418.842317</v>
+      </c>
+      <c r="E37" s="51">
+        <v>1281.5688990000001</v>
+      </c>
       <c r="F37" s="16"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A38" s="14">
         <v>20000</v>
       </c>
-      <c r="B38" s="49">
+      <c r="B38" s="2">
         <v>5</v>
       </c>
-      <c r="C38" s="22"/>
-      <c r="D38" s="22"/>
-      <c r="E38" s="22"/>
+      <c r="C38" s="51">
+        <v>3257.8568220000002</v>
+      </c>
+      <c r="D38" s="51">
+        <v>1209859.1781329999</v>
+      </c>
+      <c r="E38" s="51">
+        <v>1099.935988</v>
+      </c>
       <c r="F38" s="16"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A39" s="14">
         <v>20000</v>
       </c>
-      <c r="B39" s="49">
+      <c r="B39" s="2">
         <v>6</v>
       </c>
-      <c r="C39" s="22"/>
-      <c r="D39" s="22"/>
-      <c r="E39" s="22"/>
+      <c r="C39" s="51">
+        <v>4488.2284440000003</v>
+      </c>
+      <c r="D39" s="51">
+        <v>8238828.028895</v>
+      </c>
+      <c r="E39" s="51">
+        <v>2870.3358739999999</v>
+      </c>
       <c r="F39" s="16"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A40" s="14">
         <v>20000</v>
       </c>
-      <c r="B40" s="49">
+      <c r="B40" s="2">
         <v>7</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
+      <c r="C40" s="51">
+        <v>3995.7124840000001</v>
+      </c>
+      <c r="D40" s="51">
+        <v>4082110.0733010001</v>
+      </c>
+      <c r="E40" s="51">
+        <v>2020.423241</v>
+      </c>
       <c r="F40" s="16"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.35">
@@ -4155,9 +4315,15 @@
       <c r="B41" s="2">
         <v>8</v>
       </c>
-      <c r="C41" s="22"/>
-      <c r="D41" s="22"/>
-      <c r="E41" s="22"/>
+      <c r="C41" s="51">
+        <v>5151.6132129999996</v>
+      </c>
+      <c r="D41" s="51">
+        <v>4802509.0502460003</v>
+      </c>
+      <c r="E41" s="51">
+        <v>2191.4627650000002</v>
+      </c>
       <c r="F41" s="16"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.35">
@@ -4167,9 +4333,15 @@
       <c r="B42" s="18">
         <v>9</v>
       </c>
-      <c r="C42" s="23"/>
-      <c r="D42" s="23"/>
-      <c r="E42" s="23"/>
+      <c r="C42" s="52">
+        <v>4823.4672259999998</v>
+      </c>
+      <c r="D42" s="52">
+        <v>4116503.2375119999</v>
+      </c>
+      <c r="E42" s="52">
+        <v>2028.9167649999999</v>
+      </c>
       <c r="F42" s="20"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.35">
@@ -4179,9 +4351,18 @@
       <c r="B43" s="2">
         <v>1</v>
       </c>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
+      <c r="C43" s="7">
+        <v>3088.9511240000002</v>
+      </c>
+      <c r="D43" s="7">
+        <v>10567907.476219</v>
+      </c>
+      <c r="E43" s="7">
+        <v>3250.8318129999998</v>
+      </c>
+      <c r="F43" s="2">
+        <v>19609</v>
+      </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A44" s="6">
@@ -4190,9 +4371,15 @@
       <c r="B44" s="2">
         <v>2</v>
       </c>
-      <c r="C44" s="7"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
+      <c r="C44" s="7">
+        <v>2594.8967670000002</v>
+      </c>
+      <c r="D44" s="7">
+        <v>5805033.8766249996</v>
+      </c>
+      <c r="E44" s="7">
+        <v>2409.3637910000002</v>
+      </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A45" s="6">
@@ -4201,9 +4388,15 @@
       <c r="B45" s="2">
         <v>3</v>
       </c>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
+      <c r="C45" s="7">
+        <v>3731.2100310000001</v>
+      </c>
+      <c r="D45" s="7">
+        <v>3009602.8143659998</v>
+      </c>
+      <c r="E45" s="7">
+        <v>1734.8206869999999</v>
+      </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A46" s="6">
@@ -4212,9 +4405,15 @@
       <c r="B46" s="2">
         <v>4</v>
       </c>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
+      <c r="C46" s="7">
+        <v>3402.6427779999999</v>
+      </c>
+      <c r="D46" s="7">
+        <v>1645985.946888</v>
+      </c>
+      <c r="E46" s="7">
+        <v>1282.959838</v>
+      </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A47" s="6">
@@ -4223,9 +4422,15 @@
       <c r="B47" s="2">
         <v>5</v>
       </c>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
+      <c r="C47" s="7">
+        <v>3251.8156250000002</v>
+      </c>
+      <c r="D47" s="7">
+        <v>1220391.528616</v>
+      </c>
+      <c r="E47" s="7">
+        <v>1104.7133240000001</v>
+      </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A48" s="6">
@@ -4234,9 +4439,15 @@
       <c r="B48" s="2">
         <v>6</v>
       </c>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
+      <c r="C48" s="7">
+        <v>4484.8039639999997</v>
+      </c>
+      <c r="D48" s="7">
+        <v>8250717.0625440003</v>
+      </c>
+      <c r="E48" s="7">
+        <v>2872.4061449999999</v>
+      </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="6">
@@ -4245,9 +4456,15 @@
       <c r="B49" s="2">
         <v>7</v>
       </c>
-      <c r="C49" s="7"/>
-      <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
+      <c r="C49" s="7">
+        <v>3990.7496059999999</v>
+      </c>
+      <c r="D49" s="7">
+        <v>4111347.1126350001</v>
+      </c>
+      <c r="E49" s="7">
+        <v>2027.6457069999999</v>
+      </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" s="6">
@@ -4256,9 +4473,15 @@
       <c r="B50" s="2">
         <v>8</v>
       </c>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
+      <c r="C50" s="7">
+        <v>5127.0628699999997</v>
+      </c>
+      <c r="D50" s="7">
+        <v>4813513.8855370004</v>
+      </c>
+      <c r="E50" s="7">
+        <v>2193.9721709999999</v>
+      </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="6">
@@ -4267,9 +4490,15 @@
       <c r="B51" s="2">
         <v>9</v>
       </c>
-      <c r="C51" s="7"/>
-      <c r="D51" s="7"/>
-      <c r="E51" s="7"/>
+      <c r="C51" s="7">
+        <v>4798.4956169999996</v>
+      </c>
+      <c r="D51" s="7">
+        <v>4093820.9420520002</v>
+      </c>
+      <c r="E51" s="7">
+        <v>2023.3192879999999</v>
+      </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" s="10">
@@ -4287,7 +4516,7 @@
       <c r="A53" s="14">
         <v>30000</v>
       </c>
-      <c r="B53" s="49">
+      <c r="B53" s="2">
         <v>2</v>
       </c>
       <c r="C53" s="15"/>
@@ -4299,7 +4528,7 @@
       <c r="A54" s="14">
         <v>30000</v>
       </c>
-      <c r="B54" s="49">
+      <c r="B54" s="2">
         <v>3</v>
       </c>
       <c r="C54" s="15"/>
@@ -4311,7 +4540,7 @@
       <c r="A55" s="14">
         <v>30000</v>
       </c>
-      <c r="B55" s="49">
+      <c r="B55" s="2">
         <v>4</v>
       </c>
       <c r="C55" s="15"/>
@@ -4323,7 +4552,7 @@
       <c r="A56" s="14">
         <v>30000</v>
       </c>
-      <c r="B56" s="49">
+      <c r="B56" s="2">
         <v>5</v>
       </c>
       <c r="C56" s="15"/>
@@ -4335,7 +4564,7 @@
       <c r="A57" s="14">
         <v>30000</v>
       </c>
-      <c r="B57" s="49">
+      <c r="B57" s="2">
         <v>6</v>
       </c>
       <c r="C57" s="15"/>
@@ -4494,7 +4723,7 @@
       <c r="A71" s="14">
         <v>40000</v>
       </c>
-      <c r="B71" s="49">
+      <c r="B71" s="2">
         <v>2</v>
       </c>
       <c r="C71" s="15"/>
@@ -4506,7 +4735,7 @@
       <c r="A72" s="14">
         <v>40000</v>
       </c>
-      <c r="B72" s="49">
+      <c r="B72" s="2">
         <v>3</v>
       </c>
       <c r="C72" s="15"/>
@@ -4518,7 +4747,7 @@
       <c r="A73" s="14">
         <v>40000</v>
       </c>
-      <c r="B73" s="49">
+      <c r="B73" s="2">
         <v>4</v>
       </c>
       <c r="C73" s="15"/>
@@ -4530,7 +4759,7 @@
       <c r="A74" s="14">
         <v>40000</v>
       </c>
-      <c r="B74" s="49">
+      <c r="B74" s="2">
         <v>5</v>
       </c>
       <c r="C74" s="15"/>
@@ -4542,7 +4771,7 @@
       <c r="A75" s="14">
         <v>40000</v>
       </c>
-      <c r="B75" s="49">
+      <c r="B75" s="2">
         <v>6</v>
       </c>
       <c r="C75" s="15"/>
@@ -4701,7 +4930,7 @@
       <c r="A89" s="14">
         <v>50000</v>
       </c>
-      <c r="B89" s="49">
+      <c r="B89" s="2">
         <v>2</v>
       </c>
       <c r="C89" s="15"/>
@@ -4713,7 +4942,7 @@
       <c r="A90" s="14">
         <v>50000</v>
       </c>
-      <c r="B90" s="49">
+      <c r="B90" s="2">
         <v>3</v>
       </c>
       <c r="C90" s="15"/>
@@ -4725,7 +4954,7 @@
       <c r="A91" s="14">
         <v>50000</v>
       </c>
-      <c r="B91" s="49">
+      <c r="B91" s="2">
         <v>4</v>
       </c>
       <c r="C91" s="15"/>
@@ -4737,7 +4966,7 @@
       <c r="A92" s="14">
         <v>50000</v>
       </c>
-      <c r="B92" s="49">
+      <c r="B92" s="2">
         <v>5</v>
       </c>
       <c r="C92" s="15"/>
@@ -4749,7 +4978,7 @@
       <c r="A93" s="14">
         <v>50000</v>
       </c>
-      <c r="B93" s="49">
+      <c r="B93" s="2">
         <v>6</v>
       </c>
       <c r="C93" s="15"/>
@@ -5115,7 +5344,7 @@
       <c r="A125" s="14">
         <v>70000</v>
       </c>
-      <c r="B125" s="49">
+      <c r="B125" s="2">
         <v>2</v>
       </c>
       <c r="C125" s="15"/>
@@ -5127,7 +5356,7 @@
       <c r="A126" s="14">
         <v>70000</v>
       </c>
-      <c r="B126" s="49">
+      <c r="B126" s="2">
         <v>3</v>
       </c>
       <c r="C126" s="15"/>
@@ -5139,7 +5368,7 @@
       <c r="A127" s="14">
         <v>70000</v>
       </c>
-      <c r="B127" s="49">
+      <c r="B127" s="2">
         <v>4</v>
       </c>
       <c r="C127" s="15"/>
@@ -5151,7 +5380,7 @@
       <c r="A128" s="14">
         <v>70000</v>
       </c>
-      <c r="B128" s="49">
+      <c r="B128" s="2">
         <v>5</v>
       </c>
       <c r="C128" s="15"/>
@@ -5163,7 +5392,7 @@
       <c r="A129" s="14">
         <v>70000</v>
       </c>
-      <c r="B129" s="49">
+      <c r="B129" s="2">
         <v>6</v>
       </c>
       <c r="C129" s="15"/>
@@ -5212,16 +5441,6 @@
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A14:F14"/>
   </mergeCells>
-  <conditionalFormatting sqref="J13:O14">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color theme="9" tint="0.59999389629810485"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="J3:J15">
     <cfRule type="colorScale" priority="8">
       <colorScale>
@@ -5505,7 +5724,7 @@
       <c r="B11" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="50" t="s">
+      <c r="C11" s="45" t="s">
         <v>16</v>
       </c>
       <c r="D11" t="s">
@@ -5516,13 +5735,13 @@
       <c r="A12">
         <v>0</v>
       </c>
-      <c r="B12" s="50">
+      <c r="B12" s="45">
         <v>0</v>
       </c>
-      <c r="C12" s="50">
+      <c r="C12" s="45">
         <v>0</v>
       </c>
-      <c r="D12" s="50">
+      <c r="D12" s="45">
         <v>0</v>
       </c>
     </row>
@@ -5530,13 +5749,13 @@
       <c r="A13">
         <v>1</v>
       </c>
-      <c r="B13" s="50">
+      <c r="B13" s="45">
         <v>3079.9488820000001</v>
       </c>
-      <c r="C13" s="50">
+      <c r="C13" s="45">
         <v>10578820</v>
       </c>
-      <c r="D13" s="50">
+      <c r="D13" s="45">
         <v>3252.509963</v>
       </c>
     </row>
@@ -5544,13 +5763,13 @@
       <c r="A14">
         <v>2</v>
       </c>
-      <c r="B14" s="50">
+      <c r="B14" s="45">
         <v>2589.0103300000001</v>
       </c>
-      <c r="C14" s="50">
+      <c r="C14" s="45">
         <v>5804110</v>
       </c>
-      <c r="D14" s="50">
+      <c r="D14" s="45">
         <v>2409.1720749999999</v>
       </c>
     </row>
@@ -5558,13 +5777,13 @@
       <c r="A15">
         <v>3</v>
       </c>
-      <c r="B15" s="50">
+      <c r="B15" s="45">
         <v>3729.5815219999999</v>
       </c>
-      <c r="C15" s="50">
+      <c r="C15" s="45">
         <v>3012089</v>
       </c>
-      <c r="D15" s="50">
+      <c r="D15" s="45">
         <v>1735.5371970000001</v>
       </c>
     </row>
@@ -5572,13 +5791,13 @@
       <c r="A16">
         <v>4</v>
       </c>
-      <c r="B16" s="50">
+      <c r="B16" s="45">
         <v>3402.7270549999998</v>
       </c>
-      <c r="C16" s="50">
+      <c r="C16" s="45">
         <v>1645894</v>
       </c>
-      <c r="D16" s="50">
+      <c r="D16" s="45">
         <v>1282.924162</v>
       </c>
     </row>
@@ -5586,13 +5805,13 @@
       <c r="A17">
         <v>5</v>
       </c>
-      <c r="B17" s="50">
+      <c r="B17" s="45">
         <v>3251.2381350000001</v>
       </c>
-      <c r="C17" s="50">
+      <c r="C17" s="45">
         <v>1215558</v>
       </c>
-      <c r="D17" s="50">
+      <c r="D17" s="45">
         <v>1102.5234109999999</v>
       </c>
     </row>
@@ -5600,13 +5819,13 @@
       <c r="A18">
         <v>6</v>
       </c>
-      <c r="B18" s="50">
+      <c r="B18" s="45">
         <v>4477.8493330000001</v>
       </c>
-      <c r="C18" s="50">
+      <c r="C18" s="45">
         <v>8230023</v>
       </c>
-      <c r="D18" s="50">
+      <c r="D18" s="45">
         <v>2868.8015869999999</v>
       </c>
     </row>
@@ -5614,13 +5833,13 @@
       <c r="A19">
         <v>7</v>
       </c>
-      <c r="B19" s="50">
+      <c r="B19" s="45">
         <v>3986.910781</v>
       </c>
-      <c r="C19" s="50">
+      <c r="C19" s="45">
         <v>4091321</v>
       </c>
-      <c r="D19" s="50">
+      <c r="D19" s="45">
         <v>2022.701468</v>
       </c>
     </row>
@@ -5628,13 +5847,13 @@
       <c r="A20">
         <v>8</v>
       </c>
-      <c r="B20" s="50">
+      <c r="B20" s="45">
         <v>5127.4819710000002</v>
       </c>
-      <c r="C20" s="50">
+      <c r="C20" s="45">
         <v>4814613</v>
       </c>
-      <c r="D20" s="50">
+      <c r="D20" s="45">
         <v>2194.222569</v>
       </c>
     </row>
@@ -5642,13 +5861,13 @@
       <c r="A21">
         <v>9</v>
       </c>
-      <c r="B21" s="50">
+      <c r="B21" s="45">
         <v>4800.6275050000004</v>
       </c>
-      <c r="C21" s="50">
+      <c r="C21" s="45">
         <v>4108687</v>
       </c>
-      <c r="D21" s="50">
+      <c r="D21" s="45">
         <v>2026.989632</v>
       </c>
     </row>
@@ -5661,7 +5880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07E2FAA7-AF33-4595-8B19-D05C042724E7}">
   <dimension ref="A1:P357"/>
   <sheetViews>
-    <sheetView topLeftCell="A68" zoomScale="86" workbookViewId="0">
+    <sheetView zoomScale="86" workbookViewId="0">
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
@@ -6497,14 +6716,14 @@
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A31" s="45" t="s">
+      <c r="A31" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="46"/>
-      <c r="C31" s="46"/>
-      <c r="D31" s="46"/>
-      <c r="E31" s="46"/>
-      <c r="F31" s="47"/>
+      <c r="B31" s="48"/>
+      <c r="C31" s="48"/>
+      <c r="D31" s="48"/>
+      <c r="E31" s="48"/>
+      <c r="F31" s="49"/>
     </row>
     <row r="32" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="2" t="s">

</xml_diff>

<commit_message>
Finish simulation check for sample_medium
</commit_message>
<xml_diff>
--- a/simulation_check.xlsx
+++ b/simulation_check.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\C-Final-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2B2023-0FB3-4D00-B318-6ED407597B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD375860-DACF-4EED-888E-86475BE3986E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{603FAE4F-A0F0-414C-B275-6F2A5451B931}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="35">
   <si>
     <t>simulation #</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>Simulations</t>
+  </si>
+  <si>
+    <t>Run_time</t>
   </si>
 </sst>
 </file>
@@ -452,7 +455,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -575,15 +578,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -902,7 +902,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1039,23 +1039,23 @@
       </c>
       <c r="C9" s="27">
         <f>MIN(simulations_medium!$K$3:$K$15)</f>
-        <v>20.723022475219242</v>
+        <v>15.554014002609494</v>
       </c>
       <c r="D9" s="27">
         <f>MIN(simulations_medium!$L$3:$L$15)</f>
-        <v>4.5522546584323731</v>
+        <v>3.943857756386441</v>
       </c>
       <c r="E9" s="27">
         <f>MIN(simulations_medium!$M$3:$M$15)</f>
-        <v>8437.0454593332634</v>
+        <v>7816.7157254445674</v>
       </c>
       <c r="F9" s="27">
         <f>MIN(simulations_medium!$N$3:$N$15)</f>
-        <v>133442937.64094336</v>
+        <v>86516418.678357303</v>
       </c>
       <c r="G9" s="27">
         <f>MIN(simulations_medium!$O$3:$O$15)</f>
-        <v>11551.750414588403</v>
+        <v>9301.4202506045986</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -1068,23 +1068,23 @@
       </c>
       <c r="C10" s="25">
         <f>VLOOKUP(C9,simulations_medium!$K$3:$P$18,6,FALSE)</f>
-        <v>25000</v>
+        <v>40000</v>
       </c>
       <c r="D10" s="25">
         <f>VLOOKUP(D9,simulations_medium!$L$3:$P$18,5,FALSE)</f>
-        <v>25000</v>
+        <v>40000</v>
       </c>
       <c r="E10" s="25">
         <f>VLOOKUP(E9,simulations_medium!$M$3:$P$18,4,FALSE)</f>
-        <v>25000</v>
+        <v>65000</v>
       </c>
       <c r="F10" s="25">
         <f>VLOOKUP(F9,simulations_medium!$N$3:$P$18,3,FALSE)</f>
-        <v>25000</v>
+        <v>65000</v>
       </c>
       <c r="G10" s="25">
         <f>VLOOKUP(G9,simulations_medium!$O$3:$P$18,2,FALSE)</f>
-        <v>25000</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -1183,8 +1183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{544FD0B2-A7ED-4478-8092-5F67F619DD9A}">
   <dimension ref="A1:P64"/>
   <sheetViews>
-    <sheetView topLeftCell="B45" zoomScale="90" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView topLeftCell="B11" zoomScale="90" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1905,6 +1905,9 @@
         <v>3884</v>
       </c>
       <c r="I18" s="6"/>
+      <c r="K18" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="P18" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1930,6 +1933,13 @@
         <v>3884</v>
       </c>
       <c r="I19" s="6"/>
+      <c r="K19" s="8">
+        <v>10000</v>
+      </c>
+      <c r="L19" s="6">
+        <f>VLOOKUP(K19,$A$13:$F$64,6,FALSE)</f>
+        <v>2284</v>
+      </c>
       <c r="P19" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1955,6 +1965,13 @@
         <v>3884</v>
       </c>
       <c r="I20" s="6"/>
+      <c r="K20" s="8">
+        <v>15000</v>
+      </c>
+      <c r="L20" s="6">
+        <f t="shared" ref="L20:L31" si="5">VLOOKUP(K20,$A$16:$F$132,6,FALSE)</f>
+        <v>3884</v>
+      </c>
       <c r="P20" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1979,6 +1996,13 @@
       <c r="F21" s="13">
         <v>6970</v>
       </c>
+      <c r="K21" s="8">
+        <v>20000</v>
+      </c>
+      <c r="L21" s="6">
+        <f t="shared" si="5"/>
+        <v>6970</v>
+      </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="14">
@@ -1999,6 +2023,13 @@
       <c r="F22" s="16">
         <v>6970</v>
       </c>
+      <c r="K22" s="8">
+        <v>25000</v>
+      </c>
+      <c r="L22" s="6">
+        <f t="shared" si="5"/>
+        <v>8343</v>
+      </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" s="14">
@@ -2019,6 +2050,13 @@
       <c r="F23" s="16">
         <v>6970</v>
       </c>
+      <c r="K23" s="8">
+        <v>30000</v>
+      </c>
+      <c r="L23" s="6">
+        <f t="shared" si="5"/>
+        <v>9428</v>
+      </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" s="17">
@@ -2039,6 +2077,13 @@
       <c r="F24" s="20">
         <v>6970</v>
       </c>
+      <c r="K24" s="8">
+        <v>35000</v>
+      </c>
+      <c r="L24" s="6">
+        <f t="shared" si="5"/>
+        <v>10111</v>
+      </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" s="6">
@@ -2059,6 +2104,13 @@
       <c r="F25" s="2">
         <v>8343</v>
       </c>
+      <c r="K25" s="8">
+        <v>40000</v>
+      </c>
+      <c r="L25" s="6">
+        <f t="shared" si="5"/>
+        <v>13979</v>
+      </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" s="6">
@@ -2079,6 +2131,13 @@
       <c r="F26" s="2">
         <v>8343</v>
       </c>
+      <c r="K26" s="8">
+        <v>45000</v>
+      </c>
+      <c r="L26" s="6">
+        <f t="shared" si="5"/>
+        <v>15291</v>
+      </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" s="6">
@@ -2099,6 +2158,13 @@
       <c r="F27" s="2">
         <v>8343</v>
       </c>
+      <c r="K27" s="8">
+        <v>50000</v>
+      </c>
+      <c r="L27" s="6">
+        <f t="shared" si="5"/>
+        <v>17538</v>
+      </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" s="6">
@@ -2119,6 +2185,13 @@
       <c r="F28" s="2">
         <v>8343</v>
       </c>
+      <c r="K28" s="8">
+        <v>55000</v>
+      </c>
+      <c r="L28" s="6">
+        <f t="shared" si="5"/>
+        <v>20935</v>
+      </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" s="10">
@@ -2139,6 +2212,13 @@
       <c r="F29" s="13">
         <v>9428</v>
       </c>
+      <c r="K29" s="8">
+        <v>60000</v>
+      </c>
+      <c r="L29" s="6">
+        <f t="shared" si="5"/>
+        <v>20938</v>
+      </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" s="14">
@@ -2159,6 +2239,13 @@
       <c r="F30" s="16">
         <v>9428</v>
       </c>
+      <c r="K30" s="8">
+        <v>65000</v>
+      </c>
+      <c r="L30" s="6">
+        <f t="shared" si="5"/>
+        <v>24465</v>
+      </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" s="14">
@@ -2178,6 +2265,13 @@
       </c>
       <c r="F31" s="16">
         <v>9428</v>
+      </c>
+      <c r="K31" s="6">
+        <v>70000</v>
+      </c>
+      <c r="L31" s="6">
+        <f t="shared" si="5"/>
+        <v>25274</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.35">
@@ -2847,6 +2941,26 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="J3:J15">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="9" tint="0.59999389629810485"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J13:O14">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="9" tint="0.59999389629810485"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3:K15">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -2856,17 +2970,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J13:O14">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color theme="9" tint="0.59999389629810485"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K15">
+  <conditionalFormatting sqref="L3:L15">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -2876,7 +2980,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L3:L15">
+  <conditionalFormatting sqref="M3:M15">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -2886,7 +2990,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M15">
+  <conditionalFormatting sqref="N3:N15">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -2896,7 +3000,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3:N15">
+  <conditionalFormatting sqref="O3:O15">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2906,13 +3010,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O3:O15">
+  <conditionalFormatting sqref="L19:L31">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color theme="9" tint="0.59999389629810485"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
@@ -3139,8 +3243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32199EA4-1B1E-4F05-B93A-A4002D945EFC}">
   <dimension ref="A1:P132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="90" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43:E51"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3159,7 +3263,7 @@
     <col min="13" max="13" width="12.7265625" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="21" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="8.7265625" style="2" hidden="1" customWidth="1"/>
     <col min="17" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
@@ -3415,32 +3519,32 @@
       <c r="E7" s="45">
         <v>1282.924162</v>
       </c>
-      <c r="I7" s="9">
+      <c r="I7" s="8">
         <v>30000</v>
       </c>
       <c r="J7" s="7">
         <f>AVERAGE(ABS($C$4-C52),ABS($C$5-C53),ABS($C$6-C54),ABS($C$7-C55),ABS($C$8-C56),ABS($C$9-C57),ABS($C$10-C58),ABS($C$11-C59),ABS($C$12-C60))</f>
-        <v>3827.263946</v>
+        <v>10.739881333333162</v>
       </c>
       <c r="K7" s="7">
         <f>AVERAGE(($C$4-C52)^2, ($C$5-C53)^2, ($C$6-C54)^2, ($C$7-C55)^2,($C$8-C56)^2,($C$9-C57)^2,($C$10-C58)^2,($C$11-C59)^2,($C$12-C60)^2)</f>
-        <v>15281291.864947332</v>
+        <v>177.41652258719873</v>
       </c>
       <c r="L7" s="7">
         <f t="shared" si="0"/>
-        <v>3909.1292975478991</v>
+        <v>13.319779374569187</v>
       </c>
       <c r="M7" s="7">
         <f>AVERAGE(ABS($D$4-D52),ABS($D$5-D53),ABS($D$6-D54),ABS($D$7-D55),ABS($D$8-D56),ABS($D$9-D57),ABS($D$10-D58),ABS($D$11-D59),ABS($D$12-D60))</f>
-        <v>4833457.222222222</v>
+        <v>18949.039899333431</v>
       </c>
       <c r="N7" s="7">
         <f>AVERAGE(($D$4-D52)^2, ($D$5-D53)^2, ($D$6-D54)^2, ($D$7-D55)^2,($D$8-D56)^2,($D$9-D57)^2,($D$10-D58)^2,($D$11-D59)^2,($D$12-D60)^2)</f>
-        <v>31488038583147.668</v>
+        <v>616562148.85771608</v>
       </c>
       <c r="O7" s="7">
         <f t="shared" ref="O7:O15" si="3">SQRT(N7)</f>
-        <v>5611420.3712738957</v>
+        <v>24830.669520931489</v>
       </c>
       <c r="P7" s="6">
         <f t="shared" si="2"/>
@@ -3463,34 +3567,37 @@
       <c r="E8" s="45">
         <v>1102.5234109999999</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="8">
         <v>35000</v>
       </c>
       <c r="J8" s="7">
         <f>AVERAGE(ABS($C$4-C61),ABS($C$5-C62),ABS($C$6-C63),ABS($C$7-C64),ABS($C$8-C65),ABS($C$9-C66),ABS($C$10-C67),ABS($C$11-C68),ABS($C$12-C69))</f>
-        <v>3827.263946</v>
+        <v>7.9261505555553713</v>
       </c>
       <c r="K8" s="7">
         <f>AVERAGE(($C$4-C61)^2, ($C$5-C62)^2, ($C$6-C63)^2, ($C$7-C64)^2,($C$8-C65)^2,($C$9-C66)^2,($C$10-C67)^2,($C$11-C68)^2,($C$12-C69)^2)</f>
-        <v>15281291.864947332</v>
+        <v>70.327367245555891</v>
       </c>
       <c r="L8" s="7">
         <f t="shared" ref="L8:L15" si="4">SQRT(K8)</f>
-        <v>3909.1292975478991</v>
+        <v>8.3861413800123774</v>
       </c>
       <c r="M8" s="7">
         <f>AVERAGE(ABS($D$4-D61),ABS($D$5-D62),ABS($D$6-D63),ABS($D$7-D64),ABS($D$8-D65),ABS($D$9-D66),ABS($D$10-D67),ABS($D$11-D68),ABS($D$12-D69))</f>
-        <v>4833457.222222222</v>
+        <v>33370.464146000049</v>
       </c>
       <c r="N8" s="7">
         <f>AVERAGE(($D$4-D61)^2, ($D$5-D62)^2, ($D$6-D63)^2, ($D$7-D64)^2,($D$8-D65)^2,($D$9-D66)^2,($D$10-D67)^2,($D$11-D68)^2,($D$12-D69)^2)</f>
-        <v>31488038583147.668</v>
+        <v>2501155583.5043745</v>
       </c>
       <c r="O8" s="7">
         <f t="shared" si="3"/>
-        <v>5611420.3712738957</v>
-      </c>
-      <c r="P8" s="6"/>
+        <v>50011.554499979051</v>
+      </c>
+      <c r="P8" s="6">
+        <f t="shared" si="2"/>
+        <v>35000</v>
+      </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
@@ -3508,34 +3615,37 @@
       <c r="E9" s="45">
         <v>2868.8015869999999</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="8">
         <v>40000</v>
       </c>
       <c r="J9" s="7">
         <f>AVERAGE(ABS($C$4-C70),ABS($C$5-C71),ABS($C$6-C72),ABS($C$7-C73),ABS($C$8-C74),ABS($C$9-C75),ABS($C$10-C76),ABS($C$11-C77),ABS($C$12-C78))</f>
-        <v>3827.263946</v>
+        <v>3.5251184444445141</v>
       </c>
       <c r="K9" s="7">
         <f>AVERAGE(($C$4-C70)^2, ($C$5-C71)^2, ($C$6-C72)^2, ($C$7-C73)^2,($C$8-C74)^2,($C$9-C75)^2,($C$10-C76)^2,($C$11-C77)^2,($C$12-C78)^2)</f>
-        <v>15281291.864947332</v>
+        <v>15.554014002609494</v>
       </c>
       <c r="L9" s="7">
         <f t="shared" si="4"/>
-        <v>3909.1292975478991</v>
+        <v>3.943857756386441</v>
       </c>
       <c r="M9" s="7">
         <f>AVERAGE(ABS($D$4-D70),ABS($D$5-D71),ABS($D$6-D72),ABS($D$7-D73),ABS($D$8-D74),ABS($D$9-D75),ABS($D$10-D76),ABS($D$11-D77),ABS($D$12-D78))</f>
-        <v>4833457.222222222</v>
+        <v>18757.316034444324</v>
       </c>
       <c r="N9" s="7">
         <f>AVERAGE(($D$4-D70)^2, ($D$5-D71)^2, ($D$6-D72)^2, ($D$7-D73)^2,($D$8-D74)^2,($D$9-D75)^2,($D$10-D76)^2,($D$11-D77)^2,($D$12-D78)^2)</f>
-        <v>31488038583147.668</v>
+        <v>540381050.68917608</v>
       </c>
       <c r="O9" s="7">
         <f t="shared" si="3"/>
-        <v>5611420.3712738957</v>
-      </c>
-      <c r="P9" s="6"/>
+        <v>23246.097536773264</v>
+      </c>
+      <c r="P9" s="6">
+        <f t="shared" si="2"/>
+        <v>40000</v>
+      </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
@@ -3553,34 +3663,37 @@
       <c r="E10" s="45">
         <v>2022.701468</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="8">
         <v>45000</v>
       </c>
       <c r="J10" s="7">
         <f>AVERAGE(ABS($C$4-C79),ABS($C$5-C80),ABS($C$6-C81),ABS($C$7-C82),ABS($C$8-C83),ABS($C$9-C84),ABS($C$10-C85),ABS($C$11-C86),ABS($C$12-C87))</f>
-        <v>3827.263946</v>
+        <v>21.001518666666673</v>
       </c>
       <c r="K10" s="7">
         <f>AVERAGE(($C$4-C79)^2, ($C$5-C80)^2, ($C$6-C81)^2, ($C$7-C82)^2,($C$8-C83)^2,($C$9-C84)^2,($C$10-C85)^2,($C$11-C86)^2,($C$12-C87)^2)</f>
-        <v>15281291.864947332</v>
+        <v>497.81583578546946</v>
       </c>
       <c r="L10" s="7">
         <f t="shared" si="4"/>
-        <v>3909.1292975478991</v>
+        <v>22.311786924974644</v>
       </c>
       <c r="M10" s="7">
         <f>AVERAGE(ABS($D$4-D79),ABS($D$5-D80),ABS($D$6-D81),ABS($D$7-D82),ABS($D$8-D83),ABS($D$9-D84),ABS($D$10-D85),ABS($D$11-D86),ABS($D$12-D87))</f>
-        <v>4833457.222222222</v>
+        <v>32393.628889444335</v>
       </c>
       <c r="N10" s="7">
         <f>AVERAGE(($D$4-D79)^2, ($D$5-D80)^2, ($D$6-D81)^2, ($D$7-D82)^2,($D$8-D83)^2,($D$9-D84)^2,($D$10-D85)^2,($D$11-D86)^2,($D$12-D87)^2)</f>
-        <v>31488038583147.668</v>
+        <v>2005461006.3984532</v>
       </c>
       <c r="O10" s="7">
         <f t="shared" si="3"/>
-        <v>5611420.3712738957</v>
-      </c>
-      <c r="P10" s="6"/>
+        <v>44782.373836125</v>
+      </c>
+      <c r="P10" s="6">
+        <f t="shared" si="2"/>
+        <v>45000</v>
+      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
@@ -3598,36 +3711,36 @@
       <c r="E11" s="45">
         <v>2194.222569</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I11" s="8">
         <v>50000</v>
       </c>
       <c r="J11" s="7">
         <f>AVERAGE(ABS($C$4-C88),ABS($C$5-C89),ABS($C$6-C90),ABS($C$7-C91),ABS($C$8-C92),ABS($C$9-C93),ABS($C$10-C94),ABS($C$11-C95),ABS($C$12-C96))</f>
-        <v>3827.263946</v>
+        <v>11.552367666666619</v>
       </c>
       <c r="K11" s="7">
         <f>AVERAGE(($C$4-C88)^2, ($C$5-C89)^2, ($C$6-C90)^2, ($C$7-C91)^2,($C$8-C92)^2,($C$9-C93)^2,($C$10-C94)^2,($C$11-C95)^2,($C$12-C96)^2)</f>
-        <v>15281291.864947332</v>
+        <v>191.40784690224686</v>
       </c>
       <c r="L11" s="7">
         <f t="shared" si="4"/>
-        <v>3909.1292975478991</v>
+        <v>13.835022475668294</v>
       </c>
       <c r="M11" s="7">
         <f>AVERAGE(ABS($D$4-D88),ABS($D$5-D89),ABS($D$6-D90),ABS($D$7-D91),ABS($D$8-D92),ABS($D$9-D93),ABS($D$10-D94),ABS($D$11-D95),ABS($D$12-D96))</f>
-        <v>4833457.222222222</v>
+        <v>23282.674273111057</v>
       </c>
       <c r="N11" s="7">
         <f>AVERAGE(($D$4-D88)^2, ($D$5-D89)^2, ($D$6-D90)^2, ($D$7-D91)^2,($D$8-D92)^2,($D$9-D93)^2,($D$10-D94)^2,($D$11-D95)^2,($D$12-D96)^2)</f>
-        <v>31488038583147.668</v>
+        <v>1103288902.6666319</v>
       </c>
       <c r="O11" s="7">
         <f t="shared" si="3"/>
-        <v>5611420.3712738957</v>
+        <v>33215.792970613118</v>
       </c>
       <c r="P11" s="6">
-        <f t="shared" ref="P11:P18" si="5">I8</f>
-        <v>35000</v>
+        <f t="shared" si="2"/>
+        <v>50000</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
@@ -3646,69 +3759,69 @@
       <c r="E12" s="45">
         <v>2026.989632</v>
       </c>
-      <c r="I12" s="9">
+      <c r="I12" s="8">
         <v>55000</v>
       </c>
       <c r="J12" s="7">
         <f>AVERAGE(ABS($C$4-C97),ABS($C$5-C98),ABS($C$6-C99),ABS($C$7-C100),ABS($C$8-C101),ABS($C$9-C102),ABS($C$10-C103),ABS($C$11-C104),ABS($C$12-C105))</f>
-        <v>3827.263946</v>
+        <v>14.059312444444409</v>
       </c>
       <c r="K12" s="7">
         <f>AVERAGE(($C$4-C97)^2, ($C$5-C98)^2, ($C$6-C99)^2, ($C$7-C100)^2,($C$8-C101)^2,($C$9-C102)^2,($C$10-C103)^2,($C$11-C104)^2,($C$12-C105)^2)</f>
-        <v>15281291.864947332</v>
+        <v>246.1240734762471</v>
       </c>
       <c r="L12" s="7">
         <f t="shared" si="4"/>
-        <v>3909.1292975478991</v>
+        <v>15.688341960712327</v>
       </c>
       <c r="M12" s="7">
         <f>AVERAGE(ABS($D$4-D97),ABS($D$5-D98),ABS($D$6-D99),ABS($D$7-D100),ABS($D$8-D101),ABS($D$9-D102),ABS($D$10-D103),ABS($D$11-D104),ABS($D$12-D105))</f>
-        <v>4833457.222222222</v>
+        <v>33524.55856888881</v>
       </c>
       <c r="N12" s="7">
         <f>AVERAGE(($D$4-D97)^2, ($D$5-D98)^2, ($D$6-D99)^2, ($D$7-D100)^2,($D$8-D101)^2,($D$9-D102)^2,($D$10-D103)^2,($D$11-D104)^2,($D$12-D105)^2)</f>
-        <v>31488038583147.668</v>
+        <v>2665675967.0067959</v>
       </c>
       <c r="O12" s="7">
         <f t="shared" si="3"/>
-        <v>5611420.3712738957</v>
+        <v>51630.18465013268</v>
       </c>
       <c r="P12" s="6">
-        <f t="shared" si="5"/>
-        <v>40000</v>
+        <f t="shared" si="2"/>
+        <v>55000</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="I13" s="6">
+      <c r="I13" s="8">
         <v>60000</v>
       </c>
       <c r="J13" s="7">
         <f>AVERAGE(ABS($C$4-C106),ABS($C$5-C107),ABS($C$6-C108),ABS($C$7-C109),ABS($C$8-C110),ABS($C$9-C111),ABS($C$10-C112),ABS($C$11-C113),ABS($C$12-C114))</f>
-        <v>3827.263946</v>
+        <v>10.655182444444563</v>
       </c>
       <c r="K13" s="7">
         <f>AVERAGE(($C$4-C106)^2, ($C$5-C107)^2, ($C$6-C108)^2, ($C$7-C109)^2,($C$8-C110)^2,($C$9-C111)^2,($C$10-C112)^2,($C$11-C113)^2,($C$12-C114)^2)</f>
-        <v>15281291.864947332</v>
+        <v>179.58755860466221</v>
       </c>
       <c r="L13" s="7">
         <f t="shared" si="4"/>
-        <v>3909.1292975478991</v>
+        <v>13.40102826669141</v>
       </c>
       <c r="M13" s="7">
         <f>AVERAGE(ABS($D$4-D106),ABS($D$5-D107),ABS($D$6-D108),ABS($D$7-D109),ABS($D$8-D110),ABS($D$9-D111),ABS($D$10-D112),ABS($D$11-D113),ABS($D$12-D114))</f>
-        <v>4833457.222222222</v>
+        <v>39336.040740777767</v>
       </c>
       <c r="N13" s="7">
         <f>AVERAGE(($D$4-D106)^2, ($D$5-D107)^2, ($D$6-D108)^2, ($D$7-D109)^2,($D$8-D110)^2,($D$9-D111)^2,($D$10-D112)^2,($D$11-D113)^2,($D$12-D114)^2)</f>
-        <v>31488038583147.668</v>
+        <v>2309836993.2854748</v>
       </c>
       <c r="O13" s="7">
         <f t="shared" si="3"/>
-        <v>5611420.3712738957</v>
+        <v>48060.763552876218</v>
       </c>
       <c r="P13" s="6">
-        <f t="shared" si="5"/>
-        <v>45000</v>
+        <f t="shared" si="2"/>
+        <v>60000</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.35">
@@ -3720,36 +3833,36 @@
       <c r="D14" s="48"/>
       <c r="E14" s="48"/>
       <c r="F14" s="49"/>
-      <c r="I14" s="6">
+      <c r="I14" s="8">
         <v>65000</v>
       </c>
       <c r="J14" s="7">
         <f>AVERAGE(ABS($C$4-C115),ABS($C$5-C116),ABS($C$6-C117),ABS($C$7-C118),ABS($C$8-C119),ABS($C$9-C120),ABS($C$10-C121),ABS($C$11-C122),ABS($C$12-C123))</f>
-        <v>3827.263946</v>
+        <v>8.4648671111110865</v>
       </c>
       <c r="K14" s="7">
         <f>AVERAGE(($C$4-C115)^2, ($C$5-C116)^2, ($C$6-C117)^2, ($C$7-C118)^2,($C$8-C119)^2,($C$9-C120)^2,($C$10-C121)^2,($C$11-C122)^2,($C$12-C123)^2)</f>
-        <v>15281291.864947332</v>
+        <v>77.227647717929301</v>
       </c>
       <c r="L14" s="7">
         <f t="shared" si="4"/>
-        <v>3909.1292975478991</v>
+        <v>8.7879262467279098</v>
       </c>
       <c r="M14" s="7">
         <f>AVERAGE(ABS($D$4-D115),ABS($D$5-D116),ABS($D$6-D117),ABS($D$7-D118),ABS($D$8-D119),ABS($D$9-D120),ABS($D$10-D121),ABS($D$11-D122),ABS($D$12-D123))</f>
-        <v>4833457.222222222</v>
+        <v>7816.7157254445674</v>
       </c>
       <c r="N14" s="7">
         <f>AVERAGE(($D$4-D115)^2, ($D$5-D116)^2, ($D$6-D117)^2, ($D$7-D118)^2,($D$8-D119)^2,($D$9-D120)^2,($D$10-D121)^2,($D$11-D122)^2,($D$12-D123)^2)</f>
-        <v>31488038583147.668</v>
+        <v>86516418.678357303</v>
       </c>
       <c r="O14" s="7">
         <f t="shared" si="3"/>
-        <v>5611420.3712738957</v>
+        <v>9301.4202506045986</v>
       </c>
       <c r="P14" s="6">
-        <f t="shared" si="5"/>
-        <v>50000</v>
+        <f t="shared" si="2"/>
+        <v>65000</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.35">
@@ -3776,31 +3889,31 @@
       </c>
       <c r="J15" s="7">
         <f>AVERAGE(ABS($C$4-C124),ABS($C$5-C125),ABS($C$6-C126),ABS($C$7-C127),ABS($C$8-C128),ABS($C$9-C129),ABS($C$10-C130),ABS($C$11-C131),ABS($C$12-C132))</f>
-        <v>3827.263946</v>
+        <v>9.203892888888781</v>
       </c>
       <c r="K15" s="7">
         <f>AVERAGE(($C$4-C124)^2, ($C$5-C125)^2, ($C$6-C126)^2, ($C$7-C127)^2,($C$8-C128)^2,($C$9-C129)^2,($C$10-C130)^2,($C$11-C131)^2,($C$12-C132)^2)</f>
-        <v>15281291.864947332</v>
+        <v>110.39476139983289</v>
       </c>
       <c r="L15" s="7">
         <f t="shared" si="4"/>
-        <v>3909.1292975478991</v>
+        <v>10.506891138668607</v>
       </c>
       <c r="M15" s="7">
         <f>AVERAGE(ABS($D$4-D124),ABS($D$5-D125),ABS($D$6-D126),ABS($D$7-D127),ABS($D$8-D128),ABS($D$9-D129),ABS($D$10-D130),ABS($D$11-D131),ABS($D$12-D132))</f>
-        <v>4833457.222222222</v>
+        <v>28404.535184999877</v>
       </c>
       <c r="N15" s="7">
         <f>AVERAGE(($D$4-D124)^2, ($D$5-D125)^2, ($D$6-D126)^2, ($D$7-D127)^2,($D$8-D128)^2,($D$9-D129)^2,($D$10-D130)^2,($D$11-D131)^2,($D$12-D132)^2)</f>
-        <v>31488038583147.668</v>
+        <v>1686284641.824671</v>
       </c>
       <c r="O15" s="7">
         <f t="shared" si="3"/>
-        <v>5611420.3712738957</v>
+        <v>41064.396279802662</v>
       </c>
       <c r="P15" s="6">
-        <f t="shared" si="5"/>
-        <v>55000</v>
+        <f t="shared" si="2"/>
+        <v>70000</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.35">
@@ -3823,8 +3936,8 @@
         <v>5706</v>
       </c>
       <c r="P16" s="6">
-        <f t="shared" si="5"/>
-        <v>60000</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.35">
@@ -3845,8 +3958,8 @@
       </c>
       <c r="F17" s="16"/>
       <c r="P17" s="6">
-        <f t="shared" si="5"/>
-        <v>65000</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.35">
@@ -3866,9 +3979,12 @@
         <v>1724.5941499999999</v>
       </c>
       <c r="F18" s="16"/>
+      <c r="K18" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="P18" s="6">
-        <f t="shared" si="5"/>
-        <v>70000</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.35">
@@ -3889,6 +4005,13 @@
       </c>
       <c r="F19" s="16"/>
       <c r="I19" s="6"/>
+      <c r="K19" s="8">
+        <v>10000</v>
+      </c>
+      <c r="L19" s="6">
+        <f>VLOOKUP(K19,$A$16:$F$132,6,FALSE)</f>
+        <v>5706</v>
+      </c>
       <c r="P19" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3912,6 +4035,13 @@
       </c>
       <c r="F20" s="16"/>
       <c r="I20" s="6"/>
+      <c r="K20" s="8">
+        <v>15000</v>
+      </c>
+      <c r="L20" s="6">
+        <f t="shared" ref="L20:L31" si="5">VLOOKUP(K20,$A$16:$F$132,6,FALSE)</f>
+        <v>8582</v>
+      </c>
       <c r="P20" s="6"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.35">
@@ -3932,6 +4062,13 @@
       </c>
       <c r="F21" s="16"/>
       <c r="I21" s="6"/>
+      <c r="K21" s="8">
+        <v>20000</v>
+      </c>
+      <c r="L21" s="6">
+        <f t="shared" si="5"/>
+        <v>20300</v>
+      </c>
       <c r="P21" s="6"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.35">
@@ -3952,6 +4089,13 @@
       </c>
       <c r="F22" s="16"/>
       <c r="I22" s="6"/>
+      <c r="K22" s="8">
+        <v>25000</v>
+      </c>
+      <c r="L22" s="6">
+        <f t="shared" si="5"/>
+        <v>19609</v>
+      </c>
       <c r="P22" s="6"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.35">
@@ -3972,6 +4116,13 @@
       </c>
       <c r="F23" s="16"/>
       <c r="I23" s="6"/>
+      <c r="K23" s="8">
+        <v>30000</v>
+      </c>
+      <c r="L23" s="6">
+        <f t="shared" si="5"/>
+        <v>32812</v>
+      </c>
       <c r="P23" s="6"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.35">
@@ -3992,6 +4143,13 @@
       </c>
       <c r="F24" s="20"/>
       <c r="I24" s="6"/>
+      <c r="K24" s="8">
+        <v>35000</v>
+      </c>
+      <c r="L24" s="6">
+        <f t="shared" si="5"/>
+        <v>24192</v>
+      </c>
       <c r="P24" s="6"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.35">
@@ -4014,6 +4172,13 @@
         <v>8582</v>
       </c>
       <c r="I25" s="6"/>
+      <c r="K25" s="8">
+        <v>40000</v>
+      </c>
+      <c r="L25" s="6">
+        <f t="shared" si="5"/>
+        <v>34977</v>
+      </c>
       <c r="P25" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4036,6 +4201,13 @@
         <v>2399.9450339999999</v>
       </c>
       <c r="I26" s="6"/>
+      <c r="K26" s="8">
+        <v>45000</v>
+      </c>
+      <c r="L26" s="6">
+        <f t="shared" si="5"/>
+        <v>42096</v>
+      </c>
       <c r="P26" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4058,6 +4230,13 @@
         <v>1727.7369060000001</v>
       </c>
       <c r="I27" s="6"/>
+      <c r="K27" s="8">
+        <v>50000</v>
+      </c>
+      <c r="L27" s="6">
+        <f t="shared" si="5"/>
+        <v>43831</v>
+      </c>
       <c r="P27" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4080,6 +4259,13 @@
         <v>1277.888657</v>
       </c>
       <c r="I28" s="6"/>
+      <c r="K28" s="8">
+        <v>55000</v>
+      </c>
+      <c r="L28" s="6">
+        <f t="shared" si="5"/>
+        <v>153110</v>
+      </c>
       <c r="P28" s="6"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.35">
@@ -4099,6 +4285,13 @@
         <v>1099.3045239999999</v>
       </c>
       <c r="I29" s="6"/>
+      <c r="K29" s="8">
+        <v>60000</v>
+      </c>
+      <c r="L29" s="6">
+        <f t="shared" si="5"/>
+        <v>74655</v>
+      </c>
       <c r="P29" s="6"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.35">
@@ -4118,6 +4311,13 @@
         <v>2854.953211</v>
       </c>
       <c r="I30" s="6"/>
+      <c r="K30" s="8">
+        <v>65000</v>
+      </c>
+      <c r="L30" s="6">
+        <f t="shared" si="5"/>
+        <v>124032</v>
+      </c>
       <c r="P30" s="6"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.35">
@@ -4137,6 +4337,13 @@
         <v>2014.83286</v>
       </c>
       <c r="I31" s="6"/>
+      <c r="K31" s="6">
+        <v>70000</v>
+      </c>
+      <c r="L31" s="6">
+        <f t="shared" si="5"/>
+        <v>137495</v>
+      </c>
       <c r="P31" s="6"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.35">
@@ -4187,13 +4394,13 @@
       <c r="B34" s="11">
         <v>1</v>
       </c>
-      <c r="C34" s="50">
+      <c r="C34" s="12">
         <v>3076.2222879999999</v>
       </c>
-      <c r="D34" s="50">
+      <c r="D34" s="12">
         <v>10667607.274947001</v>
       </c>
-      <c r="E34" s="50">
+      <c r="E34" s="12">
         <v>3266.1303210000001</v>
       </c>
       <c r="F34" s="13">
@@ -4207,13 +4414,13 @@
       <c r="B35" s="2">
         <v>2</v>
       </c>
-      <c r="C35" s="51">
+      <c r="C35" s="15">
         <v>2583.7063280000002</v>
       </c>
-      <c r="D35" s="51">
+      <c r="D35" s="15">
         <v>5847004.8829929996</v>
       </c>
-      <c r="E35" s="51">
+      <c r="E35" s="15">
         <v>2418.0580810000001</v>
       </c>
       <c r="F35" s="16"/>
@@ -4225,13 +4432,13 @@
       <c r="B36" s="2">
         <v>3</v>
       </c>
-      <c r="C36" s="51">
+      <c r="C36" s="15">
         <v>3739.6070580000001</v>
       </c>
-      <c r="D36" s="51">
+      <c r="D36" s="15">
         <v>3015152.2028939999</v>
       </c>
-      <c r="E36" s="51">
+      <c r="E36" s="15">
         <v>1736.419363</v>
       </c>
       <c r="F36" s="16"/>
@@ -4243,13 +4450,13 @@
       <c r="B37" s="2">
         <v>4</v>
       </c>
-      <c r="C37" s="51">
+      <c r="C37" s="15">
         <v>3411.4610699999998</v>
       </c>
-      <c r="D37" s="51">
+      <c r="D37" s="15">
         <v>1642418.842317</v>
       </c>
-      <c r="E37" s="51">
+      <c r="E37" s="15">
         <v>1281.5688990000001</v>
       </c>
       <c r="F37" s="16"/>
@@ -4261,13 +4468,13 @@
       <c r="B38" s="2">
         <v>5</v>
       </c>
-      <c r="C38" s="51">
+      <c r="C38" s="15">
         <v>3257.8568220000002</v>
       </c>
-      <c r="D38" s="51">
+      <c r="D38" s="15">
         <v>1209859.1781329999</v>
       </c>
-      <c r="E38" s="51">
+      <c r="E38" s="15">
         <v>1099.935988</v>
       </c>
       <c r="F38" s="16"/>
@@ -4279,13 +4486,13 @@
       <c r="B39" s="2">
         <v>6</v>
       </c>
-      <c r="C39" s="51">
+      <c r="C39" s="15">
         <v>4488.2284440000003</v>
       </c>
-      <c r="D39" s="51">
+      <c r="D39" s="15">
         <v>8238828.028895</v>
       </c>
-      <c r="E39" s="51">
+      <c r="E39" s="15">
         <v>2870.3358739999999</v>
       </c>
       <c r="F39" s="16"/>
@@ -4297,13 +4504,13 @@
       <c r="B40" s="2">
         <v>7</v>
       </c>
-      <c r="C40" s="51">
+      <c r="C40" s="15">
         <v>3995.7124840000001</v>
       </c>
-      <c r="D40" s="51">
+      <c r="D40" s="15">
         <v>4082110.0733010001</v>
       </c>
-      <c r="E40" s="51">
+      <c r="E40" s="15">
         <v>2020.423241</v>
       </c>
       <c r="F40" s="16"/>
@@ -4315,13 +4522,13 @@
       <c r="B41" s="2">
         <v>8</v>
       </c>
-      <c r="C41" s="51">
+      <c r="C41" s="15">
         <v>5151.6132129999996</v>
       </c>
-      <c r="D41" s="51">
+      <c r="D41" s="15">
         <v>4802509.0502460003</v>
       </c>
-      <c r="E41" s="51">
+      <c r="E41" s="15">
         <v>2191.4627650000002</v>
       </c>
       <c r="F41" s="16"/>
@@ -4333,13 +4540,13 @@
       <c r="B42" s="18">
         <v>9</v>
       </c>
-      <c r="C42" s="52">
+      <c r="C42" s="19">
         <v>4823.4672259999998</v>
       </c>
-      <c r="D42" s="52">
+      <c r="D42" s="19">
         <v>4116503.2375119999</v>
       </c>
-      <c r="E42" s="52">
+      <c r="E42" s="19">
         <v>2028.9167649999999</v>
       </c>
       <c r="F42" s="20"/>
@@ -4507,93 +4714,143 @@
       <c r="B52" s="11">
         <v>1</v>
       </c>
-      <c r="C52" s="12"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="12"/>
-      <c r="F52" s="13"/>
+      <c r="C52" s="50">
+        <v>3103.7282030000001</v>
+      </c>
+      <c r="D52" s="50">
+        <v>10620841.400512001</v>
+      </c>
+      <c r="E52" s="50">
+        <v>3258.96324</v>
+      </c>
+      <c r="F52" s="13">
+        <v>32812</v>
+      </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="14">
         <v>30000</v>
       </c>
-      <c r="B53" s="2">
+      <c r="B53" s="51">
         <v>2</v>
       </c>
-      <c r="C53" s="15"/>
-      <c r="D53" s="15"/>
-      <c r="E53" s="15"/>
+      <c r="C53" s="52">
+        <v>2607.1722559999998</v>
+      </c>
+      <c r="D53" s="52">
+        <v>5816010.3583580004</v>
+      </c>
+      <c r="E53" s="52">
+        <v>2411.6405949999998</v>
+      </c>
       <c r="F53" s="16"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" s="14">
         <v>30000</v>
       </c>
-      <c r="B54" s="2">
+      <c r="B54" s="51">
         <v>3</v>
       </c>
-      <c r="C54" s="15"/>
-      <c r="D54" s="15"/>
-      <c r="E54" s="15"/>
+      <c r="C54" s="52">
+        <v>3736.7359070000002</v>
+      </c>
+      <c r="D54" s="52">
+        <v>3017606.6757379998</v>
+      </c>
+      <c r="E54" s="52">
+        <v>1737.125982</v>
+      </c>
       <c r="F54" s="16"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" s="14">
         <v>30000</v>
       </c>
-      <c r="B55" s="2">
+      <c r="B55" s="51">
         <v>4</v>
       </c>
-      <c r="C55" s="15"/>
-      <c r="D55" s="15"/>
-      <c r="E55" s="15"/>
+      <c r="C55" s="52">
+        <v>3406.9890820000001</v>
+      </c>
+      <c r="D55" s="52">
+        <v>1642623.835681</v>
+      </c>
+      <c r="E55" s="52">
+        <v>1281.648874</v>
+      </c>
       <c r="F55" s="16"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" s="14">
         <v>30000</v>
       </c>
-      <c r="B56" s="2">
+      <c r="B56" s="51">
         <v>5</v>
       </c>
-      <c r="C56" s="15"/>
-      <c r="D56" s="15"/>
-      <c r="E56" s="15"/>
+      <c r="C56" s="52">
+        <v>3258.0686099999998</v>
+      </c>
+      <c r="D56" s="52">
+        <v>1220073.0567960001</v>
+      </c>
+      <c r="E56" s="52">
+        <v>1104.569172</v>
+      </c>
       <c r="F56" s="16"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" s="14">
         <v>30000</v>
       </c>
-      <c r="B57" s="2">
+      <c r="B57" s="51">
         <v>6</v>
       </c>
-      <c r="C57" s="15"/>
-      <c r="D57" s="15"/>
-      <c r="E57" s="15"/>
+      <c r="C57" s="52">
+        <v>4497.4069380000001</v>
+      </c>
+      <c r="D57" s="52">
+        <v>8281288.6309599997</v>
+      </c>
+      <c r="E57" s="52">
+        <v>2877.72282</v>
+      </c>
       <c r="F57" s="16"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" s="14">
         <v>30000</v>
       </c>
-      <c r="B58" s="2">
+      <c r="B58" s="51">
         <v>7</v>
       </c>
-      <c r="C58" s="15"/>
-      <c r="D58" s="15"/>
-      <c r="E58" s="15"/>
+      <c r="C58" s="52">
+        <v>4000.8509909999998</v>
+      </c>
+      <c r="D58" s="52">
+        <v>4113658.854764</v>
+      </c>
+      <c r="E58" s="52">
+        <v>2028.2156829999999</v>
+      </c>
       <c r="F58" s="16"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" s="14">
         <v>30000</v>
       </c>
-      <c r="B59" s="2">
+      <c r="B59" s="51">
         <v>8</v>
       </c>
-      <c r="C59" s="15"/>
-      <c r="D59" s="15"/>
-      <c r="E59" s="15"/>
+      <c r="C59" s="52">
+        <v>5130.4146419999997</v>
+      </c>
+      <c r="D59" s="52">
+        <v>4802158.0496589998</v>
+      </c>
+      <c r="E59" s="52">
+        <v>2191.3826800000002</v>
+      </c>
       <c r="F59" s="16"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.35">
@@ -4603,9 +4860,15 @@
       <c r="B60" s="18">
         <v>9</v>
       </c>
-      <c r="C60" s="19"/>
-      <c r="D60" s="19"/>
-      <c r="E60" s="19"/>
+      <c r="C60" s="53">
+        <v>4800.6678169999996</v>
+      </c>
+      <c r="D60" s="53">
+        <v>4091428.732694</v>
+      </c>
+      <c r="E60" s="53">
+        <v>2022.728042</v>
+      </c>
       <c r="F60" s="20"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.35">
@@ -4615,9 +4878,18 @@
       <c r="B61" s="2">
         <v>1</v>
       </c>
-      <c r="C61" s="7"/>
-      <c r="D61" s="7"/>
-      <c r="E61" s="7"/>
+      <c r="C61" s="7">
+        <v>3090.9859799999999</v>
+      </c>
+      <c r="D61" s="7">
+        <v>10457267.273239</v>
+      </c>
+      <c r="E61" s="7">
+        <v>3233.769824</v>
+      </c>
+      <c r="F61" s="2">
+        <v>24192</v>
+      </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" s="6">
@@ -4626,9 +4898,15 @@
       <c r="B62" s="2">
         <v>2</v>
       </c>
-      <c r="C62" s="7"/>
-      <c r="D62" s="7"/>
-      <c r="E62" s="7"/>
+      <c r="C62" s="7">
+        <v>2601.4466689999999</v>
+      </c>
+      <c r="D62" s="7">
+        <v>5759135.8922290001</v>
+      </c>
+      <c r="E62" s="7">
+        <v>2399.8199709999999</v>
+      </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" s="6">
@@ -4637,9 +4915,15 @@
       <c r="B63" s="2">
         <v>3</v>
       </c>
-      <c r="C63" s="7"/>
-      <c r="D63" s="7"/>
-      <c r="E63" s="7"/>
+      <c r="C63" s="7">
+        <v>3736.054048</v>
+      </c>
+      <c r="D63" s="7">
+        <v>2984768.2116990001</v>
+      </c>
+      <c r="E63" s="7">
+        <v>1727.6481739999999</v>
+      </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" s="6">
@@ -4648,9 +4932,15 @@
       <c r="B64" s="2">
         <v>4</v>
       </c>
-      <c r="C64" s="7"/>
-      <c r="D64" s="7"/>
-      <c r="E64" s="7"/>
+      <c r="C64" s="7">
+        <v>3412.082371</v>
+      </c>
+      <c r="D64" s="7">
+        <v>1646488.9047389999</v>
+      </c>
+      <c r="E64" s="7">
+        <v>1283.1558379999999</v>
+      </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" s="6">
@@ -4659,9 +4949,15 @@
       <c r="B65" s="2">
         <v>5</v>
       </c>
-      <c r="C65" s="7"/>
-      <c r="D65" s="7"/>
-      <c r="E65" s="7"/>
+      <c r="C65" s="7">
+        <v>3258.9306769999998</v>
+      </c>
+      <c r="D65" s="7">
+        <v>1212270.281865</v>
+      </c>
+      <c r="E65" s="7">
+        <v>1101.031463</v>
+      </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" s="6">
@@ -4670,9 +4966,15 @@
       <c r="B66" s="2">
         <v>6</v>
       </c>
-      <c r="C66" s="7"/>
-      <c r="D66" s="7"/>
-      <c r="E66" s="7"/>
+      <c r="C66" s="7">
+        <v>4485.1464939999996</v>
+      </c>
+      <c r="D66" s="7">
+        <v>8162966.5732859997</v>
+      </c>
+      <c r="E66" s="7">
+        <v>2857.0905779999998</v>
+      </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" s="6">
@@ -4681,9 +4983,15 @@
       <c r="B67" s="2">
         <v>7</v>
       </c>
-      <c r="C67" s="7"/>
-      <c r="D67" s="7"/>
-      <c r="E67" s="7"/>
+      <c r="C67" s="7">
+        <v>3995.6071830000001</v>
+      </c>
+      <c r="D67" s="7">
+        <v>4074595.3629069999</v>
+      </c>
+      <c r="E67" s="7">
+        <v>2018.5626970000001</v>
+      </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" s="6">
@@ -4692,9 +5000,15 @@
       <c r="B68" s="2">
         <v>8</v>
       </c>
-      <c r="C68" s="7"/>
-      <c r="D68" s="7"/>
-      <c r="E68" s="7"/>
+      <c r="C68" s="7">
+        <v>5130.2145620000001</v>
+      </c>
+      <c r="D68" s="7">
+        <v>4824927.6400410002</v>
+      </c>
+      <c r="E68" s="7">
+        <v>2196.5717930000001</v>
+      </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" s="6">
@@ -4703,9 +5017,15 @@
       <c r="B69" s="2">
         <v>9</v>
       </c>
-      <c r="C69" s="7"/>
-      <c r="D69" s="7"/>
-      <c r="E69" s="7"/>
+      <c r="C69" s="7">
+        <v>4806.2428849999997</v>
+      </c>
+      <c r="D69" s="7">
+        <v>4117194.2277589999</v>
+      </c>
+      <c r="E69" s="7">
+        <v>2029.087043</v>
+      </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" s="10">
@@ -4714,10 +5034,18 @@
       <c r="B70" s="11">
         <v>1</v>
       </c>
-      <c r="C70" s="12"/>
-      <c r="D70" s="12"/>
-      <c r="E70" s="12"/>
-      <c r="F70" s="13"/>
+      <c r="C70" s="12">
+        <v>3083.3257020000001</v>
+      </c>
+      <c r="D70" s="12">
+        <v>10626573.966976</v>
+      </c>
+      <c r="E70" s="12">
+        <v>3259.8426290000002</v>
+      </c>
+      <c r="F70" s="13">
+        <v>34977</v>
+      </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" s="14">
@@ -4726,9 +5054,15 @@
       <c r="B71" s="2">
         <v>2</v>
       </c>
-      <c r="C71" s="15"/>
-      <c r="D71" s="15"/>
-      <c r="E71" s="15"/>
+      <c r="C71" s="15">
+        <v>2591.1803190000001</v>
+      </c>
+      <c r="D71" s="15">
+        <v>5809453.6606799997</v>
+      </c>
+      <c r="E71" s="15">
+        <v>2410.2808260000002</v>
+      </c>
       <c r="F71" s="16"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.35">
@@ -4738,9 +5072,15 @@
       <c r="B72" s="2">
         <v>3</v>
       </c>
-      <c r="C72" s="15"/>
-      <c r="D72" s="15"/>
-      <c r="E72" s="15"/>
+      <c r="C72" s="15">
+        <v>3731.6563769999998</v>
+      </c>
+      <c r="D72" s="15">
+        <v>3028572.9856690001</v>
+      </c>
+      <c r="E72" s="15">
+        <v>1740.279571</v>
+      </c>
       <c r="F72" s="16"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.35">
@@ -4750,9 +5090,15 @@
       <c r="B73" s="2">
         <v>4</v>
       </c>
-      <c r="C73" s="15"/>
-      <c r="D73" s="15"/>
-      <c r="E73" s="15"/>
+      <c r="C73" s="15">
+        <v>3400.5389540000001</v>
+      </c>
+      <c r="D73" s="15">
+        <v>1641997.0114510001</v>
+      </c>
+      <c r="E73" s="15">
+        <v>1281.4043119999999</v>
+      </c>
       <c r="F73" s="16"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.35">
@@ -4762,9 +5108,15 @@
       <c r="B74" s="2">
         <v>5</v>
       </c>
-      <c r="C74" s="15"/>
-      <c r="D74" s="15"/>
-      <c r="E74" s="15"/>
+      <c r="C74" s="15">
+        <v>3247.700112</v>
+      </c>
+      <c r="D74" s="15">
+        <v>1205950.7866420001</v>
+      </c>
+      <c r="E74" s="15">
+        <v>1098.1579059999999</v>
+      </c>
       <c r="F74" s="16"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.35">
@@ -4774,9 +5126,15 @@
       <c r="B75" s="2">
         <v>6</v>
       </c>
-      <c r="C75" s="15"/>
-      <c r="D75" s="15"/>
-      <c r="E75" s="15"/>
+      <c r="C75" s="15">
+        <v>4475.2731919999997</v>
+      </c>
+      <c r="D75" s="15">
+        <v>8257131.5978629999</v>
+      </c>
+      <c r="E75" s="15">
+        <v>2873.5225070000001</v>
+      </c>
       <c r="F75" s="16"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.35">
@@ -4786,9 +5144,15 @@
       <c r="B76" s="2">
         <v>7</v>
       </c>
-      <c r="C76" s="15"/>
-      <c r="D76" s="15"/>
-      <c r="E76" s="15"/>
+      <c r="C76" s="15">
+        <v>3983.1278090000001</v>
+      </c>
+      <c r="D76" s="15">
+        <v>4084377.5577540002</v>
+      </c>
+      <c r="E76" s="15">
+        <v>2020.9843040000001</v>
+      </c>
       <c r="F76" s="16"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.35">
@@ -4798,9 +5162,15 @@
       <c r="B77" s="2">
         <v>8</v>
       </c>
-      <c r="C77" s="15"/>
-      <c r="D77" s="15"/>
-      <c r="E77" s="15"/>
+      <c r="C77" s="15">
+        <v>5123.6038669999998</v>
+      </c>
+      <c r="D77" s="15">
+        <v>4845782.6507639997</v>
+      </c>
+      <c r="E77" s="15">
+        <v>2201.313846</v>
+      </c>
       <c r="F77" s="16"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.35">
@@ -4810,9 +5180,15 @@
       <c r="B78" s="18">
         <v>9</v>
       </c>
-      <c r="C78" s="19"/>
-      <c r="D78" s="19"/>
-      <c r="E78" s="19"/>
+      <c r="C78" s="19">
+        <v>4792.4864440000001</v>
+      </c>
+      <c r="D78" s="19">
+        <v>4129195.3382049999</v>
+      </c>
+      <c r="E78" s="19">
+        <v>2032.04216</v>
+      </c>
       <c r="F78" s="20"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.35">
@@ -4822,9 +5198,18 @@
       <c r="B79" s="2">
         <v>1</v>
       </c>
-      <c r="C79" s="15"/>
-      <c r="D79" s="15"/>
-      <c r="E79" s="15"/>
+      <c r="C79" s="15">
+        <v>3046.359841</v>
+      </c>
+      <c r="D79" s="15">
+        <v>10478797.971595</v>
+      </c>
+      <c r="E79" s="15">
+        <v>3237.0971519999998</v>
+      </c>
+      <c r="F79" s="2">
+        <v>42096</v>
+      </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" s="14">
@@ -4833,9 +5218,15 @@
       <c r="B80" s="2">
         <v>2</v>
       </c>
-      <c r="C80" s="15"/>
-      <c r="D80" s="15"/>
-      <c r="E80" s="15"/>
+      <c r="C80" s="15">
+        <v>2564.0246090000001</v>
+      </c>
+      <c r="D80" s="15">
+        <v>5769902.6218290003</v>
+      </c>
+      <c r="E80" s="15">
+        <v>2402.0621599999999</v>
+      </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" s="14">
@@ -4844,9 +5235,15 @@
       <c r="B81" s="2">
         <v>3</v>
       </c>
-      <c r="C81" s="15"/>
-      <c r="D81" s="15"/>
-      <c r="E81" s="15"/>
+      <c r="C81" s="15">
+        <v>3708.9790680000001</v>
+      </c>
+      <c r="D81" s="15">
+        <v>2991593.1003060001</v>
+      </c>
+      <c r="E81" s="15">
+        <v>1729.6222419999999</v>
+      </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82" s="14">
@@ -4855,9 +5252,15 @@
       <c r="B82" s="2">
         <v>4</v>
       </c>
-      <c r="C82" s="15"/>
-      <c r="D82" s="15"/>
-      <c r="E82" s="15"/>
+      <c r="C82" s="15">
+        <v>3388.9423670000001</v>
+      </c>
+      <c r="D82" s="15">
+        <v>1643303.005936</v>
+      </c>
+      <c r="E82" s="15">
+        <v>1281.913806</v>
+      </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" s="14">
@@ -4866,9 +5269,15 @@
       <c r="B83" s="2">
         <v>5</v>
       </c>
-      <c r="C83" s="15"/>
-      <c r="D83" s="15"/>
-      <c r="E83" s="15"/>
+      <c r="C83" s="15">
+        <v>3239.0509320000001</v>
+      </c>
+      <c r="D83" s="15">
+        <v>1218371.2541809999</v>
+      </c>
+      <c r="E83" s="15">
+        <v>1103.7985570000001</v>
+      </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" s="14">
@@ -4877,9 +5286,15 @@
       <c r="B84" s="2">
         <v>6</v>
       </c>
-      <c r="C84" s="15"/>
-      <c r="D84" s="15"/>
-      <c r="E84" s="15"/>
+      <c r="C84" s="15">
+        <v>4446.534627</v>
+      </c>
+      <c r="D84" s="15">
+        <v>8157393.4044300001</v>
+      </c>
+      <c r="E84" s="15">
+        <v>2856.1150889999999</v>
+      </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85" s="14">
@@ -4888,9 +5303,15 @@
       <c r="B85" s="2">
         <v>7</v>
       </c>
-      <c r="C85" s="15"/>
-      <c r="D85" s="15"/>
-      <c r="E85" s="15"/>
+      <c r="C85" s="15">
+        <v>3964.1993950000001</v>
+      </c>
+      <c r="D85" s="15">
+        <v>4072777.0074160001</v>
+      </c>
+      <c r="E85" s="15">
+        <v>2018.112239</v>
+      </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" s="14">
@@ -4899,9 +5320,15 @@
       <c r="B86" s="2">
         <v>8</v>
       </c>
-      <c r="C86" s="15"/>
-      <c r="D86" s="15"/>
-      <c r="E86" s="15"/>
+      <c r="C86" s="15">
+        <v>5109.1538540000001</v>
+      </c>
+      <c r="D86" s="15">
+        <v>4792111.9155379999</v>
+      </c>
+      <c r="E86" s="15">
+        <v>2189.089289</v>
+      </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" s="14">
@@ -4910,9 +5337,15 @@
       <c r="B87" s="2">
         <v>9</v>
       </c>
-      <c r="C87" s="15"/>
-      <c r="D87" s="15"/>
-      <c r="E87" s="15"/>
+      <c r="C87" s="15">
+        <v>4789.1171530000001</v>
+      </c>
+      <c r="D87" s="15">
+        <v>4090948.5671259998</v>
+      </c>
+      <c r="E87" s="15">
+        <v>2022.609346</v>
+      </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" s="10">
@@ -4921,10 +5354,18 @@
       <c r="B88" s="11">
         <v>1</v>
       </c>
-      <c r="C88" s="12"/>
-      <c r="D88" s="12"/>
-      <c r="E88" s="12"/>
-      <c r="F88" s="13"/>
+      <c r="C88" s="12">
+        <v>3082.3130780000001</v>
+      </c>
+      <c r="D88" s="12">
+        <v>10595575.62748</v>
+      </c>
+      <c r="E88" s="12">
+        <v>3255.0845810000001</v>
+      </c>
+      <c r="F88" s="13">
+        <v>43831</v>
+      </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89" s="14">
@@ -4933,9 +5374,15 @@
       <c r="B89" s="2">
         <v>2</v>
       </c>
-      <c r="C89" s="15"/>
-      <c r="D89" s="15"/>
-      <c r="E89" s="15"/>
+      <c r="C89" s="15">
+        <v>2590.526754</v>
+      </c>
+      <c r="D89" s="15">
+        <v>5802484.6445840001</v>
+      </c>
+      <c r="E89" s="15">
+        <v>2408.834707</v>
+      </c>
       <c r="F89" s="16"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.35">
@@ -4945,9 +5392,15 @@
       <c r="B90" s="2">
         <v>3</v>
       </c>
-      <c r="C90" s="15"/>
-      <c r="D90" s="15"/>
-      <c r="E90" s="15"/>
+      <c r="C90" s="15">
+        <v>3717.6914339999998</v>
+      </c>
+      <c r="D90" s="15">
+        <v>3011654.3723909999</v>
+      </c>
+      <c r="E90" s="15">
+        <v>1735.4118739999999</v>
+      </c>
       <c r="F90" s="16"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.35">
@@ -4957,9 +5410,15 @@
       <c r="B91" s="2">
         <v>4</v>
       </c>
-      <c r="C91" s="15"/>
-      <c r="D91" s="15"/>
-      <c r="E91" s="15"/>
+      <c r="C91" s="15">
+        <v>3388.0634460000001</v>
+      </c>
+      <c r="D91" s="15">
+        <v>1626268.531652</v>
+      </c>
+      <c r="E91" s="15">
+        <v>1275.25234</v>
+      </c>
       <c r="F91" s="16"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.35">
@@ -4969,9 +5428,15 @@
       <c r="B92" s="2">
         <v>5</v>
       </c>
-      <c r="C92" s="15"/>
-      <c r="D92" s="15"/>
-      <c r="E92" s="15"/>
+      <c r="C92" s="15">
+        <v>3242.2635030000001</v>
+      </c>
+      <c r="D92" s="15">
+        <v>1214857.4796750001</v>
+      </c>
+      <c r="E92" s="15">
+        <v>1102.2057339999999</v>
+      </c>
       <c r="F92" s="16"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.35">
@@ -4981,9 +5446,15 @@
       <c r="B93" s="2">
         <v>6</v>
       </c>
-      <c r="C93" s="15"/>
-      <c r="D93" s="15"/>
-      <c r="E93" s="15"/>
+      <c r="C93" s="15">
+        <v>4469.741207</v>
+      </c>
+      <c r="D93" s="15">
+        <v>8265414.6750229998</v>
+      </c>
+      <c r="E93" s="15">
+        <v>2874.9634219999998</v>
+      </c>
       <c r="F93" s="16"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.35">
@@ -4993,9 +5464,15 @@
       <c r="B94" s="2">
         <v>7</v>
       </c>
-      <c r="C94" s="15"/>
-      <c r="D94" s="15"/>
-      <c r="E94" s="15"/>
+      <c r="C94" s="15">
+        <v>3977.9548840000002</v>
+      </c>
+      <c r="D94" s="15">
+        <v>4102939.2310500001</v>
+      </c>
+      <c r="E94" s="15">
+        <v>2025.571334</v>
+      </c>
       <c r="F94" s="16"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.35">
@@ -5005,9 +5482,15 @@
       <c r="B95" s="2">
         <v>8</v>
       </c>
-      <c r="C95" s="15"/>
-      <c r="D95" s="15"/>
-      <c r="E95" s="15"/>
+      <c r="C95" s="15">
+        <v>5105.1195630000002</v>
+      </c>
+      <c r="D95" s="15">
+        <v>4764317.4283020003</v>
+      </c>
+      <c r="E95" s="15">
+        <v>2182.731644</v>
+      </c>
       <c r="F95" s="16"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.35">
@@ -5017,9 +5500,15 @@
       <c r="B96" s="18">
         <v>9</v>
       </c>
-      <c r="C96" s="19"/>
-      <c r="D96" s="19"/>
-      <c r="E96" s="19"/>
+      <c r="C96" s="19">
+        <v>4775.4915760000004</v>
+      </c>
+      <c r="D96" s="19">
+        <v>4035590.0084910002</v>
+      </c>
+      <c r="E96" s="19">
+        <v>2008.877798</v>
+      </c>
       <c r="F96" s="20"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.35">
@@ -5029,9 +5518,18 @@
       <c r="B97" s="2">
         <v>1</v>
       </c>
-      <c r="C97" s="15"/>
-      <c r="D97" s="15"/>
-      <c r="E97" s="15"/>
+      <c r="C97" s="15">
+        <v>3105.1673000000001</v>
+      </c>
+      <c r="D97" s="15">
+        <v>10697986.741622999</v>
+      </c>
+      <c r="E97" s="15">
+        <v>3270.777697</v>
+      </c>
+      <c r="F97" s="2">
+        <v>153110</v>
+      </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98" s="22">
@@ -5040,9 +5538,15 @@
       <c r="B98" s="2">
         <v>2</v>
       </c>
-      <c r="C98" s="15"/>
-      <c r="D98" s="15"/>
-      <c r="E98" s="15"/>
+      <c r="C98" s="15">
+        <v>2606.2532510000001</v>
+      </c>
+      <c r="D98" s="15">
+        <v>5847282.1960380003</v>
+      </c>
+      <c r="E98" s="15">
+        <v>2418.1154219999999</v>
+      </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99" s="22">
@@ -5051,9 +5555,15 @@
       <c r="B99" s="2">
         <v>3</v>
       </c>
-      <c r="C99" s="15"/>
-      <c r="D99" s="15"/>
-      <c r="E99" s="15"/>
+      <c r="C99" s="15">
+        <v>3743.1811870000001</v>
+      </c>
+      <c r="D99" s="15">
+        <v>3034664.3906140001</v>
+      </c>
+      <c r="E99" s="15">
+        <v>1742.0288149999999</v>
+      </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" s="22">
@@ -5062,9 +5572,15 @@
       <c r="B100" s="2">
         <v>4</v>
       </c>
-      <c r="C100" s="15"/>
-      <c r="D100" s="15"/>
-      <c r="E100" s="15"/>
+      <c r="C100" s="15">
+        <v>3409.0851870000001</v>
+      </c>
+      <c r="D100" s="15">
+        <v>1643264.8327830001</v>
+      </c>
+      <c r="E100" s="15">
+        <v>1281.898917</v>
+      </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" s="22">
@@ -5073,9 +5589,15 @@
       <c r="B101" s="2">
         <v>5</v>
       </c>
-      <c r="C101" s="15"/>
-      <c r="D101" s="15"/>
-      <c r="E101" s="15"/>
+      <c r="C101" s="15">
+        <v>3257.7562680000001</v>
+      </c>
+      <c r="D101" s="15">
+        <v>1215135.2022299999</v>
+      </c>
+      <c r="E101" s="15">
+        <v>1102.3317119999999</v>
+      </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" s="22">
@@ -5084,9 +5606,15 @@
       <c r="B102" s="2">
         <v>6</v>
       </c>
-      <c r="C102" s="15"/>
-      <c r="D102" s="15"/>
-      <c r="E102" s="15"/>
+      <c r="C102" s="15">
+        <v>4501.862102</v>
+      </c>
+      <c r="D102" s="15">
+        <v>8312645.7247679997</v>
+      </c>
+      <c r="E102" s="15">
+        <v>2883.1659199999999</v>
+      </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103" s="22">
@@ -5095,9 +5623,15 @@
       <c r="B103" s="2">
         <v>7</v>
       </c>
-      <c r="C103" s="15"/>
-      <c r="D103" s="15"/>
-      <c r="E103" s="15"/>
+      <c r="C103" s="15">
+        <v>4002.9480530000001</v>
+      </c>
+      <c r="D103" s="15">
+        <v>4114279.6333460002</v>
+      </c>
+      <c r="E103" s="15">
+        <v>2028.368712</v>
+      </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104" s="22">
@@ -5106,9 +5640,15 @@
       <c r="B104" s="2">
         <v>8</v>
       </c>
-      <c r="C104" s="15"/>
-      <c r="D104" s="15"/>
-      <c r="E104" s="15"/>
+      <c r="C104" s="15">
+        <v>5139.8759890000001</v>
+      </c>
+      <c r="D104" s="15">
+        <v>4815324.9423289998</v>
+      </c>
+      <c r="E104" s="15">
+        <v>2194.3848670000002</v>
+      </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" s="22">
@@ -5117,9 +5657,15 @@
       <c r="B105" s="2">
         <v>9</v>
       </c>
-      <c r="C105" s="15"/>
-      <c r="D105" s="15"/>
-      <c r="E105" s="15"/>
+      <c r="C105" s="15">
+        <v>4805.7799889999997</v>
+      </c>
+      <c r="D105" s="15">
+        <v>4101225.5665850001</v>
+      </c>
+      <c r="E105" s="15">
+        <v>2025.148283</v>
+      </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" s="10">
@@ -5128,10 +5674,18 @@
       <c r="B106" s="11">
         <v>1</v>
       </c>
-      <c r="C106" s="12"/>
-      <c r="D106" s="12"/>
-      <c r="E106" s="12"/>
-      <c r="F106" s="13"/>
+      <c r="C106" s="12">
+        <v>3054.344998</v>
+      </c>
+      <c r="D106" s="12">
+        <v>10504632.617658</v>
+      </c>
+      <c r="E106" s="12">
+        <v>3241.0850989999999</v>
+      </c>
+      <c r="F106" s="13">
+        <v>74655</v>
+      </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107" s="14">
@@ -5140,9 +5694,15 @@
       <c r="B107" s="2">
         <v>2</v>
       </c>
-      <c r="C107" s="15"/>
-      <c r="D107" s="15"/>
-      <c r="E107" s="15"/>
+      <c r="C107" s="15">
+        <v>2569.4005459999998</v>
+      </c>
+      <c r="D107" s="15">
+        <v>5783868.5075089997</v>
+      </c>
+      <c r="E107" s="15">
+        <v>2404.9674650000002</v>
+      </c>
       <c r="F107" s="16"/>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.35">
@@ -5152,9 +5712,15 @@
       <c r="B108" s="2">
         <v>3</v>
       </c>
-      <c r="C108" s="15"/>
-      <c r="D108" s="15"/>
-      <c r="E108" s="15"/>
+      <c r="C108" s="15">
+        <v>3724.9947729999999</v>
+      </c>
+      <c r="D108" s="15">
+        <v>3020278.8119180002</v>
+      </c>
+      <c r="E108" s="15">
+        <v>1737.894937</v>
+      </c>
       <c r="F108" s="16"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.35">
@@ -5164,9 +5730,15 @@
       <c r="B109" s="2">
         <v>4</v>
       </c>
-      <c r="C109" s="15"/>
-      <c r="D109" s="15"/>
-      <c r="E109" s="15"/>
+      <c r="C109" s="15">
+        <v>3403.272328</v>
+      </c>
+      <c r="D109" s="15">
+        <v>1676836.539932</v>
+      </c>
+      <c r="E109" s="15">
+        <v>1294.9272329999999</v>
+      </c>
       <c r="F109" s="16"/>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.35">
@@ -5176,9 +5748,15 @@
       <c r="B110" s="2">
         <v>5</v>
       </c>
-      <c r="C110" s="15"/>
-      <c r="D110" s="15"/>
-      <c r="E110" s="15"/>
+      <c r="C110" s="15">
+        <v>3246.8593780000001</v>
+      </c>
+      <c r="D110" s="15">
+        <v>1218043.375334</v>
+      </c>
+      <c r="E110" s="15">
+        <v>1103.650024</v>
+      </c>
       <c r="F110" s="16"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.35">
@@ -5188,9 +5766,15 @@
       <c r="B111" s="2">
         <v>6</v>
       </c>
-      <c r="C111" s="15"/>
-      <c r="D111" s="15"/>
-      <c r="E111" s="15"/>
+      <c r="C111" s="15">
+        <v>4460.0660289999996</v>
+      </c>
+      <c r="D111" s="15">
+        <v>8165874.1362770004</v>
+      </c>
+      <c r="E111" s="15">
+        <v>2857.5993659999999</v>
+      </c>
       <c r="F111" s="16"/>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.35">
@@ -5200,9 +5784,15 @@
       <c r="B112" s="2">
         <v>7</v>
       </c>
-      <c r="C112" s="15"/>
-      <c r="D112" s="15"/>
-      <c r="E112" s="15"/>
+      <c r="C112" s="15">
+        <v>3975.1215769999999</v>
+      </c>
+      <c r="D112" s="15">
+        <v>4074365.8344459999</v>
+      </c>
+      <c r="E112" s="15">
+        <v>2018.505842</v>
+      </c>
       <c r="F112" s="16"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.35">
@@ -5212,9 +5802,15 @@
       <c r="B113" s="2">
         <v>8</v>
       </c>
-      <c r="C113" s="15"/>
-      <c r="D113" s="15"/>
-      <c r="E113" s="15"/>
+      <c r="C113" s="15">
+        <v>5130.7158040000004</v>
+      </c>
+      <c r="D113" s="15">
+        <v>4876942.811853</v>
+      </c>
+      <c r="E113" s="15">
+        <v>2208.3801330000001</v>
+      </c>
       <c r="F113" s="16"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.35">
@@ -5224,9 +5820,15 @@
       <c r="B114" s="18">
         <v>9</v>
       </c>
-      <c r="C114" s="19"/>
-      <c r="D114" s="19"/>
-      <c r="E114" s="19"/>
+      <c r="C114" s="19">
+        <v>4808.9933590000001</v>
+      </c>
+      <c r="D114" s="19">
+        <v>4183230.9235200002</v>
+      </c>
+      <c r="E114" s="19">
+        <v>2045.2948260000001</v>
+      </c>
       <c r="F114" s="20"/>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.35">
@@ -5236,9 +5838,18 @@
       <c r="B115" s="2">
         <v>1</v>
       </c>
-      <c r="C115" s="15"/>
-      <c r="D115" s="15"/>
-      <c r="E115" s="15"/>
+      <c r="C115" s="15">
+        <v>3092.271131</v>
+      </c>
+      <c r="D115" s="15">
+        <v>10583677.071209</v>
+      </c>
+      <c r="E115" s="15">
+        <v>3253.2563799999998</v>
+      </c>
+      <c r="F115" s="2">
+        <v>124032</v>
+      </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A116" s="22">
@@ -5247,9 +5858,15 @@
       <c r="B116" s="2">
         <v>2</v>
       </c>
-      <c r="C116" s="15"/>
-      <c r="D116" s="15"/>
-      <c r="E116" s="15"/>
+      <c r="C116" s="15">
+        <v>2600.4205299999999</v>
+      </c>
+      <c r="D116" s="15">
+        <v>5802700.5626919996</v>
+      </c>
+      <c r="E116" s="15">
+        <v>2408.8795239999999</v>
+      </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A117" s="22">
@@ -5258,9 +5875,15 @@
       <c r="B117" s="2">
         <v>3</v>
       </c>
-      <c r="C117" s="15"/>
-      <c r="D117" s="15"/>
-      <c r="E117" s="15"/>
+      <c r="C117" s="15">
+        <v>3738.079424</v>
+      </c>
+      <c r="D117" s="15">
+        <v>3019915.7583770002</v>
+      </c>
+      <c r="E117" s="15">
+        <v>1737.7904820000001</v>
+      </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A118" s="22">
@@ -5269,9 +5892,15 @@
       <c r="B118" s="2">
         <v>4</v>
       </c>
-      <c r="C118" s="15"/>
-      <c r="D118" s="15"/>
-      <c r="E118" s="15"/>
+      <c r="C118" s="15">
+        <v>3410.1671540000002</v>
+      </c>
+      <c r="D118" s="15">
+        <v>1652507.8783160001</v>
+      </c>
+      <c r="E118" s="15">
+        <v>1285.4990780000001</v>
+      </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A119" s="22">
@@ -5280,9 +5909,15 @@
       <c r="B119" s="2">
         <v>5</v>
       </c>
-      <c r="C119" s="15"/>
-      <c r="D119" s="15"/>
-      <c r="E119" s="15"/>
+      <c r="C119" s="15">
+        <v>3257.0874800000001</v>
+      </c>
+      <c r="D119" s="15">
+        <v>1212376.3847320001</v>
+      </c>
+      <c r="E119" s="15">
+        <v>1101.079645</v>
+      </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A120" s="22">
@@ -5291,9 +5926,15 @@
       <c r="B120" s="2">
         <v>6</v>
       </c>
-      <c r="C120" s="15"/>
-      <c r="D120" s="15"/>
-      <c r="E120" s="15"/>
+      <c r="C120" s="15">
+        <v>4487.9199710000003</v>
+      </c>
+      <c r="D120" s="15">
+        <v>8224392.69386</v>
+      </c>
+      <c r="E120" s="15">
+        <v>2867.8201989999998</v>
+      </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A121" s="22">
@@ -5302,9 +5943,15 @@
       <c r="B121" s="2">
         <v>7</v>
       </c>
-      <c r="C121" s="15"/>
-      <c r="D121" s="15"/>
-      <c r="E121" s="15"/>
+      <c r="C121" s="15">
+        <v>3996.0693700000002</v>
+      </c>
+      <c r="D121" s="15">
+        <v>4083153.94955</v>
+      </c>
+      <c r="E121" s="15">
+        <v>2020.681556</v>
+      </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A122" s="22">
@@ -5313,9 +5960,15 @@
       <c r="B122" s="2">
         <v>8</v>
       </c>
-      <c r="C122" s="15"/>
-      <c r="D122" s="15"/>
-      <c r="E122" s="15"/>
+      <c r="C122" s="15">
+        <v>5133.7282640000003</v>
+      </c>
+      <c r="D122" s="15">
+        <v>4829203.6401180001</v>
+      </c>
+      <c r="E122" s="15">
+        <v>2197.5449119999998</v>
+      </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A123" s="22">
@@ -5324,9 +5977,15 @@
       <c r="B123" s="2">
         <v>9</v>
       </c>
-      <c r="C123" s="15"/>
-      <c r="D123" s="15"/>
-      <c r="E123" s="15"/>
+      <c r="C123" s="15">
+        <v>4805.8159939999996</v>
+      </c>
+      <c r="D123" s="15">
+        <v>4126760.6843429999</v>
+      </c>
+      <c r="E123" s="15">
+        <v>2031.4430050000001</v>
+      </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A124" s="10">
@@ -5335,10 +5994,18 @@
       <c r="B124" s="11">
         <v>1</v>
       </c>
-      <c r="C124" s="12"/>
-      <c r="D124" s="12"/>
-      <c r="E124" s="12"/>
-      <c r="F124" s="13"/>
+      <c r="C124" s="12">
+        <v>3097.1440349999998</v>
+      </c>
+      <c r="D124" s="12">
+        <v>10668748.183801999</v>
+      </c>
+      <c r="E124" s="12">
+        <v>3266.3049740000001</v>
+      </c>
+      <c r="F124" s="13">
+        <v>137495</v>
+      </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A125" s="14">
@@ -5347,9 +6014,15 @@
       <c r="B125" s="2">
         <v>2</v>
       </c>
-      <c r="C125" s="15"/>
-      <c r="D125" s="15"/>
-      <c r="E125" s="15"/>
+      <c r="C125" s="15">
+        <v>2599.9271319999998</v>
+      </c>
+      <c r="D125" s="15">
+        <v>5841291.7183889998</v>
+      </c>
+      <c r="E125" s="15">
+        <v>2416.8764379999998</v>
+      </c>
       <c r="F125" s="16"/>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.35">
@@ -5359,9 +6032,15 @@
       <c r="B126" s="2">
         <v>3</v>
       </c>
-      <c r="C126" s="15"/>
-      <c r="D126" s="15"/>
-      <c r="E126" s="15"/>
+      <c r="C126" s="15">
+        <v>3738.2225899999999</v>
+      </c>
+      <c r="D126" s="15">
+        <v>3033850.8820759999</v>
+      </c>
+      <c r="E126" s="15">
+        <v>1741.795304</v>
+      </c>
       <c r="F126" s="16"/>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.35">
@@ -5371,9 +6050,15 @@
       <c r="B127" s="2">
         <v>4</v>
       </c>
-      <c r="C127" s="15"/>
-      <c r="D127" s="15"/>
-      <c r="E127" s="15"/>
+      <c r="C127" s="15">
+        <v>3406.06774</v>
+      </c>
+      <c r="D127" s="15">
+        <v>1650468.8906400001</v>
+      </c>
+      <c r="E127" s="15">
+        <v>1284.7057600000001</v>
+      </c>
       <c r="F127" s="16"/>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.35">
@@ -5383,9 +6068,15 @@
       <c r="B128" s="2">
         <v>5</v>
       </c>
-      <c r="C128" s="15"/>
-      <c r="D128" s="15"/>
-      <c r="E128" s="15"/>
+      <c r="C128" s="15">
+        <v>3254.994005</v>
+      </c>
+      <c r="D128" s="15">
+        <v>1217659.3743970001</v>
+      </c>
+      <c r="E128" s="15">
+        <v>1103.476042</v>
+      </c>
       <c r="F128" s="16"/>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.35">
@@ -5395,9 +6086,15 @@
       <c r="B129" s="2">
         <v>6</v>
       </c>
-      <c r="C129" s="15"/>
-      <c r="D129" s="15"/>
-      <c r="E129" s="15"/>
+      <c r="C129" s="15">
+        <v>4494.7674230000002</v>
+      </c>
+      <c r="D129" s="15">
+        <v>8297778.7228739997</v>
+      </c>
+      <c r="E129" s="15">
+        <v>2880.5865239999998</v>
+      </c>
       <c r="F129" s="16"/>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.35">
@@ -5407,9 +6104,15 @@
       <c r="B130" s="2">
         <v>7</v>
       </c>
-      <c r="C130" s="15"/>
-      <c r="D130" s="15"/>
-      <c r="E130" s="15"/>
+      <c r="C130" s="15">
+        <v>3997.5505199999998</v>
+      </c>
+      <c r="D130" s="15">
+        <v>4115018.6822040002</v>
+      </c>
+      <c r="E130" s="15">
+        <v>2028.550882</v>
+      </c>
       <c r="F130" s="16"/>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.35">
@@ -5419,9 +6122,15 @@
       <c r="B131" s="2">
         <v>8</v>
       </c>
-      <c r="C131" s="15"/>
-      <c r="D131" s="15"/>
-      <c r="E131" s="15"/>
+      <c r="C131" s="15">
+        <v>5135.8459780000003</v>
+      </c>
+      <c r="D131" s="15">
+        <v>4815904.3955229996</v>
+      </c>
+      <c r="E131" s="15">
+        <v>2194.516893</v>
+      </c>
       <c r="F131" s="16"/>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.35">
@@ -5431,9 +6140,15 @@
       <c r="B132" s="18">
         <v>9</v>
       </c>
-      <c r="C132" s="19"/>
-      <c r="D132" s="19"/>
-      <c r="E132" s="19"/>
+      <c r="C132" s="19">
+        <v>4803.6911270000001</v>
+      </c>
+      <c r="D132" s="19">
+        <v>4101339.0332399998</v>
+      </c>
+      <c r="E132" s="19">
+        <v>2025.176297</v>
+      </c>
       <c r="F132" s="20"/>
     </row>
   </sheetData>
@@ -5442,7 +6157,7 @@
     <mergeCell ref="A14:F14"/>
   </mergeCells>
   <conditionalFormatting sqref="J3:J15">
-    <cfRule type="colorScale" priority="8">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5452,7 +6167,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K15">
-    <cfRule type="colorScale" priority="11">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5462,7 +6177,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:L15">
-    <cfRule type="colorScale" priority="14">
+    <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5472,7 +6187,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3:M15">
-    <cfRule type="colorScale" priority="17">
+    <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5482,7 +6197,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3:N15">
-    <cfRule type="colorScale" priority="20">
+    <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5492,12 +6207,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:O15">
-    <cfRule type="colorScale" priority="23">
+    <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
         <color theme="9" tint="0.59999389629810485"/>
         <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L19:L31">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Average is included into Summary table
</commit_message>
<xml_diff>
--- a/simulation_check.xlsx
+++ b/simulation_check.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\C-Final-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\GitHub\C++_Final_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04163811-6D05-4529-913E-A4912C4EF384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D024701F-D640-4EF2-8D1B-1C7140E51E5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{603FAE4F-A0F0-414C-B275-6F2A5451B931}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{603FAE4F-A0F0-414C-B275-6F2A5451B931}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="37">
   <si>
     <t>simulation #</t>
   </si>
@@ -147,91 +147,10 @@
     <t>Run_time</t>
   </si>
   <si>
-    <t>SUMMARY OUTPUT</t>
+    <t>Number of Simulations</t>
   </si>
   <si>
-    <t>Regression Statistics</t>
-  </si>
-  <si>
-    <t>Multiple R</t>
-  </si>
-  <si>
-    <t>R Square</t>
-  </si>
-  <si>
-    <t>Adjusted R Square</t>
-  </si>
-  <si>
-    <t>Standard Error</t>
-  </si>
-  <si>
-    <t>Observations</t>
-  </si>
-  <si>
-    <t>ANOVA</t>
-  </si>
-  <si>
-    <t>Regression</t>
-  </si>
-  <si>
-    <t>Residual</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Intercept</t>
-  </si>
-  <si>
-    <t>df</t>
-  </si>
-  <si>
-    <t>SS</t>
-  </si>
-  <si>
-    <t>MS</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>Significance F</t>
-  </si>
-  <si>
-    <t>Coefficients</t>
-  </si>
-  <si>
-    <t>t Stat</t>
-  </si>
-  <si>
-    <t>P-value</t>
-  </si>
-  <si>
-    <t>Lower 95%</t>
-  </si>
-  <si>
-    <t>Upper 95%</t>
-  </si>
-  <si>
-    <t>Lower 95.0%</t>
-  </si>
-  <si>
-    <t>Upper 95.0%</t>
-  </si>
-  <si>
-    <t>Simulations and MAE_var</t>
-  </si>
-  <si>
-    <t>Simulations and MSE_var</t>
-  </si>
-  <si>
-    <t>Based on p-value "simulation #"  variable is not statistically significant in predicting the dependent variable (MAE).</t>
-  </si>
-  <si>
-    <t>Simulations and RMSE_var</t>
-  </si>
-  <si>
-    <t>Simulations and variance</t>
+    <t xml:space="preserve">Average of Results </t>
   </si>
 </sst>
 </file>
@@ -239,11 +158,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,22 +193,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -333,7 +236,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -553,25 +456,14 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -581,69 +473,69 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
@@ -651,7 +543,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
@@ -659,11 +551,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
@@ -671,18 +563,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -695,23 +587,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1027,10 +903,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95A1AEA0-ADDF-4578-9565-5DEA63143E1E}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1041,14 +917,22 @@
     <col min="6" max="6" width="14.6328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.6328125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B1" s="24" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B2" s="26" t="str">
         <f>simulations_small!J2</f>
         <v>MAE_mean</v>
@@ -1073,8 +957,15 @@
         <f>simulations_small!O2</f>
         <v>RMSE_var</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J2" s="6">
+        <v>10000</v>
+      </c>
+      <c r="K2">
+        <f>AVERAGE(SUM(simulations_small!J3:O3),SUM(simulations_medium!J3:O3),SUM(simulations_large!J3:O3))</f>
+        <v>5212062565.6701403</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B3" s="27">
         <f>MIN(simulations_small!$J$3:$J$15)</f>
         <v>1.3737617500001136</v>
@@ -1099,8 +990,19 @@
         <f>MIN(simulations_small!$O$3:$O$15)</f>
         <v>2887.7800032286405</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J3" s="6">
+        <v>15000</v>
+      </c>
+      <c r="K3">
+        <f>AVERAGE(SUM(simulations_small!J4:O4),SUM(simulations_medium!J4:O4),SUM(simulations_large!J4:O4))</f>
+        <v>4645014919.1168776</v>
+      </c>
+      <c r="N3" s="53">
+        <f>MIN(K2:K14)</f>
+        <v>595670805.00217485</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -1128,13 +1030,45 @@
         <f>VLOOKUP(G3,simulations_small!$O$3:$P$15,2,FALSE)</f>
         <v>30000</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J4" s="8">
+        <v>20000</v>
+      </c>
+      <c r="K4">
+        <f>AVERAGE(SUM(simulations_small!J5:O5),SUM(simulations_medium!J5:O5),SUM(simulations_large!J5:O5))</f>
+        <v>2112046735.8288171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J5" s="6">
+        <v>25000</v>
+      </c>
+      <c r="K5">
+        <f>AVERAGE(SUM(simulations_small!J6:O6),SUM(simulations_medium!J6:O6),SUM(simulations_large!J6:O6))</f>
+        <v>838532812.54558706</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J6" s="8">
+        <v>30000</v>
+      </c>
+      <c r="K6">
+        <f>AVERAGE(SUM(simulations_small!J7:O7),SUM(simulations_medium!J7:O7),SUM(simulations_large!J7:O7))</f>
+        <v>1874579049.9885066</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B7" s="24" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J7" s="6">
+        <v>35000</v>
+      </c>
+      <c r="K7">
+        <f>AVERAGE(SUM(simulations_small!J8:O8),SUM(simulations_medium!J8:O8),SUM(simulations_large!J8:O8))</f>
+        <v>2955241424.4473481</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B8" s="28" t="str">
         <f>B2</f>
         <v>MAE_mean</v>
@@ -1159,8 +1093,15 @@
         <f t="shared" si="0"/>
         <v>RMSE_var</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J8" s="6">
+        <v>40000</v>
+      </c>
+      <c r="K8">
+        <f>AVERAGE(SUM(simulations_small!J9:O9),SUM(simulations_medium!J9:O9),SUM(simulations_large!J9:O9))</f>
+        <v>5700964115.570241</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B9" s="27">
         <f>MIN(simulations_medium!$J$3:$J$15)</f>
         <v>3.3914888888889942</v>
@@ -1185,8 +1126,15 @@
         <f>MIN(simulations_medium!$O$3:$O$15)</f>
         <v>9301.4202506045986</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J9" s="6">
+        <v>45000</v>
+      </c>
+      <c r="K9">
+        <f>AVERAGE(SUM(simulations_small!J10:O10),SUM(simulations_medium!J10:O10),SUM(simulations_large!J10:O10))</f>
+        <v>1585962507.4009333</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -1214,13 +1162,45 @@
         <f>VLOOKUP(G9,simulations_medium!$O$3:$P$18,2,FALSE)</f>
         <v>65000</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J10" s="9">
+        <v>50000</v>
+      </c>
+      <c r="K10" s="53">
+        <f>AVERAGE(SUM(simulations_small!J11:O11),SUM(simulations_medium!J11:O11),SUM(simulations_large!J11:O11))</f>
+        <v>595670805.00217485</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J11" s="8">
+        <v>55000</v>
+      </c>
+      <c r="K11">
+        <f>AVERAGE(SUM(simulations_small!J12:O12),SUM(simulations_medium!J12:O12),SUM(simulations_large!J12:O12))</f>
+        <v>2321312078.2334747</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J12" s="6">
+        <v>60000</v>
+      </c>
+      <c r="K12">
+        <f>AVERAGE(SUM(simulations_small!J13:O13),SUM(simulations_medium!J13:O13),SUM(simulations_large!J13:O13))</f>
+        <v>2269874745.8999739</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B13" s="24" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J13" s="6">
+        <v>65000</v>
+      </c>
+      <c r="K13">
+        <f>AVERAGE(SUM(simulations_small!J14:O14),SUM(simulations_medium!J14:O14),SUM(simulations_large!J14:O14))</f>
+        <v>2446875316.0901127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B14" s="28" t="str">
         <f>B8</f>
         <v>MAE_mean</v>
@@ -1245,8 +1225,15 @@
         <f t="shared" si="1"/>
         <v>RMSE_var</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J14" s="6">
+        <v>70000</v>
+      </c>
+      <c r="K14">
+        <f>AVERAGE(SUM(simulations_small!J15:O15),SUM(simulations_medium!J15:O15),SUM(simulations_large!J15:O15))</f>
+        <v>688144121.45951807</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B15" s="44">
         <f>MIN(simulations_large!$J$3:$J$15)</f>
         <v>30.783059199999915</v>
@@ -1272,7 +1259,7 @@
         <v>18201.661163097117</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -1309,10 +1296,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{544FD0B2-A7ED-4478-8092-5F67F619DD9A}">
-  <dimension ref="A1:R64"/>
+  <dimension ref="A1:S64"/>
   <sheetViews>
-    <sheetView topLeftCell="C28" zoomScale="90" workbookViewId="0">
-      <selection activeCell="F48" sqref="F47:F48"/>
+    <sheetView topLeftCell="C1" zoomScale="72" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3:I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1988,7 +1975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A17" s="6">
         <v>15000</v>
       </c>
@@ -2013,7 +2000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A18" s="6">
         <v>15000</v>
       </c>
@@ -2041,7 +2028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A19" s="6">
         <v>15000</v>
       </c>
@@ -2073,7 +2060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A20" s="6">
         <v>15000</v>
       </c>
@@ -2105,7 +2092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A21" s="10">
         <v>20000</v>
       </c>
@@ -2132,7 +2119,7 @@
         <v>6970</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A22" s="14">
         <v>20000</v>
       </c>
@@ -2159,7 +2146,7 @@
         <v>8343</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A23" s="14">
         <v>20000</v>
       </c>
@@ -2186,7 +2173,7 @@
         <v>9428</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A24" s="17">
         <v>20000</v>
       </c>
@@ -2213,7 +2200,7 @@
         <v>10111</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A25" s="6">
         <v>25000</v>
       </c>
@@ -2240,7 +2227,7 @@
         <v>13979</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A26" s="6">
         <v>25000</v>
       </c>
@@ -2267,7 +2254,7 @@
         <v>15291</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A27" s="6">
         <v>25000</v>
       </c>
@@ -2294,7 +2281,7 @@
         <v>17538</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A28" s="6">
         <v>25000</v>
       </c>
@@ -2321,7 +2308,7 @@
         <v>20935</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A29" s="10">
         <v>30000</v>
       </c>
@@ -2348,7 +2335,7 @@
         <v>20938</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A30" s="14">
         <v>30000</v>
       </c>
@@ -2375,7 +2362,7 @@
         <v>24465</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A31" s="14">
         <v>30000</v>
       </c>
@@ -2402,7 +2389,7 @@
         <v>25274</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A32" s="17">
         <v>30000</v>
       </c>
@@ -2421,8 +2408,19 @@
       <c r="F32" s="20">
         <v>9428</v>
       </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="I32"/>
+      <c r="J32"/>
+      <c r="K32"/>
+      <c r="L32"/>
+      <c r="M32"/>
+      <c r="N32"/>
+      <c r="O32"/>
+      <c r="P32"/>
+      <c r="Q32"/>
+      <c r="R32"/>
+      <c r="S32"/>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A33" s="6">
         <v>35000</v>
       </c>
@@ -2441,11 +2439,19 @@
       <c r="F33" s="2">
         <v>10111</v>
       </c>
-      <c r="J33" s="61" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="I33"/>
+      <c r="J33"/>
+      <c r="K33"/>
+      <c r="L33"/>
+      <c r="M33"/>
+      <c r="N33"/>
+      <c r="O33"/>
+      <c r="P33"/>
+      <c r="Q33"/>
+      <c r="R33"/>
+      <c r="S33"/>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A34" s="6">
         <v>35000</v>
       </c>
@@ -2464,9 +2470,8 @@
       <c r="F34" s="2">
         <v>10111</v>
       </c>
-      <c r="J34" t="s">
-        <v>35</v>
-      </c>
+      <c r="I34"/>
+      <c r="J34"/>
       <c r="K34"/>
       <c r="L34"/>
       <c r="M34"/>
@@ -2475,8 +2480,9 @@
       <c r="P34"/>
       <c r="Q34"/>
       <c r="R34"/>
-    </row>
-    <row r="35" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="S34"/>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A35" s="6">
         <v>35000</v>
       </c>
@@ -2495,6 +2501,7 @@
       <c r="F35" s="2">
         <v>10111</v>
       </c>
+      <c r="I35"/>
       <c r="J35"/>
       <c r="K35"/>
       <c r="L35"/>
@@ -2504,8 +2511,9 @@
       <c r="P35"/>
       <c r="Q35"/>
       <c r="R35"/>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S35"/>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A36" s="6">
         <v>35000</v>
       </c>
@@ -2524,10 +2532,9 @@
       <c r="F36" s="2">
         <v>10111</v>
       </c>
-      <c r="J36" s="56" t="s">
-        <v>36</v>
-      </c>
-      <c r="K36" s="56"/>
+      <c r="I36"/>
+      <c r="J36"/>
+      <c r="K36"/>
       <c r="L36"/>
       <c r="M36"/>
       <c r="N36"/>
@@ -2535,8 +2542,9 @@
       <c r="P36"/>
       <c r="Q36"/>
       <c r="R36"/>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S36"/>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A37" s="10">
         <v>40000</v>
       </c>
@@ -2555,12 +2563,9 @@
       <c r="F37" s="13">
         <v>13979</v>
       </c>
-      <c r="J37" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="K37" s="53">
-        <v>5.108241672607418E-3</v>
-      </c>
+      <c r="I37"/>
+      <c r="J37"/>
+      <c r="K37"/>
       <c r="L37"/>
       <c r="M37"/>
       <c r="N37"/>
@@ -2568,8 +2573,9 @@
       <c r="P37"/>
       <c r="Q37"/>
       <c r="R37"/>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S37"/>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A38" s="14">
         <v>40000</v>
       </c>
@@ -2588,12 +2594,9 @@
       <c r="F38" s="16">
         <v>13979</v>
       </c>
-      <c r="J38" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="K38" s="58">
-        <v>2.6094132985763035E-5</v>
-      </c>
+      <c r="I38"/>
+      <c r="J38"/>
+      <c r="K38"/>
       <c r="L38"/>
       <c r="M38"/>
       <c r="N38"/>
@@ -2601,8 +2604,9 @@
       <c r="P38"/>
       <c r="Q38"/>
       <c r="R38"/>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S38"/>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A39" s="14">
         <v>40000</v>
       </c>
@@ -2621,12 +2625,9 @@
       <c r="F39" s="16">
         <v>13979</v>
       </c>
-      <c r="J39" s="53" t="s">
-        <v>39</v>
-      </c>
-      <c r="K39" s="53">
-        <v>-1.9973383984354522E-2</v>
-      </c>
+      <c r="I39"/>
+      <c r="J39"/>
+      <c r="K39"/>
       <c r="L39"/>
       <c r="M39"/>
       <c r="N39"/>
@@ -2634,8 +2635,9 @@
       <c r="P39"/>
       <c r="Q39"/>
       <c r="R39"/>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S39"/>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A40" s="17">
         <v>40000</v>
       </c>
@@ -2654,12 +2656,9 @@
       <c r="F40" s="20">
         <v>13979</v>
       </c>
-      <c r="J40" s="53" t="s">
-        <v>40</v>
-      </c>
-      <c r="K40" s="53">
-        <v>640172.64137594448</v>
-      </c>
+      <c r="I40"/>
+      <c r="J40"/>
+      <c r="K40"/>
       <c r="L40"/>
       <c r="M40"/>
       <c r="N40"/>
@@ -2667,8 +2666,9 @@
       <c r="P40"/>
       <c r="Q40"/>
       <c r="R40"/>
-    </row>
-    <row r="41" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="S40"/>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A41" s="14">
         <v>45000</v>
       </c>
@@ -2687,12 +2687,9 @@
       <c r="F41" s="2">
         <v>15291</v>
       </c>
-      <c r="J41" s="54" t="s">
-        <v>41</v>
-      </c>
-      <c r="K41" s="54">
-        <v>52</v>
-      </c>
+      <c r="I41"/>
+      <c r="J41"/>
+      <c r="K41"/>
       <c r="L41"/>
       <c r="M41"/>
       <c r="N41"/>
@@ -2700,8 +2697,9 @@
       <c r="P41"/>
       <c r="Q41"/>
       <c r="R41"/>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S41"/>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A42" s="14">
         <v>45000</v>
       </c>
@@ -2720,6 +2718,7 @@
       <c r="F42" s="2">
         <v>15291</v>
       </c>
+      <c r="I42"/>
       <c r="J42"/>
       <c r="K42"/>
       <c r="L42"/>
@@ -2729,8 +2728,9 @@
       <c r="P42"/>
       <c r="Q42"/>
       <c r="R42"/>
-    </row>
-    <row r="43" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="S42"/>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A43" s="14">
         <v>45000</v>
       </c>
@@ -2749,9 +2749,8 @@
       <c r="F43" s="2">
         <v>15291</v>
       </c>
-      <c r="J43" t="s">
-        <v>42</v>
-      </c>
+      <c r="I43"/>
+      <c r="J43"/>
       <c r="K43"/>
       <c r="L43"/>
       <c r="M43"/>
@@ -2760,8 +2759,9 @@
       <c r="P43"/>
       <c r="Q43"/>
       <c r="R43"/>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S43"/>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A44" s="14">
         <v>45000</v>
       </c>
@@ -2780,27 +2780,19 @@
       <c r="F44" s="2">
         <v>15291</v>
       </c>
-      <c r="J44" s="55"/>
-      <c r="K44" s="55" t="s">
-        <v>47</v>
-      </c>
-      <c r="L44" s="55" t="s">
-        <v>48</v>
-      </c>
-      <c r="M44" s="55" t="s">
-        <v>49</v>
-      </c>
-      <c r="N44" s="55" t="s">
-        <v>50</v>
-      </c>
-      <c r="O44" s="55" t="s">
-        <v>51</v>
-      </c>
+      <c r="I44"/>
+      <c r="J44"/>
+      <c r="K44"/>
+      <c r="L44"/>
+      <c r="M44"/>
+      <c r="N44"/>
+      <c r="O44"/>
       <c r="P44"/>
       <c r="Q44"/>
       <c r="R44"/>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S44"/>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A45" s="10">
         <v>50000</v>
       </c>
@@ -2819,29 +2811,19 @@
       <c r="F45" s="13">
         <v>17538</v>
       </c>
-      <c r="J45" s="53" t="s">
-        <v>43</v>
-      </c>
-      <c r="K45" s="53">
-        <v>1</v>
-      </c>
-      <c r="L45" s="53">
-        <v>534710150.5625</v>
-      </c>
-      <c r="M45" s="53">
-        <v>534710150.5625</v>
-      </c>
-      <c r="N45" s="53">
-        <v>1.3047406953653686E-3</v>
-      </c>
-      <c r="O45" s="53">
-        <v>0.97132954942729999</v>
-      </c>
+      <c r="I45"/>
+      <c r="J45"/>
+      <c r="K45"/>
+      <c r="L45"/>
+      <c r="M45"/>
+      <c r="N45"/>
+      <c r="O45"/>
       <c r="P45"/>
       <c r="Q45"/>
       <c r="R45"/>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S45"/>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A46" s="14">
         <v>50000</v>
       </c>
@@ -2860,25 +2842,19 @@
       <c r="F46" s="16">
         <v>17538</v>
       </c>
-      <c r="J46" s="53" t="s">
-        <v>44</v>
-      </c>
-      <c r="K46" s="53">
-        <v>50</v>
-      </c>
-      <c r="L46" s="53">
-        <v>20491050538312.684</v>
-      </c>
-      <c r="M46" s="53">
-        <v>409821010766.25366</v>
-      </c>
-      <c r="N46" s="53"/>
-      <c r="O46" s="53"/>
+      <c r="I46"/>
+      <c r="J46"/>
+      <c r="K46"/>
+      <c r="L46"/>
+      <c r="M46"/>
+      <c r="N46"/>
+      <c r="O46"/>
       <c r="P46"/>
       <c r="Q46"/>
       <c r="R46"/>
-    </row>
-    <row r="47" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="S46"/>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A47" s="14">
         <v>50000</v>
       </c>
@@ -2897,23 +2873,19 @@
       <c r="F47" s="16">
         <v>17538</v>
       </c>
-      <c r="J47" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="K47" s="54">
-        <v>51</v>
-      </c>
-      <c r="L47" s="54">
-        <v>20491585248463.246</v>
-      </c>
-      <c r="M47" s="54"/>
-      <c r="N47" s="54"/>
-      <c r="O47" s="54"/>
+      <c r="I47"/>
+      <c r="J47"/>
+      <c r="K47"/>
+      <c r="L47"/>
+      <c r="M47"/>
+      <c r="N47"/>
+      <c r="O47"/>
       <c r="P47"/>
       <c r="Q47"/>
       <c r="R47"/>
-    </row>
-    <row r="48" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="S47"/>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A48" s="17">
         <v>50000</v>
       </c>
@@ -2932,6 +2904,7 @@
       <c r="F48" s="20">
         <v>17538</v>
       </c>
+      <c r="I48"/>
       <c r="J48"/>
       <c r="K48"/>
       <c r="L48"/>
@@ -2941,8 +2914,9 @@
       <c r="P48"/>
       <c r="Q48"/>
       <c r="R48"/>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S48"/>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A49" s="22">
         <v>55000</v>
       </c>
@@ -2961,33 +2935,19 @@
       <c r="F49" s="2">
         <v>20935</v>
       </c>
-      <c r="J49" s="55"/>
-      <c r="K49" s="55" t="s">
-        <v>52</v>
-      </c>
-      <c r="L49" s="55" t="s">
-        <v>40</v>
-      </c>
-      <c r="M49" s="55" t="s">
-        <v>53</v>
-      </c>
-      <c r="N49" s="55" t="s">
-        <v>54</v>
-      </c>
-      <c r="O49" s="55" t="s">
-        <v>55</v>
-      </c>
-      <c r="P49" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q49" s="55" t="s">
-        <v>57</v>
-      </c>
-      <c r="R49" s="55" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="I49"/>
+      <c r="J49"/>
+      <c r="K49"/>
+      <c r="L49"/>
+      <c r="M49"/>
+      <c r="N49"/>
+      <c r="O49"/>
+      <c r="P49"/>
+      <c r="Q49"/>
+      <c r="R49"/>
+      <c r="S49"/>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A50" s="22">
         <v>55000</v>
       </c>
@@ -3006,35 +2966,19 @@
       <c r="F50" s="2">
         <v>20935</v>
       </c>
-      <c r="J50" s="53" t="s">
-        <v>46</v>
-      </c>
-      <c r="K50" s="53">
-        <v>955829.71997783834</v>
-      </c>
-      <c r="L50" s="53">
-        <v>209545.68478179176</v>
-      </c>
-      <c r="M50" s="53">
-        <v>4.5614383372923273</v>
-      </c>
-      <c r="N50" s="53">
-        <v>3.3142796961536426E-5</v>
-      </c>
-      <c r="O50" s="53">
-        <v>534944.82540797675</v>
-      </c>
-      <c r="P50" s="53">
-        <v>1376714.6145476999</v>
-      </c>
-      <c r="Q50" s="53">
-        <v>534944.82540797675</v>
-      </c>
-      <c r="R50" s="53">
-        <v>1376714.6145476999</v>
-      </c>
-    </row>
-    <row r="51" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I50"/>
+      <c r="J50"/>
+      <c r="K50"/>
+      <c r="L50"/>
+      <c r="M50"/>
+      <c r="N50"/>
+      <c r="O50"/>
+      <c r="P50"/>
+      <c r="Q50"/>
+      <c r="R50"/>
+      <c r="S50"/>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A51" s="22">
         <v>55000</v>
       </c>
@@ -3053,35 +2997,19 @@
       <c r="F51" s="2">
         <v>20935</v>
       </c>
-      <c r="J51" s="54" t="s">
-        <v>0</v>
-      </c>
-      <c r="K51" s="54">
-        <v>-0.17140501335220015</v>
-      </c>
-      <c r="L51" s="54">
-        <v>4.7452753296505108</v>
-      </c>
-      <c r="M51" s="54">
-        <v>-3.6121194545064281E-2</v>
-      </c>
-      <c r="N51" s="57">
-        <v>0.97132954942733274</v>
-      </c>
-      <c r="O51" s="54">
-        <v>-9.702571016148676</v>
-      </c>
-      <c r="P51" s="54">
-        <v>9.3597609894442773</v>
-      </c>
-      <c r="Q51" s="54">
-        <v>-9.702571016148676</v>
-      </c>
-      <c r="R51" s="54">
-        <v>9.3597609894442773</v>
-      </c>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="I51"/>
+      <c r="J51"/>
+      <c r="K51"/>
+      <c r="L51"/>
+      <c r="M51"/>
+      <c r="N51"/>
+      <c r="O51"/>
+      <c r="P51"/>
+      <c r="Q51"/>
+      <c r="R51"/>
+      <c r="S51"/>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A52" s="22">
         <v>55000</v>
       </c>
@@ -3100,6 +3028,7 @@
       <c r="F52" s="2">
         <v>20935</v>
       </c>
+      <c r="I52"/>
       <c r="J52"/>
       <c r="K52"/>
       <c r="L52"/>
@@ -3109,8 +3038,9 @@
       <c r="P52"/>
       <c r="Q52"/>
       <c r="R52"/>
-    </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S52"/>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A53" s="10">
         <v>60000</v>
       </c>
@@ -3129,6 +3059,7 @@
       <c r="F53" s="13">
         <v>20938</v>
       </c>
+      <c r="I53"/>
       <c r="J53"/>
       <c r="K53"/>
       <c r="L53"/>
@@ -3138,8 +3069,9 @@
       <c r="P53"/>
       <c r="Q53"/>
       <c r="R53"/>
-    </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S53"/>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A54" s="14">
         <v>60000</v>
       </c>
@@ -3168,7 +3100,7 @@
       <c r="Q54"/>
       <c r="R54"/>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A55" s="14">
         <v>60000</v>
       </c>
@@ -3188,7 +3120,7 @@
         <v>20938</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A56" s="17">
         <v>60000</v>
       </c>
@@ -3208,7 +3140,7 @@
         <v>20938</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A57" s="22">
         <v>65000</v>
       </c>
@@ -3228,7 +3160,7 @@
         <v>24465</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A58" s="22">
         <v>65000</v>
       </c>
@@ -3248,7 +3180,7 @@
         <v>24465</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A59" s="22">
         <v>65000</v>
       </c>
@@ -3268,7 +3200,7 @@
         <v>24465</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A60" s="22">
         <v>65000</v>
       </c>
@@ -3288,7 +3220,7 @@
         <v>24465</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A61" s="10">
         <v>70000</v>
       </c>
@@ -3308,7 +3240,7 @@
         <v>25274</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A62" s="14">
         <v>70000</v>
       </c>
@@ -3328,7 +3260,7 @@
         <v>25274</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A63" s="14">
         <v>70000</v>
       </c>
@@ -3348,7 +3280,7 @@
         <v>25274</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A64" s="17">
         <v>70000</v>
       </c>
@@ -3675,38 +3607,36 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32199EA4-1B1E-4F05-B93A-A4002D945EFC}">
-  <dimension ref="A1:AA132"/>
+  <dimension ref="A1:R132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D32" zoomScale="90" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="54" workbookViewId="0">
+      <selection activeCell="W25" sqref="W25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.90625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.08984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.90625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.90625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="8.7265625" style="2"/>
     <col min="9" max="9" width="22.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.08984375" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.7265625" style="2" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8.7265625" style="2" hidden="1" customWidth="1"/>
     <col min="17" max="18" width="8.7265625" style="2"/>
-    <col min="19" max="19" width="22.90625" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="23" width="8.7265625" style="2"/>
-    <col min="24" max="24" width="12.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="8.7265625" style="2"/>
+    <col min="19" max="19" width="22.90625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="49" t="s">
         <v>18</v>
       </c>
@@ -3715,7 +3645,7 @@
       <c r="D1" s="49"/>
       <c r="E1" s="49"/>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
         <v>14</v>
       </c>
@@ -3749,11 +3679,8 @@
       <c r="O2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="S2" s="59" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>0</v>
       </c>
@@ -3800,19 +3727,8 @@
         <f>I3</f>
         <v>10000</v>
       </c>
-      <c r="S3" t="s">
-        <v>35</v>
-      </c>
-      <c r="T3"/>
-      <c r="U3"/>
-      <c r="V3"/>
-      <c r="W3"/>
-      <c r="X3"/>
-      <c r="Y3"/>
-      <c r="Z3"/>
-      <c r="AA3"/>
-    </row>
-    <row r="4" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -3859,17 +3775,8 @@
         <f t="shared" ref="P4:P33" si="2">I4</f>
         <v>15000</v>
       </c>
-      <c r="S4"/>
-      <c r="T4"/>
-      <c r="U4"/>
-      <c r="V4"/>
-      <c r="W4"/>
-      <c r="X4"/>
-      <c r="Y4"/>
-      <c r="Z4"/>
-      <c r="AA4"/>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -3916,19 +3823,8 @@
         <f t="shared" si="2"/>
         <v>20000</v>
       </c>
-      <c r="S5" s="56" t="s">
-        <v>36</v>
-      </c>
-      <c r="T5" s="56"/>
-      <c r="U5"/>
-      <c r="V5"/>
-      <c r="W5"/>
-      <c r="X5"/>
-      <c r="Y5"/>
-      <c r="Z5"/>
-      <c r="AA5"/>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -3975,21 +3871,8 @@
         <f t="shared" si="2"/>
         <v>25000</v>
       </c>
-      <c r="S6" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="T6" s="53">
-        <v>0.26557170530539403</v>
-      </c>
-      <c r="U6"/>
-      <c r="V6"/>
-      <c r="W6"/>
-      <c r="X6"/>
-      <c r="Y6"/>
-      <c r="Z6"/>
-      <c r="AA6"/>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -4036,21 +3919,8 @@
         <f t="shared" si="2"/>
         <v>30000</v>
       </c>
-      <c r="S7" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="T7" s="58">
-        <v>7.0528330658815058E-2</v>
-      </c>
-      <c r="U7"/>
-      <c r="V7"/>
-      <c r="W7"/>
-      <c r="X7"/>
-      <c r="Y7"/>
-      <c r="Z7"/>
-      <c r="AA7"/>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>5</v>
       </c>
@@ -4097,21 +3967,8 @@
         <f t="shared" si="2"/>
         <v>35000</v>
       </c>
-      <c r="S8" s="53" t="s">
-        <v>39</v>
-      </c>
-      <c r="T8" s="53">
-        <v>-1.3969093826747209E-2</v>
-      </c>
-      <c r="U8"/>
-      <c r="V8"/>
-      <c r="W8"/>
-      <c r="X8"/>
-      <c r="Y8"/>
-      <c r="Z8"/>
-      <c r="AA8"/>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>6</v>
       </c>
@@ -4158,21 +4015,8 @@
         <f t="shared" si="2"/>
         <v>40000</v>
       </c>
-      <c r="S9" s="53" t="s">
-        <v>40</v>
-      </c>
-      <c r="T9" s="53">
-        <v>13898.735388983358</v>
-      </c>
-      <c r="U9"/>
-      <c r="V9"/>
-      <c r="W9"/>
-      <c r="X9"/>
-      <c r="Y9"/>
-      <c r="Z9"/>
-      <c r="AA9"/>
-    </row>
-    <row r="10" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>7</v>
       </c>
@@ -4219,21 +4063,8 @@
         <f t="shared" si="2"/>
         <v>45000</v>
       </c>
-      <c r="S10" s="54" t="s">
-        <v>41</v>
-      </c>
-      <c r="T10" s="54">
-        <v>13</v>
-      </c>
-      <c r="U10"/>
-      <c r="V10"/>
-      <c r="W10"/>
-      <c r="X10"/>
-      <c r="Y10"/>
-      <c r="Z10"/>
-      <c r="AA10"/>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>8</v>
       </c>
@@ -4280,17 +4111,8 @@
         <f t="shared" si="2"/>
         <v>50000</v>
       </c>
-      <c r="S11"/>
-      <c r="T11"/>
-      <c r="U11"/>
-      <c r="V11"/>
-      <c r="W11"/>
-      <c r="X11"/>
-      <c r="Y11"/>
-      <c r="Z11"/>
-      <c r="AA11"/>
-    </row>
-    <row r="12" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>9</v>
       </c>
@@ -4337,19 +4159,8 @@
         <f t="shared" si="2"/>
         <v>55000</v>
       </c>
-      <c r="S12" t="s">
-        <v>42</v>
-      </c>
-      <c r="T12"/>
-      <c r="U12"/>
-      <c r="V12"/>
-      <c r="W12"/>
-      <c r="X12"/>
-      <c r="Y12"/>
-      <c r="Z12"/>
-      <c r="AA12"/>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="I13" s="8">
         <v>60000</v>
       </c>
@@ -4381,27 +4192,8 @@
         <f t="shared" si="2"/>
         <v>60000</v>
       </c>
-      <c r="S13" s="55"/>
-      <c r="T13" s="55" t="s">
-        <v>47</v>
-      </c>
-      <c r="U13" s="55" t="s">
-        <v>48</v>
-      </c>
-      <c r="V13" s="55" t="s">
-        <v>49</v>
-      </c>
-      <c r="W13" s="55" t="s">
-        <v>50</v>
-      </c>
-      <c r="X13" s="55" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y13"/>
-      <c r="Z13"/>
-      <c r="AA13"/>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="50" t="s">
         <v>19</v>
       </c>
@@ -4441,29 +4233,8 @@
         <f t="shared" si="2"/>
         <v>65000</v>
       </c>
-      <c r="S14" s="53" t="s">
-        <v>43</v>
-      </c>
-      <c r="T14" s="53">
-        <v>1</v>
-      </c>
-      <c r="U14" s="53">
-        <v>161239226.58234334</v>
-      </c>
-      <c r="V14" s="53">
-        <v>161239226.58234334</v>
-      </c>
-      <c r="W14" s="53">
-        <v>0.83468024129973262</v>
-      </c>
-      <c r="X14" s="53">
-        <v>0.38051195180522723</v>
-      </c>
-      <c r="Y14"/>
-      <c r="Z14"/>
-      <c r="AA14"/>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>0</v>
       </c>
@@ -4513,25 +4284,8 @@
         <f t="shared" si="2"/>
         <v>70000</v>
       </c>
-      <c r="S15" s="53" t="s">
-        <v>44</v>
-      </c>
-      <c r="T15" s="53">
-        <v>11</v>
-      </c>
-      <c r="U15" s="53">
-        <v>2124923299.542762</v>
-      </c>
-      <c r="V15" s="53">
-        <v>193174845.41297838</v>
-      </c>
-      <c r="W15" s="53"/>
-      <c r="X15" s="53"/>
-      <c r="Y15"/>
-      <c r="Z15"/>
-      <c r="AA15"/>
-    </row>
-    <row r="16" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="10">
         <v>10000</v>
       </c>
@@ -4554,23 +4308,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S16" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="T16" s="54">
-        <v>12</v>
-      </c>
-      <c r="U16" s="54">
-        <v>2286162526.1251054</v>
-      </c>
-      <c r="V16" s="54"/>
-      <c r="W16" s="54"/>
-      <c r="X16" s="54"/>
-      <c r="Y16"/>
-      <c r="Z16"/>
-      <c r="AA16"/>
-    </row>
-    <row r="17" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="14">
         <v>10000</v>
       </c>
@@ -4591,17 +4330,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S17"/>
-      <c r="T17"/>
-      <c r="U17"/>
-      <c r="V17"/>
-      <c r="W17"/>
-      <c r="X17"/>
-      <c r="Y17"/>
-      <c r="Z17"/>
-      <c r="AA17"/>
-    </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="14">
         <v>10000</v>
       </c>
@@ -4625,33 +4355,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S18" s="55"/>
-      <c r="T18" s="55" t="s">
-        <v>52</v>
-      </c>
-      <c r="U18" s="55" t="s">
-        <v>40</v>
-      </c>
-      <c r="V18" s="55" t="s">
-        <v>53</v>
-      </c>
-      <c r="W18" s="55" t="s">
-        <v>54</v>
-      </c>
-      <c r="X18" s="55" t="s">
-        <v>55</v>
-      </c>
-      <c r="Y18" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z18" s="55" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA18" s="55" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="14">
         <v>10000</v>
       </c>
@@ -4680,35 +4385,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S19" s="53" t="s">
-        <v>46</v>
-      </c>
-      <c r="T19" s="53">
-        <v>35281.757820593419</v>
-      </c>
-      <c r="U19" s="53">
-        <v>9098.8581405968198</v>
-      </c>
-      <c r="V19" s="53">
-        <v>3.8776028019576518</v>
-      </c>
-      <c r="W19" s="53">
-        <v>2.5739757452500809E-3</v>
-      </c>
-      <c r="X19" s="53">
-        <v>15255.30607936082</v>
-      </c>
-      <c r="Y19" s="53">
-        <v>55308.209561826021</v>
-      </c>
-      <c r="Z19" s="53">
-        <v>15255.30607936082</v>
-      </c>
-      <c r="AA19" s="53">
-        <v>55308.209561826021</v>
-      </c>
-    </row>
-    <row r="20" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="14">
         <v>10000</v>
       </c>
@@ -4734,35 +4412,8 @@
         <v>8582</v>
       </c>
       <c r="P20" s="6"/>
-      <c r="S20" s="54" t="s">
-        <v>0</v>
-      </c>
-      <c r="T20" s="54">
-        <v>-0.1882476896417592</v>
-      </c>
-      <c r="U20" s="54">
-        <v>0.20604856219074758</v>
-      </c>
-      <c r="V20" s="54">
-        <v>-0.91360836319493754</v>
-      </c>
-      <c r="W20" s="57">
-        <v>0.38051195180522723</v>
-      </c>
-      <c r="X20" s="54">
-        <v>-0.64175751728181363</v>
-      </c>
-      <c r="Y20" s="54">
-        <v>0.26526213799829523</v>
-      </c>
-      <c r="Z20" s="54">
-        <v>-0.64175751728181363</v>
-      </c>
-      <c r="AA20" s="54">
-        <v>0.26526213799829523</v>
-      </c>
-    </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" s="14">
         <v>10000</v>
       </c>
@@ -4788,19 +4439,8 @@
         <v>20300</v>
       </c>
       <c r="P21" s="6"/>
-      <c r="S21" s="60" t="s">
-        <v>61</v>
-      </c>
-      <c r="T21"/>
-      <c r="U21"/>
-      <c r="V21"/>
-      <c r="W21"/>
-      <c r="X21"/>
-      <c r="Y21"/>
-      <c r="Z21"/>
-      <c r="AA21"/>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="14">
         <v>10000</v>
       </c>
@@ -4826,17 +4466,8 @@
         <v>19609</v>
       </c>
       <c r="P22" s="6"/>
-      <c r="S22"/>
-      <c r="T22"/>
-      <c r="U22"/>
-      <c r="V22"/>
-      <c r="W22"/>
-      <c r="X22"/>
-      <c r="Y22"/>
-      <c r="Z22"/>
-      <c r="AA22"/>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" s="14">
         <v>10000</v>
       </c>
@@ -4862,17 +4493,8 @@
         <v>32812</v>
       </c>
       <c r="P23" s="6"/>
-      <c r="S23"/>
-      <c r="T23"/>
-      <c r="U23"/>
-      <c r="V23"/>
-      <c r="W23"/>
-      <c r="X23"/>
-      <c r="Y23"/>
-      <c r="Z23"/>
-      <c r="AA23"/>
-    </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" s="17">
         <v>10000</v>
       </c>
@@ -4898,11 +4520,8 @@
         <v>24192</v>
       </c>
       <c r="P24" s="6"/>
-      <c r="S24" s="59" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" s="6">
         <v>15000</v>
       </c>
@@ -4933,19 +4552,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S25" t="s">
-        <v>35</v>
-      </c>
-      <c r="T25"/>
-      <c r="U25"/>
-      <c r="V25"/>
-      <c r="W25"/>
-      <c r="X25"/>
-      <c r="Y25"/>
-      <c r="Z25"/>
-      <c r="AA25"/>
-    </row>
-    <row r="26" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" s="6">
         <v>15000</v>
       </c>
@@ -4973,17 +4581,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S26"/>
-      <c r="T26"/>
-      <c r="U26"/>
-      <c r="V26"/>
-      <c r="W26"/>
-      <c r="X26"/>
-      <c r="Y26"/>
-      <c r="Z26"/>
-      <c r="AA26"/>
-    </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" s="6">
         <v>15000</v>
       </c>
@@ -5011,19 +4610,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S27" s="56" t="s">
-        <v>36</v>
-      </c>
-      <c r="T27" s="56"/>
-      <c r="U27"/>
-      <c r="V27"/>
-      <c r="W27"/>
-      <c r="X27"/>
-      <c r="Y27"/>
-      <c r="Z27"/>
-      <c r="AA27"/>
-    </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" s="6">
         <v>15000</v>
       </c>
@@ -5048,21 +4636,8 @@
         <v>153110</v>
       </c>
       <c r="P28" s="6"/>
-      <c r="S28" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="T28" s="53">
-        <v>0.39274668409395302</v>
-      </c>
-      <c r="U28"/>
-      <c r="V28"/>
-      <c r="W28"/>
-      <c r="X28"/>
-      <c r="Y28"/>
-      <c r="Z28"/>
-      <c r="AA28"/>
-    </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" s="6">
         <v>15000</v>
       </c>
@@ -5087,21 +4662,8 @@
         <v>74655</v>
       </c>
       <c r="P29" s="6"/>
-      <c r="S29" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="T29" s="58">
-        <v>0.15424995786679532</v>
-      </c>
-      <c r="U29"/>
-      <c r="V29"/>
-      <c r="W29"/>
-      <c r="X29"/>
-      <c r="Y29"/>
-      <c r="Z29"/>
-      <c r="AA29"/>
-    </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" s="6">
         <v>15000</v>
       </c>
@@ -5126,21 +4688,8 @@
         <v>124032</v>
       </c>
       <c r="P30" s="6"/>
-      <c r="S30" s="53" t="s">
-        <v>39</v>
-      </c>
-      <c r="T30" s="53">
-        <v>7.7363590400140361E-2</v>
-      </c>
-      <c r="U30"/>
-      <c r="V30"/>
-      <c r="W30"/>
-      <c r="X30"/>
-      <c r="Y30"/>
-      <c r="Z30"/>
-      <c r="AA30"/>
-    </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" s="6">
         <v>15000</v>
       </c>
@@ -5165,21 +4714,8 @@
         <v>137495</v>
       </c>
       <c r="P31" s="6"/>
-      <c r="S31" s="53" t="s">
-        <v>40</v>
-      </c>
-      <c r="T31" s="53">
-        <v>2046716960.536201</v>
-      </c>
-      <c r="U31"/>
-      <c r="V31"/>
-      <c r="W31"/>
-      <c r="X31"/>
-      <c r="Y31"/>
-      <c r="Z31"/>
-      <c r="AA31"/>
-    </row>
-    <row r="32" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A32" s="6">
         <v>15000</v>
       </c>
@@ -5197,21 +4733,8 @@
       </c>
       <c r="I32" s="6"/>
       <c r="P32" s="6"/>
-      <c r="S32" s="54" t="s">
-        <v>41</v>
-      </c>
-      <c r="T32" s="54">
-        <v>13</v>
-      </c>
-      <c r="U32"/>
-      <c r="V32"/>
-      <c r="W32"/>
-      <c r="X32"/>
-      <c r="Y32"/>
-      <c r="Z32"/>
-      <c r="AA32"/>
-    </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A33" s="6">
         <v>15000</v>
       </c>
@@ -5227,22 +4750,19 @@
       <c r="E33" s="7">
         <v>2023.4115280000001</v>
       </c>
-      <c r="I33" s="6"/>
-      <c r="P33" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="S33"/>
-      <c r="T33"/>
-      <c r="U33"/>
-      <c r="V33"/>
-      <c r="W33"/>
-      <c r="X33"/>
-      <c r="Y33"/>
-      <c r="Z33"/>
-      <c r="AA33"/>
-    </row>
-    <row r="34" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H33"/>
+      <c r="I33"/>
+      <c r="J33"/>
+      <c r="K33"/>
+      <c r="L33"/>
+      <c r="M33"/>
+      <c r="N33"/>
+      <c r="O33"/>
+      <c r="P33"/>
+      <c r="Q33"/>
+      <c r="R33"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A34" s="10">
         <v>20000</v>
       </c>
@@ -5261,22 +4781,19 @@
       <c r="F34" s="13">
         <v>20300</v>
       </c>
-      <c r="I34" s="61" t="s">
-        <v>63</v>
-      </c>
-      <c r="S34" t="s">
-        <v>42</v>
-      </c>
-      <c r="T34"/>
-      <c r="U34"/>
-      <c r="V34"/>
-      <c r="W34"/>
-      <c r="X34"/>
-      <c r="Y34"/>
-      <c r="Z34"/>
-      <c r="AA34"/>
-    </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="H34"/>
+      <c r="I34"/>
+      <c r="J34"/>
+      <c r="K34"/>
+      <c r="L34"/>
+      <c r="M34"/>
+      <c r="N34"/>
+      <c r="O34"/>
+      <c r="P34"/>
+      <c r="Q34"/>
+      <c r="R34"/>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A35" s="14">
         <v>20000</v>
       </c>
@@ -5293,9 +4810,8 @@
         <v>2418.0580810000001</v>
       </c>
       <c r="F35" s="16"/>
-      <c r="I35" t="s">
-        <v>35</v>
-      </c>
+      <c r="H35"/>
+      <c r="I35"/>
       <c r="J35"/>
       <c r="K35"/>
       <c r="L35"/>
@@ -5304,27 +4820,9 @@
       <c r="O35"/>
       <c r="P35"/>
       <c r="Q35"/>
-      <c r="S35" s="55"/>
-      <c r="T35" s="55" t="s">
-        <v>47</v>
-      </c>
-      <c r="U35" s="55" t="s">
-        <v>48</v>
-      </c>
-      <c r="V35" s="55" t="s">
-        <v>49</v>
-      </c>
-      <c r="W35" s="55" t="s">
-        <v>50</v>
-      </c>
-      <c r="X35" s="55" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y35"/>
-      <c r="Z35"/>
-      <c r="AA35"/>
-    </row>
-    <row r="36" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="R35"/>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A36" s="14">
         <v>20000</v>
       </c>
@@ -5341,6 +4839,7 @@
         <v>1736.419363</v>
       </c>
       <c r="F36" s="16"/>
+      <c r="H36"/>
       <c r="I36"/>
       <c r="J36"/>
       <c r="K36"/>
@@ -5350,29 +4849,9 @@
       <c r="O36"/>
       <c r="P36"/>
       <c r="Q36"/>
-      <c r="S36" s="53" t="s">
-        <v>43</v>
-      </c>
-      <c r="T36" s="53">
-        <v>1</v>
-      </c>
-      <c r="U36" s="53">
-        <v>8.4041014827423744E+18</v>
-      </c>
-      <c r="V36" s="53">
-        <v>8.4041014827423744E+18</v>
-      </c>
-      <c r="W36" s="53">
-        <v>2.0062068601913383</v>
-      </c>
-      <c r="X36" s="53">
-        <v>0.18434686508995585</v>
-      </c>
-      <c r="Y36"/>
-      <c r="Z36"/>
-      <c r="AA36"/>
-    </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="R36"/>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A37" s="14">
         <v>20000</v>
       </c>
@@ -5389,10 +4868,9 @@
         <v>1281.5688990000001</v>
       </c>
       <c r="F37" s="16"/>
-      <c r="I37" s="56" t="s">
-        <v>36</v>
-      </c>
-      <c r="J37" s="56"/>
+      <c r="H37"/>
+      <c r="I37"/>
+      <c r="J37"/>
       <c r="K37"/>
       <c r="L37"/>
       <c r="M37"/>
@@ -5400,25 +4878,9 @@
       <c r="O37"/>
       <c r="P37"/>
       <c r="Q37"/>
-      <c r="S37" s="53" t="s">
-        <v>44</v>
-      </c>
-      <c r="T37" s="53">
-        <v>11</v>
-      </c>
-      <c r="U37" s="53">
-        <v>4.6079553482011992E+19</v>
-      </c>
-      <c r="V37" s="53">
-        <v>4.1890503165465446E+18</v>
-      </c>
-      <c r="W37" s="53"/>
-      <c r="X37" s="53"/>
-      <c r="Y37"/>
-      <c r="Z37"/>
-      <c r="AA37"/>
-    </row>
-    <row r="38" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="R37"/>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A38" s="14">
         <v>20000</v>
       </c>
@@ -5435,12 +4897,9 @@
         <v>1099.935988</v>
       </c>
       <c r="F38" s="16"/>
-      <c r="I38" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="J38" s="53">
-        <v>5.1344405923386587E-3</v>
-      </c>
+      <c r="H38"/>
+      <c r="I38"/>
+      <c r="J38"/>
       <c r="K38"/>
       <c r="L38"/>
       <c r="M38"/>
@@ -5448,23 +4907,9 @@
       <c r="O38"/>
       <c r="P38"/>
       <c r="Q38"/>
-      <c r="S38" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="T38" s="54">
-        <v>12</v>
-      </c>
-      <c r="U38" s="54">
-        <v>5.4483654964754366E+19</v>
-      </c>
-      <c r="V38" s="54"/>
-      <c r="W38" s="54"/>
-      <c r="X38" s="54"/>
-      <c r="Y38"/>
-      <c r="Z38"/>
-      <c r="AA38"/>
-    </row>
-    <row r="39" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="R38"/>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A39" s="14">
         <v>20000</v>
       </c>
@@ -5481,12 +4926,9 @@
         <v>2870.3358739999999</v>
       </c>
       <c r="F39" s="16"/>
-      <c r="I39" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="J39" s="58">
-        <v>2.6362480196254958E-5</v>
-      </c>
+      <c r="H39"/>
+      <c r="I39"/>
+      <c r="J39"/>
       <c r="K39"/>
       <c r="L39"/>
       <c r="M39"/>
@@ -5494,17 +4936,9 @@
       <c r="O39"/>
       <c r="P39"/>
       <c r="Q39"/>
-      <c r="S39"/>
-      <c r="T39"/>
-      <c r="U39"/>
-      <c r="V39"/>
-      <c r="W39"/>
-      <c r="X39"/>
-      <c r="Y39"/>
-      <c r="Z39"/>
-      <c r="AA39"/>
-    </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="R39"/>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A40" s="14">
         <v>20000</v>
       </c>
@@ -5521,12 +4955,9 @@
         <v>2020.423241</v>
       </c>
       <c r="F40" s="16"/>
-      <c r="I40" s="53" t="s">
-        <v>39</v>
-      </c>
-      <c r="J40" s="53">
-        <v>-8.6690604547585599E-3</v>
-      </c>
+      <c r="H40"/>
+      <c r="I40"/>
+      <c r="J40"/>
       <c r="K40"/>
       <c r="L40"/>
       <c r="M40"/>
@@ -5534,33 +4965,9 @@
       <c r="O40"/>
       <c r="P40"/>
       <c r="Q40"/>
-      <c r="S40" s="55"/>
-      <c r="T40" s="55" t="s">
-        <v>52</v>
-      </c>
-      <c r="U40" s="55" t="s">
-        <v>40</v>
-      </c>
-      <c r="V40" s="55" t="s">
-        <v>53</v>
-      </c>
-      <c r="W40" s="55" t="s">
-        <v>54</v>
-      </c>
-      <c r="X40" s="55" t="s">
-        <v>55</v>
-      </c>
-      <c r="Y40" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z40" s="55" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA40" s="55" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="R40"/>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A41" s="14">
         <v>20000</v>
       </c>
@@ -5577,12 +4984,9 @@
         <v>2191.4627650000002</v>
       </c>
       <c r="F41" s="16"/>
-      <c r="I41" s="53" t="s">
-        <v>40</v>
-      </c>
-      <c r="J41" s="53">
-        <v>2870742.7075453</v>
-      </c>
+      <c r="H41"/>
+      <c r="I41"/>
+      <c r="J41"/>
       <c r="K41"/>
       <c r="L41"/>
       <c r="M41"/>
@@ -5590,35 +4994,9 @@
       <c r="O41"/>
       <c r="P41"/>
       <c r="Q41"/>
-      <c r="S41" s="53" t="s">
-        <v>46</v>
-      </c>
-      <c r="T41" s="53">
-        <v>3687828271.8079886</v>
-      </c>
-      <c r="U41" s="53">
-        <v>1339890771.115298</v>
-      </c>
-      <c r="V41" s="53">
-        <v>2.7523350046946846</v>
-      </c>
-      <c r="W41" s="53">
-        <v>1.881194984141463E-2</v>
-      </c>
-      <c r="X41" s="53">
-        <v>738748568.43947554</v>
-      </c>
-      <c r="Y41" s="53">
-        <v>6636907975.1765022</v>
-      </c>
-      <c r="Z41" s="53">
-        <v>738748568.43947554</v>
-      </c>
-      <c r="AA41" s="53">
-        <v>6636907975.1765022</v>
-      </c>
-    </row>
-    <row r="42" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="R41"/>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A42" s="17">
         <v>20000</v>
       </c>
@@ -5635,12 +5013,9 @@
         <v>2028.9167649999999</v>
       </c>
       <c r="F42" s="20"/>
-      <c r="I42" s="54" t="s">
-        <v>41</v>
-      </c>
-      <c r="J42" s="54">
-        <v>117</v>
-      </c>
+      <c r="H42"/>
+      <c r="I42"/>
+      <c r="J42"/>
       <c r="K42"/>
       <c r="L42"/>
       <c r="M42"/>
@@ -5648,35 +5023,9 @@
       <c r="O42"/>
       <c r="P42"/>
       <c r="Q42"/>
-      <c r="S42" s="54" t="s">
-        <v>0</v>
-      </c>
-      <c r="T42" s="54">
-        <v>-42977.380922205986</v>
-      </c>
-      <c r="U42" s="54">
-        <v>30342.5509679229</v>
-      </c>
-      <c r="V42" s="54">
-        <v>-1.4164063188899376</v>
-      </c>
-      <c r="W42" s="57">
-        <v>0.18434686508995504</v>
-      </c>
-      <c r="X42" s="54">
-        <v>-109760.88532192848</v>
-      </c>
-      <c r="Y42" s="54">
-        <v>23806.123477516499</v>
-      </c>
-      <c r="Z42" s="54">
-        <v>-109760.88532192848</v>
-      </c>
-      <c r="AA42" s="54">
-        <v>23806.123477516499</v>
-      </c>
-    </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="R42"/>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A43" s="6">
         <v>25000</v>
       </c>
@@ -5695,6 +5044,7 @@
       <c r="F43" s="2">
         <v>19609</v>
       </c>
+      <c r="H43"/>
       <c r="I43"/>
       <c r="J43"/>
       <c r="K43"/>
@@ -5704,17 +5054,9 @@
       <c r="O43"/>
       <c r="P43"/>
       <c r="Q43"/>
-      <c r="S43"/>
-      <c r="T43"/>
-      <c r="U43"/>
-      <c r="V43"/>
-      <c r="W43"/>
-      <c r="X43"/>
-      <c r="Y43"/>
-      <c r="Z43"/>
-      <c r="AA43"/>
-    </row>
-    <row r="44" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="R43"/>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A44" s="6">
         <v>25000</v>
       </c>
@@ -5730,9 +5072,8 @@
       <c r="E44" s="7">
         <v>2409.3637910000002</v>
       </c>
-      <c r="I44" t="s">
-        <v>42</v>
-      </c>
+      <c r="H44"/>
+      <c r="I44"/>
       <c r="J44"/>
       <c r="K44"/>
       <c r="L44"/>
@@ -5741,17 +5082,9 @@
       <c r="O44"/>
       <c r="P44"/>
       <c r="Q44"/>
-      <c r="S44"/>
-      <c r="T44"/>
-      <c r="U44"/>
-      <c r="V44"/>
-      <c r="W44"/>
-      <c r="X44"/>
-      <c r="Y44"/>
-      <c r="Z44"/>
-      <c r="AA44"/>
-    </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="R44"/>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A45" s="6">
         <v>25000</v>
       </c>
@@ -5767,36 +5100,19 @@
       <c r="E45" s="7">
         <v>1734.8206869999999</v>
       </c>
-      <c r="I45" s="55"/>
-      <c r="J45" s="55" t="s">
-        <v>47</v>
-      </c>
-      <c r="K45" s="55" t="s">
-        <v>48</v>
-      </c>
-      <c r="L45" s="55" t="s">
-        <v>49</v>
-      </c>
-      <c r="M45" s="55" t="s">
-        <v>50</v>
-      </c>
-      <c r="N45" s="55" t="s">
-        <v>51</v>
-      </c>
+      <c r="H45"/>
+      <c r="I45"/>
+      <c r="J45"/>
+      <c r="K45"/>
+      <c r="L45"/>
+      <c r="M45"/>
+      <c r="N45"/>
       <c r="O45"/>
       <c r="P45"/>
       <c r="Q45"/>
-      <c r="S45"/>
-      <c r="T45"/>
-      <c r="U45"/>
-      <c r="V45"/>
-      <c r="W45"/>
-      <c r="X45"/>
-      <c r="Y45"/>
-      <c r="Z45"/>
-      <c r="AA45"/>
-    </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="R45"/>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A46" s="6">
         <v>25000</v>
       </c>
@@ -5812,32 +5128,19 @@
       <c r="E46" s="7">
         <v>1282.959838</v>
       </c>
-      <c r="I46" s="53" t="s">
-        <v>43</v>
-      </c>
-      <c r="J46" s="53">
-        <v>1</v>
-      </c>
-      <c r="K46" s="53">
-        <v>24985272858.375</v>
-      </c>
-      <c r="L46" s="53">
-        <v>24985272858.375</v>
-      </c>
-      <c r="M46" s="53">
-        <v>3.0317651474179789E-3</v>
-      </c>
-      <c r="N46" s="53">
-        <v>0.95618503943484356</v>
-      </c>
+      <c r="H46"/>
+      <c r="I46"/>
+      <c r="J46"/>
+      <c r="K46"/>
+      <c r="L46"/>
+      <c r="M46"/>
+      <c r="N46"/>
       <c r="O46"/>
       <c r="P46"/>
       <c r="Q46"/>
-      <c r="S46" s="59" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="R46"/>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A47" s="6">
         <v>25000</v>
       </c>
@@ -5853,36 +5156,19 @@
       <c r="E47" s="7">
         <v>1104.7133240000001</v>
       </c>
-      <c r="I47" s="53" t="s">
-        <v>44</v>
-      </c>
-      <c r="J47" s="53">
-        <v>115</v>
-      </c>
-      <c r="K47" s="53">
-        <v>947733824686319.75</v>
-      </c>
-      <c r="L47" s="53">
-        <v>8241163692924.5195</v>
-      </c>
-      <c r="M47" s="53"/>
-      <c r="N47" s="53"/>
+      <c r="H47"/>
+      <c r="I47"/>
+      <c r="J47"/>
+      <c r="K47"/>
+      <c r="L47"/>
+      <c r="M47"/>
+      <c r="N47"/>
       <c r="O47"/>
       <c r="P47"/>
       <c r="Q47"/>
-      <c r="S47" t="s">
-        <v>35</v>
-      </c>
-      <c r="T47"/>
-      <c r="U47"/>
-      <c r="V47"/>
-      <c r="W47"/>
-      <c r="X47"/>
-      <c r="Y47"/>
-      <c r="Z47"/>
-      <c r="AA47"/>
-    </row>
-    <row r="48" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="R47"/>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A48" s="6">
         <v>25000</v>
       </c>
@@ -5898,32 +5184,19 @@
       <c r="E48" s="7">
         <v>2872.4061449999999</v>
       </c>
-      <c r="I48" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="J48" s="54">
-        <v>116</v>
-      </c>
-      <c r="K48" s="54">
-        <v>947758809959178.13</v>
-      </c>
-      <c r="L48" s="54"/>
-      <c r="M48" s="54"/>
-      <c r="N48" s="54"/>
+      <c r="H48"/>
+      <c r="I48"/>
+      <c r="J48"/>
+      <c r="K48"/>
+      <c r="L48"/>
+      <c r="M48"/>
+      <c r="N48"/>
       <c r="O48"/>
       <c r="P48"/>
       <c r="Q48"/>
-      <c r="S48"/>
-      <c r="T48"/>
-      <c r="U48"/>
-      <c r="V48"/>
-      <c r="W48"/>
-      <c r="X48"/>
-      <c r="Y48"/>
-      <c r="Z48"/>
-      <c r="AA48"/>
-    </row>
-    <row r="49" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="R48"/>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A49" s="6">
         <v>25000</v>
       </c>
@@ -5939,6 +5212,7 @@
       <c r="E49" s="7">
         <v>2027.6457069999999</v>
       </c>
+      <c r="H49"/>
       <c r="I49"/>
       <c r="J49"/>
       <c r="K49"/>
@@ -5948,19 +5222,9 @@
       <c r="O49"/>
       <c r="P49"/>
       <c r="Q49"/>
-      <c r="S49" s="56" t="s">
-        <v>36</v>
-      </c>
-      <c r="T49" s="56"/>
-      <c r="U49"/>
-      <c r="V49"/>
-      <c r="W49"/>
-      <c r="X49"/>
-      <c r="Y49"/>
-      <c r="Z49"/>
-      <c r="AA49"/>
-    </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="R49"/>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A50" s="6">
         <v>25000</v>
       </c>
@@ -5976,46 +5240,19 @@
       <c r="E50" s="7">
         <v>2193.9721709999999</v>
       </c>
-      <c r="I50" s="55"/>
-      <c r="J50" s="55" t="s">
-        <v>52</v>
-      </c>
-      <c r="K50" s="55" t="s">
-        <v>40</v>
-      </c>
-      <c r="L50" s="55" t="s">
-        <v>53</v>
-      </c>
-      <c r="M50" s="55" t="s">
-        <v>54</v>
-      </c>
-      <c r="N50" s="55" t="s">
-        <v>55</v>
-      </c>
-      <c r="O50" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="P50" s="55" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q50" s="55" t="s">
-        <v>58</v>
-      </c>
-      <c r="S50" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="T50" s="53">
-        <v>0.31593288065638897</v>
-      </c>
-      <c r="U50"/>
-      <c r="V50"/>
-      <c r="W50"/>
-      <c r="X50"/>
-      <c r="Y50"/>
-      <c r="Z50"/>
-      <c r="AA50"/>
-    </row>
-    <row r="51" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="H50"/>
+      <c r="I50"/>
+      <c r="J50"/>
+      <c r="K50"/>
+      <c r="L50"/>
+      <c r="M50"/>
+      <c r="N50"/>
+      <c r="O50"/>
+      <c r="P50"/>
+      <c r="Q50"/>
+      <c r="R50"/>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A51" s="6">
         <v>25000</v>
       </c>
@@ -6031,48 +5268,19 @@
       <c r="E51" s="7">
         <v>2023.3192879999999</v>
       </c>
-      <c r="I51" s="53" t="s">
-        <v>46</v>
-      </c>
-      <c r="J51" s="53">
-        <v>4797363.5304690916</v>
-      </c>
-      <c r="K51" s="53">
-        <v>626447.41705089598</v>
-      </c>
-      <c r="L51" s="53">
-        <v>7.6580466291224694</v>
-      </c>
-      <c r="M51" s="53">
-        <v>6.4388254350216774E-12</v>
-      </c>
-      <c r="N51" s="53">
-        <v>3556491.7626696108</v>
-      </c>
-      <c r="O51" s="53">
-        <v>6038235.2982685724</v>
-      </c>
-      <c r="P51" s="53">
-        <v>3556491.7626696108</v>
-      </c>
-      <c r="Q51" s="53">
-        <v>6038235.2982685724</v>
-      </c>
-      <c r="S51" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="T51" s="58">
-        <v>9.9813585079844128E-2</v>
-      </c>
-      <c r="U51"/>
-      <c r="V51"/>
-      <c r="W51"/>
-      <c r="X51"/>
-      <c r="Y51"/>
-      <c r="Z51"/>
-      <c r="AA51"/>
-    </row>
-    <row r="52" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H51"/>
+      <c r="I51"/>
+      <c r="J51"/>
+      <c r="K51"/>
+      <c r="L51"/>
+      <c r="M51"/>
+      <c r="N51"/>
+      <c r="O51"/>
+      <c r="P51"/>
+      <c r="Q51"/>
+      <c r="R51"/>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A52" s="10">
         <v>30000</v>
       </c>
@@ -6091,48 +5299,19 @@
       <c r="F52" s="13">
         <v>32812</v>
       </c>
-      <c r="I52" s="54" t="s">
-        <v>0</v>
-      </c>
-      <c r="J52" s="54">
-        <v>0.78111521130988426</v>
-      </c>
-      <c r="K52" s="54">
-        <v>14.186240468518623</v>
-      </c>
-      <c r="L52" s="54">
-        <v>5.506146699284388E-2</v>
-      </c>
-      <c r="M52" s="57">
-        <v>0.95618503943494426</v>
-      </c>
-      <c r="N52" s="54">
-        <v>-27.319096888645269</v>
-      </c>
-      <c r="O52" s="54">
-        <v>28.881327311265039</v>
-      </c>
-      <c r="P52" s="54">
-        <v>-27.319096888645269</v>
-      </c>
-      <c r="Q52" s="54">
-        <v>28.881327311265039</v>
-      </c>
-      <c r="S52" s="53" t="s">
-        <v>39</v>
-      </c>
-      <c r="T52" s="53">
-        <v>1.7978456450739054E-2</v>
-      </c>
-      <c r="U52"/>
-      <c r="V52"/>
-      <c r="W52"/>
-      <c r="X52"/>
-      <c r="Y52"/>
-      <c r="Z52"/>
-      <c r="AA52"/>
-    </row>
-    <row r="53" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="H52"/>
+      <c r="I52"/>
+      <c r="J52"/>
+      <c r="K52"/>
+      <c r="L52"/>
+      <c r="M52"/>
+      <c r="N52"/>
+      <c r="O52"/>
+      <c r="P52"/>
+      <c r="Q52"/>
+      <c r="R52"/>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A53" s="14">
         <v>30000</v>
       </c>
@@ -6149,6 +5328,7 @@
         <v>2411.6405949999998</v>
       </c>
       <c r="F53" s="16"/>
+      <c r="H53"/>
       <c r="I53"/>
       <c r="J53"/>
       <c r="K53"/>
@@ -6158,21 +5338,9 @@
       <c r="O53"/>
       <c r="P53"/>
       <c r="Q53"/>
-      <c r="S53" s="53" t="s">
-        <v>40</v>
-      </c>
-      <c r="T53" s="53">
-        <v>21046.232431807952</v>
-      </c>
-      <c r="U53"/>
-      <c r="V53"/>
-      <c r="W53"/>
-      <c r="X53"/>
-      <c r="Y53"/>
-      <c r="Z53"/>
-      <c r="AA53"/>
-    </row>
-    <row r="54" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="R53"/>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A54" s="14">
         <v>30000</v>
       </c>
@@ -6189,6 +5357,7 @@
         <v>1737.125982</v>
       </c>
       <c r="F54" s="16"/>
+      <c r="H54"/>
       <c r="I54"/>
       <c r="J54"/>
       <c r="K54"/>
@@ -6198,21 +5367,9 @@
       <c r="O54"/>
       <c r="P54"/>
       <c r="Q54"/>
-      <c r="S54" s="54" t="s">
-        <v>41</v>
-      </c>
-      <c r="T54" s="54">
-        <v>13</v>
-      </c>
-      <c r="U54"/>
-      <c r="V54"/>
-      <c r="W54"/>
-      <c r="X54"/>
-      <c r="Y54"/>
-      <c r="Z54"/>
-      <c r="AA54"/>
-    </row>
-    <row r="55" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="R54"/>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A55" s="14">
         <v>30000</v>
       </c>
@@ -6229,6 +5386,7 @@
         <v>1281.648874</v>
       </c>
       <c r="F55" s="16"/>
+      <c r="H55"/>
       <c r="I55"/>
       <c r="J55"/>
       <c r="K55"/>
@@ -6238,17 +5396,9 @@
       <c r="O55"/>
       <c r="P55"/>
       <c r="Q55"/>
-      <c r="S55"/>
-      <c r="T55"/>
-      <c r="U55"/>
-      <c r="V55"/>
-      <c r="W55"/>
-      <c r="X55"/>
-      <c r="Y55"/>
-      <c r="Z55"/>
-      <c r="AA55"/>
-    </row>
-    <row r="56" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="R55"/>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A56" s="14">
         <v>30000</v>
       </c>
@@ -6265,19 +5415,19 @@
         <v>1104.569172</v>
       </c>
       <c r="F56" s="16"/>
-      <c r="S56" t="s">
-        <v>42</v>
-      </c>
-      <c r="T56"/>
-      <c r="U56"/>
-      <c r="V56"/>
-      <c r="W56"/>
-      <c r="X56"/>
-      <c r="Y56"/>
-      <c r="Z56"/>
-      <c r="AA56"/>
-    </row>
-    <row r="57" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="H56"/>
+      <c r="I56"/>
+      <c r="J56"/>
+      <c r="K56"/>
+      <c r="L56"/>
+      <c r="M56"/>
+      <c r="N56"/>
+      <c r="O56"/>
+      <c r="P56"/>
+      <c r="Q56"/>
+      <c r="R56"/>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A57" s="14">
         <v>30000</v>
       </c>
@@ -6294,27 +5444,19 @@
         <v>2877.72282</v>
       </c>
       <c r="F57" s="16"/>
-      <c r="S57" s="55"/>
-      <c r="T57" s="55" t="s">
-        <v>47</v>
-      </c>
-      <c r="U57" s="55" t="s">
-        <v>48</v>
-      </c>
-      <c r="V57" s="55" t="s">
-        <v>49</v>
-      </c>
-      <c r="W57" s="55" t="s">
-        <v>50</v>
-      </c>
-      <c r="X57" s="55" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y57"/>
-      <c r="Z57"/>
-      <c r="AA57"/>
-    </row>
-    <row r="58" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="H57"/>
+      <c r="I57"/>
+      <c r="J57"/>
+      <c r="K57"/>
+      <c r="L57"/>
+      <c r="M57"/>
+      <c r="N57"/>
+      <c r="O57"/>
+      <c r="P57"/>
+      <c r="Q57"/>
+      <c r="R57"/>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A58" s="14">
         <v>30000</v>
       </c>
@@ -6331,29 +5473,8 @@
         <v>2028.2156829999999</v>
       </c>
       <c r="F58" s="16"/>
-      <c r="S58" s="53" t="s">
-        <v>43</v>
-      </c>
-      <c r="T58" s="53">
-        <v>1</v>
-      </c>
-      <c r="U58" s="53">
-        <v>540254770.12535381</v>
-      </c>
-      <c r="V58" s="53">
-        <v>540254770.12535381</v>
-      </c>
-      <c r="W58" s="53">
-        <v>1.2196911858258497</v>
-      </c>
-      <c r="X58" s="53">
-        <v>0.2929934913423991</v>
-      </c>
-      <c r="Y58"/>
-      <c r="Z58"/>
-      <c r="AA58"/>
-    </row>
-    <row r="59" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A59" s="14">
         <v>30000</v>
       </c>
@@ -6370,25 +5491,8 @@
         <v>2191.3826800000002</v>
       </c>
       <c r="F59" s="16"/>
-      <c r="S59" s="53" t="s">
-        <v>44</v>
-      </c>
-      <c r="T59" s="53">
-        <v>11</v>
-      </c>
-      <c r="U59" s="53">
-        <v>4872382895.3105335</v>
-      </c>
-      <c r="V59" s="53">
-        <v>442943899.57368487</v>
-      </c>
-      <c r="W59" s="53"/>
-      <c r="X59" s="53"/>
-      <c r="Y59"/>
-      <c r="Z59"/>
-      <c r="AA59"/>
-    </row>
-    <row r="60" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A60" s="17">
         <v>30000</v>
       </c>
@@ -6405,23 +5509,8 @@
         <v>2022.728042</v>
       </c>
       <c r="F60" s="20"/>
-      <c r="S60" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="T60" s="54">
-        <v>12</v>
-      </c>
-      <c r="U60" s="54">
-        <v>5412637665.4358873</v>
-      </c>
-      <c r="V60" s="54"/>
-      <c r="W60" s="54"/>
-      <c r="X60" s="54"/>
-      <c r="Y60"/>
-      <c r="Z60"/>
-      <c r="AA60"/>
-    </row>
-    <row r="61" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A61" s="6">
         <v>35000</v>
       </c>
@@ -6440,17 +5529,8 @@
       <c r="F61" s="2">
         <v>24192</v>
       </c>
-      <c r="S61"/>
-      <c r="T61"/>
-      <c r="U61"/>
-      <c r="V61"/>
-      <c r="W61"/>
-      <c r="X61"/>
-      <c r="Y61"/>
-      <c r="Z61"/>
-      <c r="AA61"/>
-    </row>
-    <row r="62" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A62" s="6">
         <v>35000</v>
       </c>
@@ -6466,33 +5546,8 @@
       <c r="E62" s="7">
         <v>2399.8199709999999</v>
       </c>
-      <c r="S62" s="55"/>
-      <c r="T62" s="55" t="s">
-        <v>52</v>
-      </c>
-      <c r="U62" s="55" t="s">
-        <v>40</v>
-      </c>
-      <c r="V62" s="55" t="s">
-        <v>53</v>
-      </c>
-      <c r="W62" s="55" t="s">
-        <v>54</v>
-      </c>
-      <c r="X62" s="55" t="s">
-        <v>55</v>
-      </c>
-      <c r="Y62" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z62" s="55" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA62" s="55" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="63" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A63" s="6">
         <v>35000</v>
       </c>
@@ -6508,35 +5563,8 @@
       <c r="E63" s="7">
         <v>1727.6481739999999</v>
       </c>
-      <c r="S63" s="53" t="s">
-        <v>46</v>
-      </c>
-      <c r="T63" s="53">
-        <v>53183.51909513335</v>
-      </c>
-      <c r="U63" s="53">
-        <v>13777.993316056352</v>
-      </c>
-      <c r="V63" s="53">
-        <v>3.8600337418624879</v>
-      </c>
-      <c r="W63" s="53">
-        <v>2.6531528598414261E-3</v>
-      </c>
-      <c r="X63" s="53">
-        <v>22858.360270651538</v>
-      </c>
-      <c r="Y63" s="53">
-        <v>83508.677919615162</v>
-      </c>
-      <c r="Z63" s="53">
-        <v>22858.360270651538</v>
-      </c>
-      <c r="AA63" s="53">
-        <v>83508.677919615162</v>
-      </c>
-    </row>
-    <row r="64" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A64" s="6">
         <v>35000</v>
       </c>
@@ -6552,35 +5580,8 @@
       <c r="E64" s="7">
         <v>1283.1558379999999</v>
       </c>
-      <c r="S64" s="54" t="s">
-        <v>0</v>
-      </c>
-      <c r="T64" s="54">
-        <v>-0.3445828087926936</v>
-      </c>
-      <c r="U64" s="54">
-        <v>0.31201010816736702</v>
-      </c>
-      <c r="V64" s="54">
-        <v>-1.1043962992630165</v>
-      </c>
-      <c r="W64" s="57">
-        <v>0.29299349134239949</v>
-      </c>
-      <c r="X64" s="54">
-        <v>-1.0313124266676552</v>
-      </c>
-      <c r="Y64" s="54">
-        <v>0.34214680908226808</v>
-      </c>
-      <c r="Z64" s="54">
-        <v>-1.0313124266676552</v>
-      </c>
-      <c r="AA64" s="54">
-        <v>0.34214680908226808</v>
-      </c>
-    </row>
-    <row r="65" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" s="6">
         <v>35000</v>
       </c>
@@ -6596,17 +5597,8 @@
       <c r="E65" s="7">
         <v>1101.031463</v>
       </c>
-      <c r="S65"/>
-      <c r="T65"/>
-      <c r="U65"/>
-      <c r="V65"/>
-      <c r="W65"/>
-      <c r="X65"/>
-      <c r="Y65"/>
-      <c r="Z65"/>
-      <c r="AA65"/>
-    </row>
-    <row r="66" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" s="6">
         <v>35000</v>
       </c>
@@ -6622,17 +5614,8 @@
       <c r="E66" s="7">
         <v>2857.0905779999998</v>
       </c>
-      <c r="S66"/>
-      <c r="T66"/>
-      <c r="U66"/>
-      <c r="V66"/>
-      <c r="W66"/>
-      <c r="X66"/>
-      <c r="Y66"/>
-      <c r="Z66"/>
-      <c r="AA66"/>
-    </row>
-    <row r="67" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" s="6">
         <v>35000</v>
       </c>
@@ -6648,17 +5631,8 @@
       <c r="E67" s="7">
         <v>2018.5626970000001</v>
       </c>
-      <c r="S67"/>
-      <c r="T67"/>
-      <c r="U67"/>
-      <c r="V67"/>
-      <c r="W67"/>
-      <c r="X67"/>
-      <c r="Y67"/>
-      <c r="Z67"/>
-      <c r="AA67"/>
-    </row>
-    <row r="68" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" s="6">
         <v>35000</v>
       </c>
@@ -6675,7 +5649,7 @@
         <v>2196.5717930000001</v>
       </c>
     </row>
-    <row r="69" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" s="6">
         <v>35000</v>
       </c>
@@ -6692,7 +5666,7 @@
         <v>2029.087043</v>
       </c>
     </row>
-    <row r="70" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" s="10">
         <v>40000</v>
       </c>
@@ -6712,7 +5686,7 @@
         <v>34977</v>
       </c>
     </row>
-    <row r="71" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" s="14">
         <v>40000</v>
       </c>
@@ -6730,7 +5704,7 @@
       </c>
       <c r="F71" s="16"/>
     </row>
-    <row r="72" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" s="14">
         <v>40000</v>
       </c>
@@ -6748,7 +5722,7 @@
       </c>
       <c r="F72" s="16"/>
     </row>
-    <row r="73" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" s="14">
         <v>40000</v>
       </c>
@@ -6766,7 +5740,7 @@
       </c>
       <c r="F73" s="16"/>
     </row>
-    <row r="74" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" s="14">
         <v>40000</v>
       </c>
@@ -6784,7 +5758,7 @@
       </c>
       <c r="F74" s="16"/>
     </row>
-    <row r="75" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" s="14">
         <v>40000</v>
       </c>
@@ -6802,7 +5776,7 @@
       </c>
       <c r="F75" s="16"/>
     </row>
-    <row r="76" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" s="14">
         <v>40000</v>
       </c>
@@ -6820,7 +5794,7 @@
       </c>
       <c r="F76" s="16"/>
     </row>
-    <row r="77" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" s="14">
         <v>40000</v>
       </c>
@@ -6838,7 +5812,7 @@
       </c>
       <c r="F77" s="16"/>
     </row>
-    <row r="78" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" s="17">
         <v>40000</v>
       </c>
@@ -6856,7 +5830,7 @@
       </c>
       <c r="F78" s="20"/>
     </row>
-    <row r="79" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79" s="14">
         <v>45000</v>
       </c>
@@ -6876,7 +5850,7 @@
         <v>42096</v>
       </c>
     </row>
-    <row r="80" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" s="14">
         <v>45000</v>
       </c>
@@ -8270,8 +7244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07E2FAA7-AF33-4595-8B19-D05C042724E7}">
   <dimension ref="A1:P357"/>
   <sheetViews>
-    <sheetView zoomScale="86" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView zoomScale="44" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Changing the formula of Average calculation
</commit_message>
<xml_diff>
--- a/simulation_check.xlsx
+++ b/simulation_check.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\C-Final-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\GitHub\C++_Final_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38364B56-965D-4B40-B9F5-12012F6AD34B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20AC039F-1E3C-4DB2-8830-DA70BF9A3F81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{603FAE4F-A0F0-414C-B275-6F2A5451B931}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{603FAE4F-A0F0-414C-B275-6F2A5451B931}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="4" r:id="rId1"/>
@@ -158,9 +158,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -459,11 +459,11 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -473,69 +473,69 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
@@ -543,36 +543,41 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -585,11 +590,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -907,8 +907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95A1AEA0-ADDF-4578-9565-5DEA63143E1E}">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -963,9 +963,9 @@
       <c r="J2" s="6">
         <v>10000</v>
       </c>
-      <c r="K2" s="51">
-        <f>AVERAGE(SUM(simulations_small!J3:O3),SUM(simulations_medium!J3:O3),SUM(simulations_large!J3:O3))</f>
-        <v>5212062565.6701403</v>
+      <c r="K2" s="47">
+        <f>AVERAGE(SUM(simulations_small!M3:O3),SUM(simulations_medium!M3:O3),SUM(simulations_large!M3:O3))</f>
+        <v>5212055330.3555641</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
@@ -996,13 +996,13 @@
       <c r="J3" s="6">
         <v>15000</v>
       </c>
-      <c r="K3" s="51">
-        <f>AVERAGE(SUM(simulations_small!J4:O4),SUM(simulations_medium!J4:O4),SUM(simulations_large!J4:O4))</f>
-        <v>4645014919.1168776</v>
-      </c>
-      <c r="N3" s="52">
+      <c r="K3" s="47">
+        <f>AVERAGE(SUM(simulations_small!M4:O4),SUM(simulations_medium!M4:O4),SUM(simulations_large!M4:O4))</f>
+        <v>4645007633.29638</v>
+      </c>
+      <c r="N3" s="48">
         <f>MIN(K2:K14)</f>
-        <v>595670805.00217485</v>
+        <v>595663988.86136937</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
@@ -1036,27 +1036,27 @@
       <c r="J4" s="8">
         <v>20000</v>
       </c>
-      <c r="K4" s="51">
-        <f>AVERAGE(SUM(simulations_small!J5:O5),SUM(simulations_medium!J5:O5),SUM(simulations_large!J5:O5))</f>
-        <v>2112046735.8288171</v>
+      <c r="K4" s="47">
+        <f>AVERAGE(SUM(simulations_small!M5:O5),SUM(simulations_medium!M5:O5),SUM(simulations_large!M5:O5))</f>
+        <v>2112039822.6323636</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="J5" s="6">
         <v>25000</v>
       </c>
-      <c r="K5" s="51">
-        <f>AVERAGE(SUM(simulations_small!J6:O6),SUM(simulations_medium!J6:O6),SUM(simulations_large!J6:O6))</f>
-        <v>838532812.54558706</v>
+      <c r="K5" s="47">
+        <f>AVERAGE(SUM(simulations_small!M6:O6),SUM(simulations_medium!M6:O6),SUM(simulations_large!M6:O6))</f>
+        <v>838526026.82951367</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="J6" s="8">
         <v>30000</v>
       </c>
-      <c r="K6" s="51">
-        <f>AVERAGE(SUM(simulations_small!J7:O7),SUM(simulations_medium!J7:O7),SUM(simulations_large!J7:O7))</f>
-        <v>1874579049.9885066</v>
+      <c r="K6" s="47">
+        <f>AVERAGE(SUM(simulations_small!M7:O7),SUM(simulations_medium!M7:O7),SUM(simulations_large!M7:O7))</f>
+        <v>1874572191.5957472</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
@@ -1066,9 +1066,9 @@
       <c r="J7" s="6">
         <v>35000</v>
       </c>
-      <c r="K7" s="51">
-        <f>AVERAGE(SUM(simulations_small!J8:O8),SUM(simulations_medium!J8:O8),SUM(simulations_large!J8:O8))</f>
-        <v>2955241424.4473481</v>
+      <c r="K7" s="47">
+        <f>AVERAGE(SUM(simulations_small!M8:O8),SUM(simulations_medium!M8:O8),SUM(simulations_large!M8:O8))</f>
+        <v>2955234339.5841203</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
@@ -1099,9 +1099,9 @@
       <c r="J8" s="6">
         <v>40000</v>
       </c>
-      <c r="K8" s="51">
-        <f>AVERAGE(SUM(simulations_small!J9:O9),SUM(simulations_medium!J9:O9),SUM(simulations_large!J9:O9))</f>
-        <v>5700964115.570241</v>
+      <c r="K8" s="47">
+        <f>AVERAGE(SUM(simulations_small!M9:O9),SUM(simulations_medium!M9:O9),SUM(simulations_large!M9:O9))</f>
+        <v>5700956947.7433271</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
@@ -1132,9 +1132,9 @@
       <c r="J9" s="6">
         <v>45000</v>
       </c>
-      <c r="K9" s="51">
-        <f>AVERAGE(SUM(simulations_small!J10:O10),SUM(simulations_medium!J10:O10),SUM(simulations_large!J10:O10))</f>
-        <v>1585962507.4009333</v>
+      <c r="K9" s="47">
+        <f>AVERAGE(SUM(simulations_small!M10:O10),SUM(simulations_medium!M10:O10),SUM(simulations_large!M10:O10))</f>
+        <v>1585955150.0458393</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
@@ -1168,27 +1168,27 @@
       <c r="J10" s="9">
         <v>50000</v>
       </c>
-      <c r="K10" s="52">
-        <f>AVERAGE(SUM(simulations_small!J11:O11),SUM(simulations_medium!J11:O11),SUM(simulations_large!J11:O11))</f>
-        <v>595670805.00217485</v>
+      <c r="K10" s="48">
+        <f>AVERAGE(SUM(simulations_small!M11:O11),SUM(simulations_medium!M11:O11),SUM(simulations_large!M11:O11))</f>
+        <v>595663988.86136937</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="J11" s="8">
         <v>55000</v>
       </c>
-      <c r="K11" s="51">
-        <f>AVERAGE(SUM(simulations_small!J12:O12),SUM(simulations_medium!J12:O12),SUM(simulations_large!J12:O12))</f>
-        <v>2321312078.2334747</v>
+      <c r="K11" s="47">
+        <f>AVERAGE(SUM(simulations_small!M12:O12),SUM(simulations_medium!M12:O12),SUM(simulations_large!M12:O12))</f>
+        <v>2321305185.002944</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="J12" s="6">
         <v>60000</v>
       </c>
-      <c r="K12" s="51">
-        <f>AVERAGE(SUM(simulations_small!J13:O13),SUM(simulations_medium!J13:O13),SUM(simulations_large!J13:O13))</f>
-        <v>2269874745.8999739</v>
+      <c r="K12" s="47">
+        <f>AVERAGE(SUM(simulations_small!M13:O13),SUM(simulations_medium!M13:O13),SUM(simulations_large!M13:O13))</f>
+        <v>2269867824.6664844</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
@@ -1198,9 +1198,9 @@
       <c r="J13" s="6">
         <v>65000</v>
       </c>
-      <c r="K13" s="51">
-        <f>AVERAGE(SUM(simulations_small!J14:O14),SUM(simulations_medium!J14:O14),SUM(simulations_large!J14:O14))</f>
-        <v>2446875316.0901127</v>
+      <c r="K13" s="47">
+        <f>AVERAGE(SUM(simulations_small!M14:O14),SUM(simulations_medium!M14:O14),SUM(simulations_large!M14:O14))</f>
+        <v>2446868182.972899</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
@@ -1231,9 +1231,9 @@
       <c r="J14" s="6">
         <v>70000</v>
       </c>
-      <c r="K14" s="51">
-        <f>AVERAGE(SUM(simulations_small!J15:O15),SUM(simulations_medium!J15:O15),SUM(simulations_large!J15:O15))</f>
-        <v>688144121.45951807</v>
+      <c r="K14" s="47">
+        <f>AVERAGE(SUM(simulations_small!M15:O15),SUM(simulations_medium!M15:O15),SUM(simulations_large!M15:O15))</f>
+        <v>688137236.06868434</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
@@ -1301,8 +1301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{544FD0B2-A7ED-4478-8092-5F67F619DD9A}">
   <dimension ref="A1:S64"/>
   <sheetViews>
-    <sheetView topLeftCell="B11" zoomScale="72" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:I15"/>
+    <sheetView topLeftCell="B1" zoomScale="72" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1326,13 +1326,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
@@ -1709,14 +1709,14 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A11" s="48" t="s">
+      <c r="A11" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="49"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="50"/>
+      <c r="B11" s="54"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="55"/>
       <c r="I11" s="6">
         <v>50000</v>
       </c>
@@ -3613,7 +3613,7 @@
   <dimension ref="A1:R132"/>
   <sheetViews>
     <sheetView topLeftCell="E1" zoomScale="54" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18:L31"/>
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3640,13 +3640,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
@@ -4197,14 +4197,14 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A14" s="48" t="s">
+      <c r="A14" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="49"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="50"/>
+      <c r="B14" s="54"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="54"/>
+      <c r="F14" s="55"/>
       <c r="I14" s="8">
         <v>65000</v>
       </c>
@@ -7247,8 +7247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07E2FAA7-AF33-4595-8B19-D05C042724E7}">
   <dimension ref="A1:P357"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="82" workbookViewId="0">
-      <selection activeCell="F333" sqref="F333"/>
+    <sheetView zoomScale="82" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8176,14 +8176,14 @@
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A31" s="48" t="s">
+      <c r="A31" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="49"/>
-      <c r="C31" s="49"/>
-      <c r="D31" s="49"/>
-      <c r="E31" s="49"/>
-      <c r="F31" s="50"/>
+      <c r="B31" s="54"/>
+      <c r="C31" s="54"/>
+      <c r="D31" s="54"/>
+      <c r="E31" s="54"/>
+      <c r="F31" s="55"/>
       <c r="K31" s="6">
         <v>70000</v>
       </c>
@@ -8219,13 +8219,13 @@
       <c r="B33" s="32">
         <v>1</v>
       </c>
-      <c r="C33" s="54">
+      <c r="C33" s="50">
         <v>3109.353975</v>
       </c>
-      <c r="D33" s="54">
+      <c r="D33" s="50">
         <v>10751363.301992999</v>
       </c>
-      <c r="E33" s="54">
+      <c r="E33" s="50">
         <v>3278.9271570000001</v>
       </c>
       <c r="F33" s="33">
@@ -8653,13 +8653,13 @@
       <c r="B57" s="37">
         <v>25</v>
       </c>
-      <c r="C57" s="55">
+      <c r="C57" s="51">
         <v>14800.385935</v>
       </c>
-      <c r="D57" s="55">
+      <c r="D57" s="51">
         <v>4082713.1555440002</v>
       </c>
-      <c r="E57" s="55">
+      <c r="E57" s="51">
         <v>2020.572482</v>
       </c>
       <c r="F57" s="38"/>
@@ -9099,13 +9099,13 @@
       <c r="B83" s="32">
         <v>1</v>
       </c>
-      <c r="C83" s="54">
+      <c r="C83" s="50">
         <v>3071.014408</v>
       </c>
-      <c r="D83" s="54">
+      <c r="D83" s="50">
         <v>10764645.165635999</v>
       </c>
-      <c r="E83" s="54">
+      <c r="E83" s="50">
         <v>3280.951869</v>
       </c>
       <c r="F83" s="33">
@@ -9533,13 +9533,13 @@
       <c r="B107" s="37">
         <v>25</v>
       </c>
-      <c r="C107" s="55">
+      <c r="C107" s="51">
         <v>14809.715630999999</v>
       </c>
-      <c r="D107" s="55">
+      <c r="D107" s="51">
         <v>4201622.0101349996</v>
       </c>
-      <c r="E107" s="55">
+      <c r="E107" s="51">
         <v>2049.7858449999999</v>
       </c>
       <c r="F107" s="38"/>
@@ -9979,13 +9979,13 @@
       <c r="B133" s="32">
         <v>1</v>
       </c>
-      <c r="C133" s="54">
+      <c r="C133" s="50">
         <v>3106.8163669999999</v>
       </c>
-      <c r="D133" s="54">
+      <c r="D133" s="50">
         <v>10703096.314175</v>
       </c>
-      <c r="E133" s="54">
+      <c r="E133" s="50">
         <v>3271.5586979999998</v>
       </c>
       <c r="F133" s="33">
@@ -10413,13 +10413,13 @@
       <c r="B157" s="37">
         <v>25</v>
       </c>
-      <c r="C157" s="55">
+      <c r="C157" s="51">
         <v>14811.738169</v>
       </c>
-      <c r="D157" s="55">
+      <c r="D157" s="51">
         <v>4165925.8051479999</v>
       </c>
-      <c r="E157" s="55">
+      <c r="E157" s="51">
         <v>2041.0599709999999</v>
       </c>
       <c r="F157" s="38"/>
@@ -10859,13 +10859,13 @@
       <c r="B183" s="32">
         <v>1</v>
       </c>
-      <c r="C183" s="54">
+      <c r="C183" s="50">
         <v>3105.4071330000002</v>
       </c>
-      <c r="D183" s="54">
+      <c r="D183" s="50">
         <v>10891229.301669</v>
       </c>
-      <c r="E183" s="54">
+      <c r="E183" s="50">
         <v>3300.1862529999999</v>
       </c>
       <c r="F183" s="33">
@@ -11293,13 +11293,13 @@
       <c r="B207" s="37">
         <v>25</v>
       </c>
-      <c r="C207" s="55">
+      <c r="C207" s="51">
         <v>14777.254542999999</v>
       </c>
-      <c r="D207" s="55">
+      <c r="D207" s="51">
         <v>4065776.4732889999</v>
       </c>
-      <c r="E207" s="55">
+      <c r="E207" s="51">
         <v>2016.377066</v>
       </c>
       <c r="F207" s="38"/>
@@ -11739,16 +11739,16 @@
       <c r="B233" s="32">
         <v>1</v>
       </c>
-      <c r="C233" s="54">
+      <c r="C233" s="50">
         <v>3109.812872</v>
       </c>
-      <c r="D233" s="54">
+      <c r="D233" s="50">
         <v>10499386.834208</v>
       </c>
-      <c r="E233" s="54">
+      <c r="E233" s="50">
         <v>3240.2757339999998</v>
       </c>
-      <c r="F233" s="53">
+      <c r="F233" s="49">
         <v>235408</v>
       </c>
       <c r="G233" s="43"/>
@@ -12174,13 +12174,13 @@
       <c r="B257" s="37">
         <v>25</v>
       </c>
-      <c r="C257" s="55">
+      <c r="C257" s="51">
         <v>14815.369366999999</v>
       </c>
-      <c r="D257" s="55">
+      <c r="D257" s="51">
         <v>4104781.4520820002</v>
       </c>
-      <c r="E257" s="55">
+      <c r="E257" s="51">
         <v>2026.0260249999999</v>
       </c>
       <c r="F257" s="38"/>
@@ -12620,13 +12620,13 @@
       <c r="B283" s="32">
         <v>1</v>
       </c>
-      <c r="C283" s="54">
+      <c r="C283" s="50">
         <v>3083.7531119999999</v>
       </c>
-      <c r="D283" s="54">
+      <c r="D283" s="50">
         <v>10418957.66835</v>
       </c>
-      <c r="E283" s="54">
+      <c r="E283" s="50">
         <v>3227.841023</v>
       </c>
       <c r="F283" s="33">
@@ -13054,13 +13054,13 @@
       <c r="B307" s="37">
         <v>25</v>
       </c>
-      <c r="C307" s="55">
+      <c r="C307" s="51">
         <v>14798.855186000001</v>
       </c>
-      <c r="D307" s="55">
+      <c r="D307" s="51">
         <v>4025539.5519019999</v>
       </c>
-      <c r="E307" s="55">
+      <c r="E307" s="51">
         <v>2006.3747289999999</v>
       </c>
       <c r="F307" s="38"/>
@@ -13500,13 +13500,13 @@
       <c r="B333" s="32">
         <v>1</v>
       </c>
-      <c r="C333" s="54">
+      <c r="C333" s="50">
         <v>3077.6002079999998</v>
       </c>
-      <c r="D333" s="54">
+      <c r="D333" s="50">
         <v>10632106.511628</v>
       </c>
-      <c r="E333" s="54">
+      <c r="E333" s="50">
         <v>3260.6911100000002</v>
       </c>
       <c r="F333" s="33">
@@ -13934,13 +13934,13 @@
       <c r="B357" s="37">
         <v>25</v>
       </c>
-      <c r="C357" s="55">
+      <c r="C357" s="51">
         <v>14805.626915000001</v>
       </c>
-      <c r="D357" s="55">
+      <c r="D357" s="51">
         <v>4105543.2465090002</v>
       </c>
-      <c r="E357" s="55">
+      <c r="E357" s="51">
         <v>2026.2140179999999</v>
       </c>
       <c r="F357" s="38"/>

</xml_diff>

<commit_message>
correction to the runtime to make same type for all s/m/l
</commit_message>
<xml_diff>
--- a/simulation_check.xlsx
+++ b/simulation_check.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\GitHub\C++_Final_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20AC039F-1E3C-4DB2-8830-DA70BF9A3F81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8582E5F6-5A2C-42A4-BCFF-E682BF405688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{603FAE4F-A0F0-414C-B275-6F2A5451B931}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{603FAE4F-A0F0-414C-B275-6F2A5451B931}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="4" r:id="rId1"/>
@@ -907,7 +907,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95A1AEA0-ADDF-4578-9565-5DEA63143E1E}">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
@@ -1301,8 +1301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{544FD0B2-A7ED-4478-8092-5F67F619DD9A}">
   <dimension ref="A1:S64"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="72" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="72" workbookViewId="0">
+      <selection activeCell="K58" sqref="K58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1867,9 +1867,7 @@
       <c r="E14" s="15">
         <v>956.84260500000005</v>
       </c>
-      <c r="F14" s="16">
-        <v>2284</v>
-      </c>
+      <c r="F14" s="16"/>
       <c r="I14" s="6">
         <v>65000</v>
       </c>
@@ -1918,9 +1916,7 @@
       <c r="E15" s="15">
         <v>1060.5067240000001</v>
       </c>
-      <c r="F15" s="16">
-        <v>2284</v>
-      </c>
+      <c r="F15" s="16"/>
       <c r="I15" s="6">
         <v>70000</v>
       </c>
@@ -1969,9 +1965,7 @@
       <c r="E16" s="19">
         <v>0</v>
       </c>
-      <c r="F16" s="20">
-        <v>2284</v>
-      </c>
+      <c r="F16" s="20"/>
       <c r="I16" s="6"/>
       <c r="P16" s="6">
         <f t="shared" si="2"/>
@@ -2019,9 +2013,6 @@
       <c r="E18" s="7">
         <v>955.42025000000001</v>
       </c>
-      <c r="F18" s="2">
-        <v>3884</v>
-      </c>
       <c r="I18" s="6"/>
       <c r="K18" s="2" t="s">
         <v>34</v>
@@ -2047,9 +2038,6 @@
       <c r="E19" s="7">
         <v>1070.8456739999999</v>
       </c>
-      <c r="F19" s="2">
-        <v>3884</v>
-      </c>
       <c r="I19" s="6"/>
       <c r="K19" s="8">
         <v>10000</v>
@@ -2079,9 +2067,6 @@
       <c r="E20" s="7">
         <v>0</v>
       </c>
-      <c r="F20" s="2">
-        <v>3884</v>
-      </c>
       <c r="I20" s="6"/>
       <c r="K20" s="8">
         <v>15000</v>
@@ -2138,9 +2123,7 @@
       <c r="E22" s="22">
         <v>957.96374200000002</v>
       </c>
-      <c r="F22" s="16">
-        <v>6970</v>
-      </c>
+      <c r="F22" s="16"/>
       <c r="K22" s="8">
         <v>25000</v>
       </c>
@@ -2165,9 +2148,7 @@
       <c r="E23" s="22">
         <v>1061.8034250000001</v>
       </c>
-      <c r="F23" s="16">
-        <v>6970</v>
-      </c>
+      <c r="F23" s="16"/>
       <c r="K23" s="8">
         <v>30000</v>
       </c>
@@ -2192,9 +2173,7 @@
       <c r="E24" s="23">
         <v>0</v>
       </c>
-      <c r="F24" s="20">
-        <v>6970</v>
-      </c>
+      <c r="F24" s="20"/>
       <c r="K24" s="8">
         <v>35000</v>
       </c>
@@ -2246,9 +2225,6 @@
       <c r="E26" s="7">
         <v>960.78185599999995</v>
       </c>
-      <c r="F26" s="2">
-        <v>8343</v>
-      </c>
       <c r="K26" s="8">
         <v>45000</v>
       </c>
@@ -2273,9 +2249,6 @@
       <c r="E27" s="7">
         <v>1069.885413</v>
       </c>
-      <c r="F27" s="2">
-        <v>8343</v>
-      </c>
       <c r="K27" s="8">
         <v>50000</v>
       </c>
@@ -2300,9 +2273,6 @@
       <c r="E28" s="7">
         <v>0</v>
       </c>
-      <c r="F28" s="2">
-        <v>8343</v>
-      </c>
       <c r="K28" s="8">
         <v>55000</v>
       </c>
@@ -2354,9 +2324,7 @@
       <c r="E30" s="15">
         <v>954.08429100000001</v>
       </c>
-      <c r="F30" s="16">
-        <v>9428</v>
-      </c>
+      <c r="F30" s="16"/>
       <c r="K30" s="8">
         <v>65000</v>
       </c>
@@ -2381,9 +2349,7 @@
       <c r="E31" s="15">
         <v>1067.560334</v>
       </c>
-      <c r="F31" s="16">
-        <v>9428</v>
-      </c>
+      <c r="F31" s="16"/>
       <c r="K31" s="6">
         <v>70000</v>
       </c>
@@ -2408,9 +2374,7 @@
       <c r="E32" s="19">
         <v>0</v>
       </c>
-      <c r="F32" s="20">
-        <v>9428</v>
-      </c>
+      <c r="F32" s="20"/>
       <c r="I32"/>
       <c r="J32"/>
       <c r="K32"/>
@@ -2470,9 +2434,6 @@
       <c r="E34" s="7">
         <v>952.679169</v>
       </c>
-      <c r="F34" s="2">
-        <v>10111</v>
-      </c>
       <c r="I34"/>
       <c r="J34"/>
       <c r="K34"/>
@@ -2501,9 +2462,6 @@
       <c r="E35" s="7">
         <v>1065.333322</v>
       </c>
-      <c r="F35" s="2">
-        <v>10111</v>
-      </c>
       <c r="I35"/>
       <c r="J35"/>
       <c r="K35"/>
@@ -2532,9 +2490,6 @@
       <c r="E36" s="7">
         <v>0</v>
       </c>
-      <c r="F36" s="2">
-        <v>10111</v>
-      </c>
       <c r="I36"/>
       <c r="J36"/>
       <c r="K36"/>
@@ -2594,9 +2549,7 @@
       <c r="E38" s="15">
         <v>954.06686200000001</v>
       </c>
-      <c r="F38" s="16">
-        <v>13979</v>
-      </c>
+      <c r="F38" s="16"/>
       <c r="I38"/>
       <c r="J38"/>
       <c r="K38"/>
@@ -2625,9 +2578,7 @@
       <c r="E39" s="15">
         <v>1065.448815</v>
       </c>
-      <c r="F39" s="16">
-        <v>13979</v>
-      </c>
+      <c r="F39" s="16"/>
       <c r="I39"/>
       <c r="J39"/>
       <c r="K39"/>
@@ -2656,9 +2607,7 @@
       <c r="E40" s="19">
         <v>0</v>
       </c>
-      <c r="F40" s="20">
-        <v>13979</v>
-      </c>
+      <c r="F40" s="20"/>
       <c r="I40"/>
       <c r="J40"/>
       <c r="K40"/>
@@ -2718,9 +2667,6 @@
       <c r="E42" s="15">
         <v>959.33007699999996</v>
       </c>
-      <c r="F42" s="2">
-        <v>15291</v>
-      </c>
       <c r="I42"/>
       <c r="J42"/>
       <c r="K42"/>
@@ -2749,9 +2695,6 @@
       <c r="E43" s="15">
         <v>1059.0502819999999</v>
       </c>
-      <c r="F43" s="2">
-        <v>15291</v>
-      </c>
       <c r="I43"/>
       <c r="J43"/>
       <c r="K43"/>
@@ -2780,9 +2723,6 @@
       <c r="E44" s="15">
         <v>0</v>
       </c>
-      <c r="F44" s="2">
-        <v>15291</v>
-      </c>
       <c r="I44"/>
       <c r="J44"/>
       <c r="K44"/>
@@ -2842,9 +2782,7 @@
       <c r="E46" s="15">
         <v>953.94431999999995</v>
       </c>
-      <c r="F46" s="16">
-        <v>17538</v>
-      </c>
+      <c r="F46" s="16"/>
       <c r="I46"/>
       <c r="J46"/>
       <c r="K46"/>
@@ -2873,9 +2811,7 @@
       <c r="E47" s="15">
         <v>1068.110713</v>
       </c>
-      <c r="F47" s="16">
-        <v>17538</v>
-      </c>
+      <c r="F47" s="16"/>
       <c r="I47"/>
       <c r="J47"/>
       <c r="K47"/>
@@ -2904,9 +2840,7 @@
       <c r="E48" s="19">
         <v>0</v>
       </c>
-      <c r="F48" s="20">
-        <v>17538</v>
-      </c>
+      <c r="F48" s="20"/>
       <c r="I48"/>
       <c r="J48"/>
       <c r="K48"/>
@@ -2966,9 +2900,6 @@
       <c r="E50" s="15">
         <v>955.40336000000002</v>
       </c>
-      <c r="F50" s="2">
-        <v>20935</v>
-      </c>
       <c r="I50"/>
       <c r="J50"/>
       <c r="K50"/>
@@ -2997,9 +2928,6 @@
       <c r="E51" s="15">
         <v>1066.0621020000001</v>
       </c>
-      <c r="F51" s="2">
-        <v>20935</v>
-      </c>
       <c r="I51"/>
       <c r="J51"/>
       <c r="K51"/>
@@ -3028,9 +2956,6 @@
       <c r="E52" s="15">
         <v>0</v>
       </c>
-      <c r="F52" s="2">
-        <v>20935</v>
-      </c>
       <c r="I52"/>
       <c r="J52"/>
       <c r="K52"/>
@@ -3090,9 +3015,7 @@
       <c r="E54" s="15">
         <v>953.03556000000003</v>
       </c>
-      <c r="F54" s="16">
-        <v>20938</v>
-      </c>
+      <c r="F54" s="16"/>
       <c r="J54"/>
       <c r="K54"/>
       <c r="L54"/>
@@ -3119,9 +3042,7 @@
       <c r="E55" s="15">
         <v>1067.5580729999999</v>
       </c>
-      <c r="F55" s="16">
-        <v>20938</v>
-      </c>
+      <c r="F55" s="16"/>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A56" s="17">
@@ -3139,9 +3060,7 @@
       <c r="E56" s="19">
         <v>0</v>
       </c>
-      <c r="F56" s="20">
-        <v>20938</v>
-      </c>
+      <c r="F56" s="20"/>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A57" s="22">
@@ -3179,9 +3098,6 @@
       <c r="E58" s="15">
         <v>952.55669399999999</v>
       </c>
-      <c r="F58" s="2">
-        <v>24465</v>
-      </c>
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A59" s="22">
@@ -3199,9 +3115,6 @@
       <c r="E59" s="15">
         <v>1065.004291</v>
       </c>
-      <c r="F59" s="2">
-        <v>24465</v>
-      </c>
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A60" s="22">
@@ -3219,9 +3132,6 @@
       <c r="E60" s="15">
         <v>0</v>
       </c>
-      <c r="F60" s="2">
-        <v>24465</v>
-      </c>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A61" s="10">
@@ -3259,9 +3169,7 @@
       <c r="E62" s="15">
         <v>955.281612</v>
       </c>
-      <c r="F62" s="16">
-        <v>25274</v>
-      </c>
+      <c r="F62" s="16"/>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A63" s="14">
@@ -3279,9 +3187,7 @@
       <c r="E63" s="15">
         <v>1060.259544</v>
       </c>
-      <c r="F63" s="16">
-        <v>25274</v>
-      </c>
+      <c r="F63" s="16"/>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A64" s="17">
@@ -3299,9 +3205,7 @@
       <c r="E64" s="19">
         <v>0</v>
       </c>
-      <c r="F64" s="20">
-        <v>25274</v>
-      </c>
+      <c r="F64" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3612,7 +3516,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32199EA4-1B1E-4F05-B93A-A4002D945EFC}">
   <dimension ref="A1:R132"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="54" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="54" workbookViewId="0">
       <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
@@ -7247,7 +7151,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07E2FAA7-AF33-4595-8B19-D05C042724E7}">
   <dimension ref="A1:P357"/>
   <sheetViews>
-    <sheetView zoomScale="82" workbookViewId="0">
+    <sheetView topLeftCell="A52" zoomScale="82" workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
model test is done
</commit_message>
<xml_diff>
--- a/simulation_check.xlsx
+++ b/simulation_check.xlsx
@@ -8,18 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\GitHub\C++_Final_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8582E5F6-5A2C-42A4-BCFF-E682BF405688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA2B5A7-04E8-405F-B0ED-B403F06516AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{603FAE4F-A0F0-414C-B275-6F2A5451B931}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="6" activeTab="7" xr2:uid="{603FAE4F-A0F0-414C-B275-6F2A5451B931}"/>
   </bookViews>
   <sheets>
-    <sheet name="Summary" sheetId="4" r:id="rId1"/>
-    <sheet name="simulations_small" sheetId="1" r:id="rId2"/>
+    <sheet name="training summary" sheetId="4" r:id="rId1"/>
+    <sheet name="training_small" sheetId="1" r:id="rId2"/>
     <sheet name="output_small_th" sheetId="3" state="hidden" r:id="rId3"/>
-    <sheet name="simulations_medium" sheetId="7" r:id="rId4"/>
+    <sheet name="training_medium" sheetId="7" r:id="rId4"/>
     <sheet name="output_medium_th" sheetId="8" state="hidden" r:id="rId5"/>
-    <sheet name="simulations_large" sheetId="5" r:id="rId6"/>
-    <sheet name="output_large_th" sheetId="6" state="hidden" r:id="rId7"/>
+    <sheet name="training_large" sheetId="5" r:id="rId6"/>
+    <sheet name="test_1" sheetId="9" r:id="rId7"/>
+    <sheet name="test_2" sheetId="10" r:id="rId8"/>
+    <sheet name="test_3" sheetId="11" r:id="rId9"/>
+    <sheet name="output_large_th" sheetId="6" state="hidden" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="37">
   <si>
     <t>simulation #</t>
   </si>
@@ -461,7 +464,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -589,6 +592,21 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -908,7 +926,7 @@
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -937,67 +955,67 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B2" s="26" t="str">
-        <f>simulations_small!J2</f>
+        <f>training_small!J2</f>
         <v>MAE_mean</v>
       </c>
       <c r="C2" s="26" t="str">
-        <f>simulations_small!K2</f>
+        <f>training_small!K2</f>
         <v>MSE_mean</v>
       </c>
       <c r="D2" s="26" t="str">
-        <f>simulations_small!L2</f>
+        <f>training_small!L2</f>
         <v>RMSE_mean</v>
       </c>
       <c r="E2" s="26" t="str">
-        <f>simulations_small!M2</f>
+        <f>training_small!M2</f>
         <v>MAE_Var</v>
       </c>
       <c r="F2" s="26" t="str">
-        <f>simulations_small!N2</f>
+        <f>training_small!N2</f>
         <v>MSE_var</v>
       </c>
       <c r="G2" s="26" t="str">
-        <f>simulations_small!O2</f>
+        <f>training_small!O2</f>
         <v>RMSE_var</v>
       </c>
       <c r="J2" s="6">
         <v>10000</v>
       </c>
       <c r="K2" s="47">
-        <f>AVERAGE(SUM(simulations_small!M3:O3),SUM(simulations_medium!M3:O3),SUM(simulations_large!M3:O3))</f>
+        <f>AVERAGE(SUM(training_small!M3:O3),SUM(training_medium!M3:O3),SUM(training_large!M3:O3))</f>
         <v>5212055330.3555641</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B3" s="27">
-        <f>MIN(simulations_small!$J$3:$J$15)</f>
+        <f>MIN(training_small!$J$3:$J$15)</f>
         <v>1.3737617500001136</v>
       </c>
       <c r="C3" s="27">
-        <f>MIN(simulations_small!$K$3:$K$15)</f>
+        <f>MIN(training_small!$K$3:$K$15)</f>
         <v>3.1700814093177105</v>
       </c>
       <c r="D3" s="27">
-        <f>MIN(simulations_small!$L$3:$L$15)</f>
+        <f>MIN(training_small!$L$3:$L$15)</f>
         <v>1.7804722433438018</v>
       </c>
       <c r="E3" s="27">
-        <f>MIN(simulations_small!$M$3:$M$15)</f>
+        <f>MIN(training_small!$M$3:$M$15)</f>
         <v>2083.1086031650316</v>
       </c>
       <c r="F3" s="27">
-        <f>MIN(simulations_small!$N$3:$N$15)</f>
+        <f>MIN(training_small!$N$3:$N$15)</f>
         <v>8339273.347047206</v>
       </c>
       <c r="G3" s="27">
-        <f>MIN(simulations_small!$O$3:$O$15)</f>
+        <f>MIN(training_small!$O$3:$O$15)</f>
         <v>2887.7800032286405</v>
       </c>
       <c r="J3" s="6">
         <v>15000</v>
       </c>
       <c r="K3" s="47">
-        <f>AVERAGE(SUM(simulations_small!M4:O4),SUM(simulations_medium!M4:O4),SUM(simulations_large!M4:O4))</f>
+        <f>AVERAGE(SUM(training_small!M4:O4),SUM(training_medium!M4:O4),SUM(training_large!M4:O4))</f>
         <v>4645007633.29638</v>
       </c>
       <c r="N3" s="48">
@@ -1010,34 +1028,34 @@
         <v>33</v>
       </c>
       <c r="B4" s="25">
-        <f>VLOOKUP(B3,simulations_small!$J$3:$P$15,7,FALSE)</f>
+        <f>VLOOKUP(B3,training_small!$J$3:$P$15,7,FALSE)</f>
         <v>60000</v>
       </c>
       <c r="C4" s="25">
-        <f>VLOOKUP(C3,simulations_small!$K$3:$P$15,6,FALSE)</f>
+        <f>VLOOKUP(C3,training_small!$K$3:$P$15,6,FALSE)</f>
         <v>70000</v>
       </c>
       <c r="D4" s="25">
-        <f>VLOOKUP(D3,simulations_small!$L$3:$P$15,5,FALSE)</f>
+        <f>VLOOKUP(D3,training_small!$L$3:$P$15,5,FALSE)</f>
         <v>70000</v>
       </c>
       <c r="E4" s="25">
-        <f>VLOOKUP(E3,simulations_small!$M$3:$P$15,4,FALSE)</f>
+        <f>VLOOKUP(E3,training_small!$M$3:$P$15,4,FALSE)</f>
         <v>55000</v>
       </c>
       <c r="F4" s="25">
-        <f>VLOOKUP(F3,simulations_small!$N$3:$P$15,3,FALSE)</f>
+        <f>VLOOKUP(F3,training_small!$N$3:$P$15,3,FALSE)</f>
         <v>30000</v>
       </c>
       <c r="G4" s="25">
-        <f>VLOOKUP(G3,simulations_small!$O$3:$P$15,2,FALSE)</f>
+        <f>VLOOKUP(G3,training_small!$O$3:$P$15,2,FALSE)</f>
         <v>30000</v>
       </c>
       <c r="J4" s="8">
         <v>20000</v>
       </c>
       <c r="K4" s="47">
-        <f>AVERAGE(SUM(simulations_small!M5:O5),SUM(simulations_medium!M5:O5),SUM(simulations_large!M5:O5))</f>
+        <f>AVERAGE(SUM(training_small!M5:O5),SUM(training_medium!M5:O5),SUM(training_large!M5:O5))</f>
         <v>2112039822.6323636</v>
       </c>
     </row>
@@ -1046,7 +1064,7 @@
         <v>25000</v>
       </c>
       <c r="K5" s="47">
-        <f>AVERAGE(SUM(simulations_small!M6:O6),SUM(simulations_medium!M6:O6),SUM(simulations_large!M6:O6))</f>
+        <f>AVERAGE(SUM(training_small!M6:O6),SUM(training_medium!M6:O6),SUM(training_large!M6:O6))</f>
         <v>838526026.82951367</v>
       </c>
     </row>
@@ -1055,7 +1073,7 @@
         <v>30000</v>
       </c>
       <c r="K6" s="47">
-        <f>AVERAGE(SUM(simulations_small!M7:O7),SUM(simulations_medium!M7:O7),SUM(simulations_large!M7:O7))</f>
+        <f>AVERAGE(SUM(training_small!M7:O7),SUM(training_medium!M7:O7),SUM(training_large!M7:O7))</f>
         <v>1874572191.5957472</v>
       </c>
     </row>
@@ -1067,7 +1085,7 @@
         <v>35000</v>
       </c>
       <c r="K7" s="47">
-        <f>AVERAGE(SUM(simulations_small!M8:O8),SUM(simulations_medium!M8:O8),SUM(simulations_large!M8:O8))</f>
+        <f>AVERAGE(SUM(training_small!M8:O8),SUM(training_medium!M8:O8),SUM(training_large!M8:O8))</f>
         <v>2955234339.5841203</v>
       </c>
     </row>
@@ -1100,40 +1118,40 @@
         <v>40000</v>
       </c>
       <c r="K8" s="47">
-        <f>AVERAGE(SUM(simulations_small!M9:O9),SUM(simulations_medium!M9:O9),SUM(simulations_large!M9:O9))</f>
+        <f>AVERAGE(SUM(training_small!M9:O9),SUM(training_medium!M9:O9),SUM(training_large!M9:O9))</f>
         <v>5700956947.7433271</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B9" s="27">
-        <f>MIN(simulations_medium!$J$3:$J$15)</f>
+        <f>MIN(training_medium!$J$3:$J$15)</f>
         <v>3.3914888888889942</v>
       </c>
       <c r="C9" s="27">
-        <f>MIN(simulations_medium!$K$3:$K$15)</f>
+        <f>MIN(training_medium!$K$3:$K$15)</f>
         <v>15.554014002609494</v>
       </c>
       <c r="D9" s="27">
-        <f>MIN(simulations_medium!$L$3:$L$15)</f>
+        <f>MIN(training_medium!$L$3:$L$15)</f>
         <v>3.943857756386441</v>
       </c>
       <c r="E9" s="27">
-        <f>MIN(simulations_medium!$M$3:$M$15)</f>
+        <f>MIN(training_medium!$M$3:$M$15)</f>
         <v>7816.7157254445674</v>
       </c>
       <c r="F9" s="27">
-        <f>MIN(simulations_medium!$N$3:$N$15)</f>
+        <f>MIN(training_medium!$N$3:$N$15)</f>
         <v>86516418.678357303</v>
       </c>
       <c r="G9" s="27">
-        <f>MIN(simulations_medium!$O$3:$O$15)</f>
+        <f>MIN(training_medium!$O$3:$O$15)</f>
         <v>9301.4202506045986</v>
       </c>
       <c r="J9" s="6">
         <v>45000</v>
       </c>
       <c r="K9" s="47">
-        <f>AVERAGE(SUM(simulations_small!M10:O10),SUM(simulations_medium!M10:O10),SUM(simulations_large!M10:O10))</f>
+        <f>AVERAGE(SUM(training_small!M10:O10),SUM(training_medium!M10:O10),SUM(training_large!M10:O10))</f>
         <v>1585955150.0458393</v>
       </c>
     </row>
@@ -1142,34 +1160,34 @@
         <v>33</v>
       </c>
       <c r="B10" s="25">
-        <f>VLOOKUP(B9,simulations_medium!$J$3:$P$18,7,FALSE)</f>
+        <f>VLOOKUP(B9,training_medium!$J$3:$P$18,7,FALSE)</f>
         <v>25000</v>
       </c>
       <c r="C10" s="25">
-        <f>VLOOKUP(C9,simulations_medium!$K$3:$P$18,6,FALSE)</f>
+        <f>VLOOKUP(C9,training_medium!$K$3:$P$18,6,FALSE)</f>
         <v>40000</v>
       </c>
       <c r="D10" s="25">
-        <f>VLOOKUP(D9,simulations_medium!$L$3:$P$18,5,FALSE)</f>
+        <f>VLOOKUP(D9,training_medium!$L$3:$P$18,5,FALSE)</f>
         <v>40000</v>
       </c>
       <c r="E10" s="25">
-        <f>VLOOKUP(E9,simulations_medium!$M$3:$P$18,4,FALSE)</f>
+        <f>VLOOKUP(E9,training_medium!$M$3:$P$18,4,FALSE)</f>
         <v>65000</v>
       </c>
       <c r="F10" s="25">
-        <f>VLOOKUP(F9,simulations_medium!$N$3:$P$18,3,FALSE)</f>
+        <f>VLOOKUP(F9,training_medium!$N$3:$P$18,3,FALSE)</f>
         <v>65000</v>
       </c>
       <c r="G10" s="25">
-        <f>VLOOKUP(G9,simulations_medium!$O$3:$P$18,2,FALSE)</f>
+        <f>VLOOKUP(G9,training_medium!$O$3:$P$18,2,FALSE)</f>
         <v>65000</v>
       </c>
       <c r="J10" s="9">
         <v>50000</v>
       </c>
       <c r="K10" s="48">
-        <f>AVERAGE(SUM(simulations_small!M11:O11),SUM(simulations_medium!M11:O11),SUM(simulations_large!M11:O11))</f>
+        <f>AVERAGE(SUM(training_small!M11:O11),SUM(training_medium!M11:O11),SUM(training_large!M11:O11))</f>
         <v>595663988.86136937</v>
       </c>
     </row>
@@ -1178,7 +1196,7 @@
         <v>55000</v>
       </c>
       <c r="K11" s="47">
-        <f>AVERAGE(SUM(simulations_small!M12:O12),SUM(simulations_medium!M12:O12),SUM(simulations_large!M12:O12))</f>
+        <f>AVERAGE(SUM(training_small!M12:O12),SUM(training_medium!M12:O12),SUM(training_large!M12:O12))</f>
         <v>2321305185.002944</v>
       </c>
     </row>
@@ -1187,7 +1205,7 @@
         <v>60000</v>
       </c>
       <c r="K12" s="47">
-        <f>AVERAGE(SUM(simulations_small!M13:O13),SUM(simulations_medium!M13:O13),SUM(simulations_large!M13:O13))</f>
+        <f>AVERAGE(SUM(training_small!M13:O13),SUM(training_medium!M13:O13),SUM(training_large!M13:O13))</f>
         <v>2269867824.6664844</v>
       </c>
     </row>
@@ -1199,7 +1217,7 @@
         <v>65000</v>
       </c>
       <c r="K13" s="47">
-        <f>AVERAGE(SUM(simulations_small!M14:O14),SUM(simulations_medium!M14:O14),SUM(simulations_large!M14:O14))</f>
+        <f>AVERAGE(SUM(training_small!M14:O14),SUM(training_medium!M14:O14),SUM(training_large!M14:O14))</f>
         <v>2446868182.972899</v>
       </c>
     </row>
@@ -1232,33 +1250,33 @@
         <v>70000</v>
       </c>
       <c r="K14" s="47">
-        <f>AVERAGE(SUM(simulations_small!M15:O15),SUM(simulations_medium!M15:O15),SUM(simulations_large!M15:O15))</f>
+        <f>AVERAGE(SUM(training_small!M15:O15),SUM(training_medium!M15:O15),SUM(training_large!M15:O15))</f>
         <v>688137236.06868434</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B15" s="42">
-        <f>MIN(simulations_large!$J$3:$J$15)</f>
+        <f>MIN(training_large!$J$3:$J$15)</f>
         <v>30.783059199999915</v>
       </c>
       <c r="C15" s="42">
-        <f>MIN(simulations_large!$K$3:$K$15)</f>
+        <f>MIN(training_large!$K$3:$K$15)</f>
         <v>20030.831877420351</v>
       </c>
       <c r="D15" s="42">
-        <f>MIN(simulations_large!$L$3:$L$15)</f>
+        <f>MIN(training_large!$L$3:$L$15)</f>
         <v>141.53032140647582</v>
       </c>
       <c r="E15" s="42">
-        <f>MIN(simulations_large!$M$3:$M$15)</f>
+        <f>MIN(training_large!$M$3:$M$15)</f>
         <v>12465.253210959938</v>
       </c>
       <c r="F15" s="42">
-        <f>MIN(simulations_large!$N$3:$N$15)</f>
+        <f>MIN(training_large!$N$3:$N$15)</f>
         <v>331300469.0961979</v>
       </c>
       <c r="G15" s="42">
-        <f>MIN(simulations_large!$O$3:$O$15)</f>
+        <f>MIN(training_large!$O$3:$O$15)</f>
         <v>18201.661163097117</v>
       </c>
     </row>
@@ -1267,33 +1285,937 @@
         <v>33</v>
       </c>
       <c r="B16" s="25">
-        <f>VLOOKUP(B15,simulations_large!$J$3:$P$15,7,FALSE)</f>
+        <f>VLOOKUP(B15,training_large!$J$3:$P$15,7,FALSE)</f>
         <v>70000</v>
       </c>
       <c r="C16" s="25">
-        <f>VLOOKUP(C15,simulations_large!$K$3:$P$15,6,FALSE)</f>
+        <f>VLOOKUP(C15,training_large!$K$3:$P$15,6,FALSE)</f>
         <v>50000</v>
       </c>
       <c r="D16" s="25">
-        <f>VLOOKUP(D15,simulations_large!$L$3:$P$15,5,FALSE)</f>
+        <f>VLOOKUP(D15,training_large!$L$3:$P$15,5,FALSE)</f>
         <v>50000</v>
       </c>
       <c r="E16" s="25">
-        <f>VLOOKUP(E15,simulations_large!$M$3:$P$15,4,FALSE)</f>
+        <f>VLOOKUP(E15,training_large!$M$3:$P$15,4,FALSE)</f>
         <v>70000</v>
       </c>
       <c r="F16" s="25">
-        <f>VLOOKUP(F15,simulations_large!$N$3:$P$15,3,FALSE)</f>
+        <f>VLOOKUP(F15,training_large!$N$3:$P$15,3,FALSE)</f>
         <v>70000</v>
       </c>
       <c r="G16" s="25">
-        <f>VLOOKUP(G15,simulations_large!$O$3:$P$15,2,FALSE)</f>
+        <f>VLOOKUP(G15,training_large!$O$3:$P$15,2,FALSE)</f>
         <v>70000</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E7CF371-4E5D-45D3-9680-881967F627C5}">
+  <dimension ref="A2:F55"/>
+  <sheetViews>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B2" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>4800</v>
+      </c>
+      <c r="E3">
+        <v>60</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>5200</v>
+      </c>
+      <c r="E4">
+        <v>60</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>5000</v>
+      </c>
+      <c r="E5">
+        <v>60</v>
+      </c>
+      <c r="F5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6">
+        <v>5400</v>
+      </c>
+      <c r="E6">
+        <v>60</v>
+      </c>
+      <c r="F6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>5000</v>
+      </c>
+      <c r="E7">
+        <v>60</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <v>5500</v>
+      </c>
+      <c r="E8">
+        <v>60</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9">
+        <v>5500</v>
+      </c>
+      <c r="E9">
+        <v>60</v>
+      </c>
+      <c r="F9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10">
+        <v>5000</v>
+      </c>
+      <c r="E10">
+        <v>60</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11">
+        <v>5000</v>
+      </c>
+      <c r="E11">
+        <v>60</v>
+      </c>
+      <c r="F11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12">
+        <v>5500</v>
+      </c>
+      <c r="E12">
+        <v>60</v>
+      </c>
+      <c r="F12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <v>5500</v>
+      </c>
+      <c r="E13">
+        <v>60</v>
+      </c>
+      <c r="F13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <v>5000</v>
+      </c>
+      <c r="E14">
+        <v>60</v>
+      </c>
+      <c r="F14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15">
+        <v>4600</v>
+      </c>
+      <c r="E15">
+        <v>60</v>
+      </c>
+      <c r="F15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16">
+        <v>5100</v>
+      </c>
+      <c r="E16">
+        <v>60</v>
+      </c>
+      <c r="F16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17">
+        <v>5200</v>
+      </c>
+      <c r="E17">
+        <v>60</v>
+      </c>
+      <c r="F17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18">
+        <v>5000</v>
+      </c>
+      <c r="E18">
+        <v>60</v>
+      </c>
+      <c r="F18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19">
+        <v>5500</v>
+      </c>
+      <c r="E19">
+        <v>60</v>
+      </c>
+      <c r="F19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20">
+        <v>5500</v>
+      </c>
+      <c r="E20">
+        <v>60</v>
+      </c>
+      <c r="F20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21">
+        <v>5000</v>
+      </c>
+      <c r="E21">
+        <v>60</v>
+      </c>
+      <c r="F21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22">
+        <v>5000</v>
+      </c>
+      <c r="E22">
+        <v>60</v>
+      </c>
+      <c r="F22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23">
+        <v>5500</v>
+      </c>
+      <c r="E23">
+        <v>60</v>
+      </c>
+      <c r="F23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>21</v>
+      </c>
+      <c r="B24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24">
+        <v>5500</v>
+      </c>
+      <c r="E24">
+        <v>60</v>
+      </c>
+      <c r="F24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>22</v>
+      </c>
+      <c r="B25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25">
+        <v>5000</v>
+      </c>
+      <c r="E25">
+        <v>60</v>
+      </c>
+      <c r="F25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>23</v>
+      </c>
+      <c r="B26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26">
+        <v>5000</v>
+      </c>
+      <c r="E26">
+        <v>60</v>
+      </c>
+      <c r="F26">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>24</v>
+      </c>
+      <c r="B27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27">
+        <v>5400</v>
+      </c>
+      <c r="E27">
+        <v>60</v>
+      </c>
+      <c r="F27">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>25</v>
+      </c>
+      <c r="B28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30" s="29">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>3079.9488820000001</v>
+      </c>
+      <c r="D31" s="29">
+        <v>10578820</v>
+      </c>
+      <c r="E31">
+        <v>3252.509963</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32">
+        <v>2589.0103300000001</v>
+      </c>
+      <c r="D32" s="29">
+        <v>5804110</v>
+      </c>
+      <c r="E32">
+        <v>2409.1720749999999</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="C33">
+        <v>3729.5815219999999</v>
+      </c>
+      <c r="D33" s="29">
+        <v>3012089</v>
+      </c>
+      <c r="E33">
+        <v>1735.5371970000001</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B34">
+        <v>4</v>
+      </c>
+      <c r="C34">
+        <v>3402.7270549999998</v>
+      </c>
+      <c r="D34" s="29">
+        <v>1645894</v>
+      </c>
+      <c r="E34">
+        <v>1282.924162</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B35">
+        <v>5</v>
+      </c>
+      <c r="C35">
+        <v>4321.9101819999996</v>
+      </c>
+      <c r="D35" s="29">
+        <v>5027045</v>
+      </c>
+      <c r="E35">
+        <v>2242.10716</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B36">
+        <v>6</v>
+      </c>
+      <c r="C36">
+        <v>4167.8139469999996</v>
+      </c>
+      <c r="D36" s="29">
+        <v>4021661</v>
+      </c>
+      <c r="E36">
+        <v>2005.407995</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B37">
+        <v>7</v>
+      </c>
+      <c r="C37">
+        <v>6615.584038</v>
+      </c>
+      <c r="D37" s="29">
+        <v>3323337</v>
+      </c>
+      <c r="E37">
+        <v>1823.0021959999999</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B38">
+        <v>8</v>
+      </c>
+      <c r="C38">
+        <v>5902.7270429999999</v>
+      </c>
+      <c r="D38" s="29">
+        <v>1645895</v>
+      </c>
+      <c r="E38">
+        <v>1282.924205</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B39">
+        <v>9</v>
+      </c>
+      <c r="C39">
+        <v>6821.9101689999998</v>
+      </c>
+      <c r="D39" s="29">
+        <v>5027045</v>
+      </c>
+      <c r="E39">
+        <v>2242.1071900000002</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B40">
+        <v>10</v>
+      </c>
+      <c r="C40">
+        <v>6667.8139350000001</v>
+      </c>
+      <c r="D40" s="29">
+        <v>4021661</v>
+      </c>
+      <c r="E40">
+        <v>2005.4080269999999</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B41">
+        <v>11</v>
+      </c>
+      <c r="C41">
+        <v>9115.5840250000001</v>
+      </c>
+      <c r="D41" s="29">
+        <v>3323337</v>
+      </c>
+      <c r="E41">
+        <v>1823.00225</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B42">
+        <v>12</v>
+      </c>
+      <c r="C42">
+        <v>9115.5840250000001</v>
+      </c>
+      <c r="D42" s="29">
+        <v>1645895</v>
+      </c>
+      <c r="E42">
+        <v>1282.9242750000001</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B43">
+        <v>13</v>
+      </c>
+      <c r="C43">
+        <v>8251.2381100000002</v>
+      </c>
+      <c r="D43" s="29">
+        <v>1215558</v>
+      </c>
+      <c r="E43">
+        <v>1102.5235359999999</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B44">
+        <v>14</v>
+      </c>
+      <c r="C44">
+        <v>9477.8493080000007</v>
+      </c>
+      <c r="D44" s="29">
+        <v>8230023</v>
+      </c>
+      <c r="E44">
+        <v>2868.801645</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B45">
+        <v>15</v>
+      </c>
+      <c r="C45">
+        <v>8986.9107569999996</v>
+      </c>
+      <c r="D45" s="29">
+        <v>4091322</v>
+      </c>
+      <c r="E45">
+        <v>2022.7015449999999</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B46">
+        <v>16</v>
+      </c>
+      <c r="C46">
+        <v>9906.0938829999996</v>
+      </c>
+      <c r="D46" s="29">
+        <v>10676060</v>
+      </c>
+      <c r="E46">
+        <v>3267.4243820000002</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B47">
+        <v>17</v>
+      </c>
+      <c r="C47">
+        <v>9751.9976480000005</v>
+      </c>
+      <c r="D47" s="29">
+        <v>8693013</v>
+      </c>
+      <c r="E47">
+        <v>2948.3916479999998</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B48">
+        <v>18</v>
+      </c>
+      <c r="C48">
+        <v>12199.767739000001</v>
+      </c>
+      <c r="D48" s="29">
+        <v>3861120</v>
+      </c>
+      <c r="E48">
+        <v>1964.9733530000001</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B49">
+        <v>19</v>
+      </c>
+      <c r="C49">
+        <v>11486.910744000001</v>
+      </c>
+      <c r="D49" s="29">
+        <v>4091322</v>
+      </c>
+      <c r="E49">
+        <v>2022.701607</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B50">
+        <v>20</v>
+      </c>
+      <c r="C50">
+        <v>12406.093870000001</v>
+      </c>
+      <c r="D50" s="29">
+        <v>10676060</v>
+      </c>
+      <c r="E50">
+        <v>3267.4244279999998</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B51">
+        <v>21</v>
+      </c>
+      <c r="C51">
+        <v>12251.997635</v>
+      </c>
+      <c r="D51" s="29">
+        <v>8693014</v>
+      </c>
+      <c r="E51">
+        <v>2948.3917000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B52">
+        <v>22</v>
+      </c>
+      <c r="C52">
+        <v>14699.767726</v>
+      </c>
+      <c r="D52" s="29">
+        <v>3861121</v>
+      </c>
+      <c r="E52">
+        <v>1964.9734370000001</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B53">
+        <v>23</v>
+      </c>
+      <c r="C53">
+        <v>13986.910717999999</v>
+      </c>
+      <c r="D53" s="29">
+        <v>4091322</v>
+      </c>
+      <c r="E53">
+        <v>2022.7017800000001</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B54">
+        <v>24</v>
+      </c>
+      <c r="C54">
+        <v>15127.481922999999</v>
+      </c>
+      <c r="D54" s="29">
+        <v>4814614</v>
+      </c>
+      <c r="E54">
+        <v>2194.2227910000001</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B55">
+        <v>25</v>
+      </c>
+      <c r="C55">
+        <v>14800.627458000001</v>
+      </c>
+      <c r="D55" s="29">
+        <v>4108688</v>
+      </c>
+      <c r="E55">
+        <v>2026.9898519999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1301,8 +2223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{544FD0B2-A7ED-4478-8092-5F67F619DD9A}">
   <dimension ref="A1:S64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="72" workbookViewId="0">
-      <selection activeCell="K58" sqref="K58"/>
+    <sheetView topLeftCell="B1" zoomScale="72" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3:O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7151,8 +8073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07E2FAA7-AF33-4595-8B19-D05C042724E7}">
   <dimension ref="A1:P357"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScale="82" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView zoomScale="82" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13938,905 +14860,907 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E7CF371-4E5D-45D3-9680-881967F627C5}">
-  <dimension ref="A2:F55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E65EBE07-936B-40B2-8C67-B5100E097F4C}">
+  <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="13" max="13" width="11.08984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B2" s="40" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="40" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B1" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B2" s="58" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="58" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="56">
+        <f>AVERAGE(ABS($C$4-C14),ABS($C$5-C15),ABS($C$6-C16),ABS($C$7-C17), ABS(C8-C18),ABS(C9-C19))</f>
+        <v>1.9768808333333492</v>
+      </c>
+      <c r="J2" s="56">
+        <f>AVERAGE(($C$4-C14)^2,($C$5-C15)^2,($C$6-C16)^2,($C$7-C17)^2,(C8-C18)^2,(C9-C19)^2)</f>
+        <v>4.5148130547306247</v>
+      </c>
+      <c r="K2" s="56">
+        <f t="shared" ref="K2" si="0">SQRT(J2)</f>
+        <v>2.1248089454655976</v>
+      </c>
+      <c r="L2" s="56">
+        <f>AVERAGE(ABS($D$4-D14),ABS($D$5-D15),ABS($D$6-D16),ABS($D$7-D17), ABS(D8-D18),ABS(D9-D19))</f>
+        <v>473.154626000002</v>
+      </c>
+      <c r="M2" s="56">
+        <f>AVERAGE(($D$4-D14)^2,($D$5-D15)^2,($D$6-D16)^2,($D$7-D17)^2,(D8-D18)^2,(D9-D19)^2)</f>
+        <v>395877.93759168102</v>
+      </c>
+      <c r="N2" s="56">
+        <f t="shared" ref="N2" si="1">SQRT(M2)</f>
+        <v>629.18831647741285</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B3" s="57">
+        <v>0</v>
+      </c>
+      <c r="C3" s="57">
+        <v>0</v>
+      </c>
+      <c r="D3" s="57">
+        <v>0</v>
+      </c>
+      <c r="E3" s="57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B4" s="57">
+        <v>1</v>
+      </c>
+      <c r="C4" s="57">
+        <v>-68.708804000000001</v>
+      </c>
+      <c r="D4" s="57">
+        <v>27128.451845</v>
+      </c>
+      <c r="E4" s="57">
+        <v>164.70716999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B5" s="57">
+        <v>2</v>
+      </c>
+      <c r="C5" s="57">
+        <v>258.73477200000002</v>
+      </c>
+      <c r="D5" s="57">
+        <v>167658.64587099999</v>
+      </c>
+      <c r="E5" s="57">
+        <v>409.46141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B6" s="57">
+        <v>3</v>
+      </c>
+      <c r="C6" s="57">
+        <v>874.72454900000002</v>
+      </c>
+      <c r="D6" s="57">
+        <v>85449.068721000003</v>
+      </c>
+      <c r="E6" s="57">
+        <v>292.31672700000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B7" s="57">
+        <v>4</v>
+      </c>
+      <c r="C7" s="57">
+        <v>741.26522299999999</v>
+      </c>
+      <c r="D7" s="57">
+        <v>167658.64826700001</v>
+      </c>
+      <c r="E7" s="57">
+        <v>409.461412</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B8" s="57">
+        <v>5</v>
+      </c>
+      <c r="C8" s="57">
+        <v>883.83662200000003</v>
+      </c>
+      <c r="D8" s="57">
+        <v>69755.045148999998</v>
+      </c>
+      <c r="E8" s="57">
+        <v>264.11180400000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B9" s="57">
         <v>6</v>
       </c>
-      <c r="D2" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="40" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3">
+      <c r="C9" s="57">
+        <v>1067.6732469999999</v>
+      </c>
+      <c r="D9" s="57">
+        <v>279020.17066100001</v>
+      </c>
+      <c r="E9" s="57">
+        <v>528.22359900000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A12" s="53" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="54"/>
+      <c r="C12" s="54"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="55"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B13" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B14" s="57">
+        <v>1</v>
+      </c>
+      <c r="C14" s="57">
+        <v>-69.379067000000006</v>
+      </c>
+      <c r="D14" s="57">
+        <v>27328.011849999999</v>
+      </c>
+      <c r="E14" s="57">
+        <v>165.31186199999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B15" s="57">
+        <v>2</v>
+      </c>
+      <c r="C15" s="57">
+        <v>256.45200899999998</v>
+      </c>
+      <c r="D15" s="57">
+        <v>168039.78580000001</v>
+      </c>
+      <c r="E15" s="57">
+        <v>409.92656099999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B16" s="57">
+        <v>3</v>
+      </c>
+      <c r="C16" s="57">
+        <v>876.50158199999998</v>
+      </c>
+      <c r="D16" s="57">
+        <v>85601.967950000006</v>
+      </c>
+      <c r="E16" s="57">
+        <v>292.57814000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B17" s="57">
+        <v>4</v>
+      </c>
+      <c r="C17" s="57">
+        <v>743.54799100000002</v>
+      </c>
+      <c r="D17" s="57">
+        <v>168039.78580000001</v>
+      </c>
+      <c r="E17" s="57">
+        <v>409.92656099999999</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B18" s="57">
+        <v>5</v>
+      </c>
+      <c r="C18" s="57">
+        <v>885.45277599999997</v>
+      </c>
+      <c r="D18" s="57">
+        <v>70099.881370000003</v>
+      </c>
+      <c r="E18" s="57">
+        <v>264.763822</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B19" s="57">
+        <v>6</v>
+      </c>
+      <c r="C19" s="57">
+        <v>1070.9055510000001</v>
+      </c>
+      <c r="D19" s="57">
+        <v>280399.52549999999</v>
+      </c>
+      <c r="E19" s="57">
+        <v>529.52764400000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A12:F12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94758BC1-2CCA-481E-AF67-9C7CD61EE707}">
+  <dimension ref="A1:N19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="13" max="13" width="11.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B1" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B2" s="60" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="60" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="60" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="7">
+        <f>AVERAGE(ABS($C$4-C14),ABS($C$5-C15),ABS($C$6-C16),ABS($C$7-C17), ABS(C8-C18),ABS(C9-C19))</f>
+        <v>2.588224166666663</v>
+      </c>
+      <c r="J2" s="7">
+        <f>AVERAGE(($C$4-C14)^2,($C$5-C15)^2,($C$6-C16)^2,($C$7-C17)^2,(C8-C18)^2,(C9-C19)^2)</f>
+        <v>8.5307796505198201</v>
+      </c>
+      <c r="K2" s="7">
+        <f t="shared" ref="K2" si="0">SQRT(J2)</f>
+        <v>2.9207498438791055</v>
+      </c>
+      <c r="L2" s="7">
+        <f>AVERAGE(ABS($D$4-D14),ABS($D$5-D15),ABS($D$6-D16),ABS($D$7-D17), ABS(D8-D18),ABS(D9-D19))</f>
+        <v>511.79385200000007</v>
+      </c>
+      <c r="M2" s="7">
+        <f>AVERAGE(($D$4-D14)^2,($D$5-D15)^2,($D$6-D16)^2,($D$7-D17)^2,(D8-D18)^2,(D9-D19)^2)</f>
+        <v>548936.78202390438</v>
+      </c>
+      <c r="N2" s="7">
+        <f t="shared" ref="N2" si="1">SQRT(M2)</f>
+        <v>740.90268053497039</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B3" s="59">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3">
-        <v>4800</v>
-      </c>
-      <c r="E3">
-        <v>60</v>
-      </c>
-      <c r="F3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4">
+      <c r="C3" s="59">
+        <v>0</v>
+      </c>
+      <c r="D3" s="59">
+        <v>0</v>
+      </c>
+      <c r="E3" s="59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B4" s="59">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4">
-        <v>5200</v>
-      </c>
-      <c r="E4">
-        <v>60</v>
-      </c>
-      <c r="F4">
+      <c r="C4" s="59">
+        <v>-183.836625</v>
+      </c>
+      <c r="D4" s="59">
+        <v>69755.041398000001</v>
+      </c>
+      <c r="E4" s="59">
+        <v>264.11179700000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B5" s="59">
+        <v>2</v>
+      </c>
+      <c r="C5" s="59">
+        <v>-41.265225999999998</v>
+      </c>
+      <c r="D5" s="59">
+        <v>167658.64554699999</v>
+      </c>
+      <c r="E5" s="59">
+        <v>409.461409</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B6" s="59">
+        <v>3</v>
+      </c>
+      <c r="C6" s="59">
+        <v>231.31504000000001</v>
+      </c>
+      <c r="D6" s="59">
+        <v>61338.763644999999</v>
+      </c>
+      <c r="E6" s="59">
+        <v>247.66663800000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B7" s="59">
+        <v>4</v>
+      </c>
+      <c r="C7" s="59">
+        <v>-158.73477299999999</v>
+      </c>
+      <c r="D7" s="59">
+        <v>167658.64566400001</v>
+      </c>
+      <c r="E7" s="59">
+        <v>409.461409</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B8" s="59">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5">
+      <c r="C8" s="59">
+        <v>98.187709999999996</v>
+      </c>
+      <c r="D8" s="59">
+        <v>38763.349247999999</v>
+      </c>
+      <c r="E8" s="59">
+        <v>196.88410099999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B9" s="59">
+        <v>6</v>
+      </c>
+      <c r="C9" s="59">
+        <v>196.37542099999999</v>
+      </c>
+      <c r="D9" s="59">
+        <v>155053.39699000001</v>
+      </c>
+      <c r="E9" s="59">
+        <v>393.76820199999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A12" s="53" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="54"/>
+      <c r="C12" s="54"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="55"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B13" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5">
-        <v>5000</v>
-      </c>
-      <c r="E5">
-        <v>60</v>
-      </c>
-      <c r="F5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6">
+      <c r="D13" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6">
-        <v>5400</v>
-      </c>
-      <c r="E6">
-        <v>60</v>
-      </c>
-      <c r="F6">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7">
+      <c r="E13" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7">
-        <v>5000</v>
-      </c>
-      <c r="E7">
-        <v>60</v>
-      </c>
-      <c r="F7">
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B14" s="59">
+        <v>1</v>
+      </c>
+      <c r="C14" s="59">
+        <v>-181.649552</v>
+      </c>
+      <c r="D14" s="59">
+        <v>69065.686079999999</v>
+      </c>
+      <c r="E14" s="59">
+        <v>262.80351200000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B15" s="59">
+        <v>2</v>
+      </c>
+      <c r="C15" s="59">
+        <v>-37.248085000000003</v>
+      </c>
+      <c r="D15" s="59">
+        <v>167592.42180000001</v>
+      </c>
+      <c r="E15" s="59">
+        <v>409.38053400000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B16" s="59">
+        <v>3</v>
+      </c>
+      <c r="C16" s="59">
+        <v>231.59438</v>
+      </c>
+      <c r="D16" s="59">
+        <v>61575.392099999997</v>
+      </c>
+      <c r="E16" s="59">
+        <v>248.14389399999999</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B17" s="59">
+        <v>4</v>
+      </c>
+      <c r="C17" s="59">
+        <v>-162.751915</v>
+      </c>
+      <c r="D17" s="59">
+        <v>167592.42180000001</v>
+      </c>
+      <c r="E17" s="59">
+        <v>409.38053400000001</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B18" s="59">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8">
+      <c r="C18" s="59">
+        <v>96.511493999999999</v>
+      </c>
+      <c r="D18" s="59">
+        <v>38360.88291</v>
+      </c>
+      <c r="E18" s="59">
+        <v>195.85934499999999</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B19" s="59">
+        <v>6</v>
+      </c>
+      <c r="C19" s="59">
+        <v>193.022988</v>
+      </c>
+      <c r="D19" s="59">
+        <v>153443.53159999999</v>
+      </c>
+      <c r="E19" s="59">
+        <v>391.71868899999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A12:F12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75932BC4-4BC3-4AD2-9864-9185FC06DF6F}">
+  <dimension ref="A1:N27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="13" max="13" width="11.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B1" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B2" s="62" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="62" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="62" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="7">
+        <f>AVERAGE(ABS($C$4-C14),ABS($C$5-C15),ABS($C$6-C16),ABS($C$7-C17), ABS(C8-C18),ABS(C9-C19))</f>
+        <v>0.52213950000000509</v>
+      </c>
+      <c r="J2" s="7">
+        <f>AVERAGE(($C$4-C14)^2,($C$5-C15)^2,($C$6-C16)^2,($C$7-C17)^2,(C8-C18)^2,(C9-C19)^2)</f>
+        <v>0.32701922982283871</v>
+      </c>
+      <c r="K2" s="7">
+        <f t="shared" ref="K2" si="0">SQRT(J2)</f>
+        <v>0.57185595198689565</v>
+      </c>
+      <c r="L2" s="7">
+        <f>AVERAGE(ABS($D$4-D14),ABS($D$5-D15),ABS($D$6-D16),ABS($D$7-D17), ABS(D8-D18),ABS(D9-D19))</f>
+        <v>406.55218100000457</v>
+      </c>
+      <c r="M2" s="7">
+        <f>AVERAGE(($D$4-D14)^2,($D$5-D15)^2,($D$6-D16)^2,($D$7-D17)^2,(D8-D18)^2,(D9-D19)^2)</f>
+        <v>235438.63354525031</v>
+      </c>
+      <c r="N2" s="7">
+        <f t="shared" ref="N2" si="1">SQRT(M2)</f>
+        <v>485.22019078481298</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B3" s="61">
+        <v>0</v>
+      </c>
+      <c r="C3" s="61">
+        <v>0</v>
+      </c>
+      <c r="D3" s="61">
+        <v>0</v>
+      </c>
+      <c r="E3" s="61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B4" s="61">
+        <v>1</v>
+      </c>
+      <c r="C4" s="61">
+        <v>-136.290133</v>
+      </c>
+      <c r="D4" s="61">
+        <v>53125.096712999999</v>
+      </c>
+      <c r="E4" s="61">
+        <v>230.488821</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B5" s="61">
+        <v>2</v>
+      </c>
+      <c r="C5" s="61">
+        <v>58.734772999999997</v>
+      </c>
+      <c r="D5" s="61">
+        <v>167658.645556</v>
+      </c>
+      <c r="E5" s="61">
+        <v>409.461409</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B6" s="61">
+        <v>3</v>
+      </c>
+      <c r="C6" s="61">
+        <v>255.11019400000001</v>
+      </c>
+      <c r="D6" s="61">
+        <v>66752.123804999996</v>
+      </c>
+      <c r="E6" s="61">
+        <v>258.36432400000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B7" s="61">
+        <v>4</v>
+      </c>
+      <c r="C7" s="61">
+        <v>-258.73477200000002</v>
+      </c>
+      <c r="D7" s="61">
+        <v>167658.64587099999</v>
+      </c>
+      <c r="E7" s="61">
+        <v>409.46141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B8" s="61">
         <v>5</v>
       </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8">
-        <v>5500</v>
-      </c>
-      <c r="E8">
-        <v>60</v>
-      </c>
-      <c r="F8">
+      <c r="C8" s="61">
+        <v>68.708804000000001</v>
+      </c>
+      <c r="D8" s="61">
+        <v>27128.451845</v>
+      </c>
+      <c r="E8" s="61">
+        <v>164.70716999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B9" s="61">
+        <v>6</v>
+      </c>
+      <c r="C9" s="61">
+        <v>137.417608</v>
+      </c>
+      <c r="D9" s="61">
+        <v>108513.80738</v>
+      </c>
+      <c r="E9" s="61">
+        <v>329.41433999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A12" s="53" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="54"/>
+      <c r="C12" s="54"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="55"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B13" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B14" s="61">
+        <v>1</v>
+      </c>
+      <c r="C14" s="61">
+        <v>-135.99306999999999</v>
+      </c>
+      <c r="D14" s="61">
+        <v>52750.987679999998</v>
+      </c>
+      <c r="E14" s="61">
+        <v>229.67583200000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B15" s="61">
+        <v>2</v>
+      </c>
+      <c r="C15" s="61">
+        <v>59.385553999999999</v>
+      </c>
+      <c r="D15" s="61">
+        <v>167842.66130000001</v>
+      </c>
+      <c r="E15" s="61">
+        <v>409.68605200000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B16" s="61">
+        <v>3</v>
+      </c>
+      <c r="C16" s="61">
+        <v>254.908231</v>
+      </c>
+      <c r="D16" s="61">
+        <v>67286.563460000005</v>
+      </c>
+      <c r="E16" s="61">
+        <v>259.39653700000002</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B17" s="61">
+        <v>4</v>
+      </c>
+      <c r="C17" s="61">
+        <v>-259.38555400000001</v>
+      </c>
+      <c r="D17" s="61">
+        <v>167842.66130000001</v>
+      </c>
+      <c r="E17" s="61">
+        <v>409.68605200000002</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B18" s="61">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9">
+      <c r="C18" s="61">
+        <v>68.264720999999994</v>
+      </c>
+      <c r="D18" s="61">
+        <v>26895.905200000001</v>
+      </c>
+      <c r="E18" s="61">
+        <v>163.99971099999999</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B19" s="61">
         <v>6</v>
       </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9">
-        <v>5500</v>
-      </c>
-      <c r="E9">
-        <v>60</v>
-      </c>
-      <c r="F9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10">
-        <v>5000</v>
-      </c>
-      <c r="E10">
-        <v>60</v>
-      </c>
-      <c r="F10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11">
-        <v>5000</v>
-      </c>
-      <c r="E11">
-        <v>60</v>
-      </c>
-      <c r="F11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12">
-        <v>5500</v>
-      </c>
-      <c r="E12">
-        <v>60</v>
-      </c>
-      <c r="F12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>10</v>
-      </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13">
-        <v>5500</v>
-      </c>
-      <c r="E13">
-        <v>60</v>
-      </c>
-      <c r="F13">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <v>11</v>
-      </c>
-      <c r="B14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14">
-        <v>5000</v>
-      </c>
-      <c r="E14">
-        <v>60</v>
-      </c>
-      <c r="F14">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <v>12</v>
-      </c>
-      <c r="B15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15">
-        <v>4600</v>
-      </c>
-      <c r="E15">
-        <v>60</v>
-      </c>
-      <c r="F15">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <v>13</v>
-      </c>
-      <c r="B16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16">
-        <v>5100</v>
-      </c>
-      <c r="E16">
-        <v>60</v>
-      </c>
-      <c r="F16">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <v>14</v>
-      </c>
-      <c r="B17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17">
-        <v>5200</v>
-      </c>
-      <c r="E17">
-        <v>60</v>
-      </c>
-      <c r="F17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18">
-        <v>15</v>
-      </c>
-      <c r="B18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18">
-        <v>5000</v>
-      </c>
-      <c r="E18">
-        <v>60</v>
-      </c>
-      <c r="F18">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19">
-        <v>16</v>
-      </c>
-      <c r="B19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19">
-        <v>5500</v>
-      </c>
-      <c r="E19">
-        <v>60</v>
-      </c>
-      <c r="F19">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20">
-        <v>17</v>
-      </c>
-      <c r="B20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20">
-        <v>5500</v>
-      </c>
-      <c r="E20">
-        <v>60</v>
-      </c>
-      <c r="F20">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21">
-        <v>18</v>
-      </c>
-      <c r="B21" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21">
-        <v>5000</v>
-      </c>
-      <c r="E21">
-        <v>60</v>
-      </c>
-      <c r="F21">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22">
-        <v>19</v>
-      </c>
-      <c r="B22" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22">
-        <v>5000</v>
-      </c>
-      <c r="E22">
-        <v>60</v>
-      </c>
-      <c r="F22">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23">
-        <v>20</v>
-      </c>
-      <c r="B23" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23">
-        <v>5500</v>
-      </c>
-      <c r="E23">
-        <v>60</v>
-      </c>
-      <c r="F23">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24">
-        <v>21</v>
-      </c>
-      <c r="B24" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24">
-        <v>5500</v>
-      </c>
-      <c r="E24">
-        <v>60</v>
-      </c>
-      <c r="F24">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25">
-        <v>22</v>
-      </c>
-      <c r="B25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25">
-        <v>5000</v>
-      </c>
-      <c r="E25">
-        <v>60</v>
-      </c>
-      <c r="F25">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26">
-        <v>23</v>
-      </c>
-      <c r="B26" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26">
-        <v>5000</v>
-      </c>
-      <c r="E26">
-        <v>60</v>
-      </c>
-      <c r="F26">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27">
-        <v>24</v>
-      </c>
-      <c r="B27" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" t="s">
-        <v>12</v>
-      </c>
-      <c r="D27">
-        <v>5400</v>
-      </c>
-      <c r="E27">
-        <v>60</v>
-      </c>
-      <c r="F27">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28">
-        <v>25</v>
-      </c>
-      <c r="B28" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B30">
-        <v>0</v>
-      </c>
-      <c r="C30">
-        <v>0</v>
-      </c>
-      <c r="D30" s="29">
-        <v>0</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31">
-        <v>3079.9488820000001</v>
-      </c>
-      <c r="D31" s="29">
-        <v>10578820</v>
-      </c>
-      <c r="E31">
-        <v>3252.509963</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B32">
-        <v>2</v>
-      </c>
-      <c r="C32">
-        <v>2589.0103300000001</v>
-      </c>
-      <c r="D32" s="29">
-        <v>5804110</v>
-      </c>
-      <c r="E32">
-        <v>2409.1720749999999</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B33">
-        <v>3</v>
-      </c>
-      <c r="C33">
-        <v>3729.5815219999999</v>
-      </c>
-      <c r="D33" s="29">
-        <v>3012089</v>
-      </c>
-      <c r="E33">
-        <v>1735.5371970000001</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B34">
-        <v>4</v>
-      </c>
-      <c r="C34">
-        <v>3402.7270549999998</v>
-      </c>
-      <c r="D34" s="29">
-        <v>1645894</v>
-      </c>
-      <c r="E34">
-        <v>1282.924162</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B35">
-        <v>5</v>
-      </c>
-      <c r="C35">
-        <v>4321.9101819999996</v>
-      </c>
-      <c r="D35" s="29">
-        <v>5027045</v>
-      </c>
-      <c r="E35">
-        <v>2242.10716</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B36">
-        <v>6</v>
-      </c>
-      <c r="C36">
-        <v>4167.8139469999996</v>
-      </c>
-      <c r="D36" s="29">
-        <v>4021661</v>
-      </c>
-      <c r="E36">
-        <v>2005.407995</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B37">
-        <v>7</v>
-      </c>
-      <c r="C37">
-        <v>6615.584038</v>
-      </c>
-      <c r="D37" s="29">
-        <v>3323337</v>
-      </c>
-      <c r="E37">
-        <v>1823.0021959999999</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B38">
-        <v>8</v>
-      </c>
-      <c r="C38">
-        <v>5902.7270429999999</v>
-      </c>
-      <c r="D38" s="29">
-        <v>1645895</v>
-      </c>
-      <c r="E38">
-        <v>1282.924205</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B39">
-        <v>9</v>
-      </c>
-      <c r="C39">
-        <v>6821.9101689999998</v>
-      </c>
-      <c r="D39" s="29">
-        <v>5027045</v>
-      </c>
-      <c r="E39">
-        <v>2242.1071900000002</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B40">
-        <v>10</v>
-      </c>
-      <c r="C40">
-        <v>6667.8139350000001</v>
-      </c>
-      <c r="D40" s="29">
-        <v>4021661</v>
-      </c>
-      <c r="E40">
-        <v>2005.4080269999999</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B41">
-        <v>11</v>
-      </c>
-      <c r="C41">
-        <v>9115.5840250000001</v>
-      </c>
-      <c r="D41" s="29">
-        <v>3323337</v>
-      </c>
-      <c r="E41">
-        <v>1823.00225</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B42">
-        <v>12</v>
-      </c>
-      <c r="C42">
-        <v>9115.5840250000001</v>
-      </c>
-      <c r="D42" s="29">
-        <v>1645895</v>
-      </c>
-      <c r="E42">
-        <v>1282.9242750000001</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B43">
-        <v>13</v>
-      </c>
-      <c r="C43">
-        <v>8251.2381100000002</v>
-      </c>
-      <c r="D43" s="29">
-        <v>1215558</v>
-      </c>
-      <c r="E43">
-        <v>1102.5235359999999</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B44">
-        <v>14</v>
-      </c>
-      <c r="C44">
-        <v>9477.8493080000007</v>
-      </c>
-      <c r="D44" s="29">
-        <v>8230023</v>
-      </c>
-      <c r="E44">
-        <v>2868.801645</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B45">
-        <v>15</v>
-      </c>
-      <c r="C45">
-        <v>8986.9107569999996</v>
-      </c>
-      <c r="D45" s="29">
-        <v>4091322</v>
-      </c>
-      <c r="E45">
-        <v>2022.7015449999999</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B46">
-        <v>16</v>
-      </c>
-      <c r="C46">
-        <v>9906.0938829999996</v>
-      </c>
-      <c r="D46" s="29">
-        <v>10676060</v>
-      </c>
-      <c r="E46">
-        <v>3267.4243820000002</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B47">
-        <v>17</v>
-      </c>
-      <c r="C47">
-        <v>9751.9976480000005</v>
-      </c>
-      <c r="D47" s="29">
-        <v>8693013</v>
-      </c>
-      <c r="E47">
-        <v>2948.3916479999998</v>
-      </c>
-    </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B48">
-        <v>18</v>
-      </c>
-      <c r="C48">
-        <v>12199.767739000001</v>
-      </c>
-      <c r="D48" s="29">
-        <v>3861120</v>
-      </c>
-      <c r="E48">
-        <v>1964.9733530000001</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B49">
-        <v>19</v>
-      </c>
-      <c r="C49">
-        <v>11486.910744000001</v>
-      </c>
-      <c r="D49" s="29">
-        <v>4091322</v>
-      </c>
-      <c r="E49">
-        <v>2022.701607</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B50">
-        <v>20</v>
-      </c>
-      <c r="C50">
-        <v>12406.093870000001</v>
-      </c>
-      <c r="D50" s="29">
-        <v>10676060</v>
-      </c>
-      <c r="E50">
-        <v>3267.4244279999998</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B51">
-        <v>21</v>
-      </c>
-      <c r="C51">
-        <v>12251.997635</v>
-      </c>
-      <c r="D51" s="29">
-        <v>8693014</v>
-      </c>
-      <c r="E51">
-        <v>2948.3917000000001</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B52">
-        <v>22</v>
-      </c>
-      <c r="C52">
-        <v>14699.767726</v>
-      </c>
-      <c r="D52" s="29">
-        <v>3861121</v>
-      </c>
-      <c r="E52">
-        <v>1964.9734370000001</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B53">
-        <v>23</v>
-      </c>
-      <c r="C53">
-        <v>13986.910717999999</v>
-      </c>
-      <c r="D53" s="29">
-        <v>4091322</v>
-      </c>
-      <c r="E53">
-        <v>2022.7017800000001</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B54">
-        <v>24</v>
-      </c>
-      <c r="C54">
-        <v>15127.481922999999</v>
-      </c>
-      <c r="D54" s="29">
-        <v>4814614</v>
-      </c>
-      <c r="E54">
-        <v>2194.2227910000001</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B55">
-        <v>25</v>
-      </c>
-      <c r="C55">
-        <v>14800.627458000001</v>
-      </c>
-      <c r="D55" s="29">
-        <v>4108688</v>
-      </c>
-      <c r="E55">
-        <v>2026.9898519999999</v>
-      </c>
+      <c r="C19" s="61">
+        <v>136.52944299999999</v>
+      </c>
+      <c r="D19" s="61">
+        <v>107583.6208</v>
+      </c>
+      <c r="E19" s="61">
+        <v>327.99942199999998</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B21" s="61"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="61"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B22" s="61"/>
+      <c r="C22" s="61"/>
+      <c r="D22" s="61"/>
+      <c r="E22" s="61"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B23" s="61"/>
+      <c r="C23" s="61"/>
+      <c r="D23" s="61"/>
+      <c r="E23" s="61"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B24" s="61"/>
+      <c r="C24" s="61"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="61"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B25" s="61"/>
+      <c r="C25" s="61"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="61"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B26" s="61"/>
+      <c r="C26" s="61"/>
+      <c r="D26" s="61"/>
+      <c r="E26" s="61"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B27" s="61"/>
+      <c r="C27" s="61"/>
+      <c r="D27" s="61"/>
+      <c r="E27" s="61"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A12:F12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>